<commit_message>
changed .xslx to include api key, changed validate to second page, added get_api_key method
</commit_message>
<xml_diff>
--- a/meraki/app/static/template.xlsx
+++ b/meraki/app/static/template.xlsx
@@ -1,25 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28410"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhouj/Desktop/Meraki-Bulk-Configuration-Tool-master 2/meraki/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/demelloi/PycharmProjects/meraki/app/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Port Configuration" sheetId="1" r:id="rId1"/>
-    <sheet name="Base Configuration" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
+    <sheet name="Port Configuration" sheetId="1" r:id="rId2"/>
+    <sheet name="Base Configuration" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -28,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="25">
   <si>
     <t>Hostname</t>
   </si>
@@ -101,12 +99,15 @@
   <si>
     <t>200,210,220,232,236,400</t>
   </si>
+  <si>
+    <t>API Key</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -120,6 +121,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF444444"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -142,10 +148,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -491,9 +498,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -2225,7 +2255,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1"/>
   <sheetViews>

</xml_diff>

<commit_message>
changes to template and step1 instructions
</commit_message>
<xml_diff>
--- a/meraki/app/static/template.xlsx
+++ b/meraki/app/static/template.xlsx
@@ -1,25 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28410"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhouj/Desktop/Meraki-Bulk-Configuration-Tool-master 2/meraki/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/demelloi/PycharmProjects/meraki/app/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Port Configuration" sheetId="1" r:id="rId1"/>
-    <sheet name="Base Configuration" sheetId="2" r:id="rId2"/>
+    <sheet name="API Key" sheetId="3" r:id="rId1"/>
+    <sheet name="Port Configuration" sheetId="1" r:id="rId2"/>
+    <sheet name="Base Configuration" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -28,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="25">
   <si>
     <t>Hostname</t>
   </si>
@@ -100,6 +98,9 @@
   </si>
   <si>
     <t>200,210,220,232,236,400</t>
+  </si>
+  <si>
+    <t>API Key</t>
   </si>
 </sst>
 </file>
@@ -491,9 +492,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -2225,7 +2246,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1"/>
   <sheetViews>

</xml_diff>

<commit_message>
changed static template and reformated code
</commit_message>
<xml_diff>
--- a/meraki/app/static/template.xlsx
+++ b/meraki/app/static/template.xlsx
@@ -1,23 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26311"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28502"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/demelloi/PycharmProjects/meraki/app/static/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chongw/PycharmProjects/meraki/Meraki-Bulk-Configuration-Tool/meraki/app/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="API Key" sheetId="3" r:id="rId1"/>
-    <sheet name="Port Configuration" sheetId="1" r:id="rId2"/>
-    <sheet name="Base Configuration" sheetId="2" r:id="rId3"/>
+    <sheet name="Base Configuration" sheetId="2" r:id="rId2"/>
+    <sheet name="Port Configuration" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -494,7 +497,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
@@ -511,6 +514,1441 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
+    <col min="257" max="260" width="10.83203125" customWidth="1"/>
+    <col min="262" max="263" width="10.83203125" customWidth="1"/>
+    <col min="265" max="298" width="10.83203125" customWidth="1"/>
+    <col min="300" max="301" width="10.83203125" customWidth="1"/>
+    <col min="304" max="304" width="10.83203125" customWidth="1"/>
+    <col min="306" max="308" width="10.83203125" customWidth="1"/>
+    <col min="310" max="340" width="10.83203125" customWidth="1"/>
+    <col min="342" max="343" width="10.83203125" customWidth="1"/>
+    <col min="345" max="356" width="10.83203125" customWidth="1"/>
+    <col min="358" max="359" width="10.83203125" customWidth="1"/>
+    <col min="362" max="364" width="10.83203125" customWidth="1"/>
+    <col min="368" max="369" width="10.83203125" customWidth="1"/>
+    <col min="371" max="371" width="10.83203125" customWidth="1"/>
+    <col min="375" max="385" width="10.83203125" customWidth="1"/>
+    <col min="388" max="390" width="10.83203125" customWidth="1"/>
+    <col min="392" max="400" width="10.83203125" customWidth="1"/>
+    <col min="402" max="402" width="10.83203125" customWidth="1"/>
+    <col min="404" max="405" width="10.83203125" customWidth="1"/>
+    <col min="407" max="407" width="10.83203125" customWidth="1"/>
+    <col min="409" max="431" width="10.83203125" customWidth="1"/>
+    <col min="433" max="439" width="10.83203125" customWidth="1"/>
+    <col min="441" max="454" width="10.83203125" customWidth="1"/>
+    <col min="457" max="462" width="10.83203125" customWidth="1"/>
+    <col min="465" max="470" width="10.83203125" customWidth="1"/>
+    <col min="473" max="487" width="10.83203125" customWidth="1"/>
+    <col min="489" max="495" width="10.83203125" customWidth="1"/>
+    <col min="497" max="503" width="10.83203125" customWidth="1"/>
+    <col min="505" max="512" width="10.83203125" customWidth="1"/>
+    <col min="515" max="517" width="10.83203125" customWidth="1"/>
+    <col min="520" max="521" width="10.83203125" customWidth="1"/>
+    <col min="523" max="523" width="10.83203125" customWidth="1"/>
+    <col min="525" max="525" width="10.83203125" customWidth="1"/>
+    <col min="527" max="527" width="10.83203125" customWidth="1"/>
+    <col min="529" max="529" width="10.83203125" customWidth="1"/>
+    <col min="537" max="544" width="10.83203125" customWidth="1"/>
+    <col min="546" max="546" width="10.83203125" customWidth="1"/>
+    <col min="550" max="550" width="10.83203125" customWidth="1"/>
+    <col min="554" max="554" width="10.83203125" customWidth="1"/>
+    <col min="557" max="557" width="10.83203125" customWidth="1"/>
+    <col min="559" max="561" width="10.83203125" customWidth="1"/>
+    <col min="563" max="564" width="10.83203125" customWidth="1"/>
+    <col min="567" max="576" width="10.83203125" customWidth="1"/>
+    <col min="586" max="586" width="10.83203125" customWidth="1"/>
+    <col min="588" max="588" width="10.83203125" customWidth="1"/>
+    <col min="593" max="594" width="10.83203125" customWidth="1"/>
+    <col min="597" max="599" width="10.83203125" customWidth="1"/>
+    <col min="601" max="609" width="10.83203125" customWidth="1"/>
+    <col min="613" max="614" width="10.83203125" customWidth="1"/>
+    <col min="616" max="617" width="10.83203125" customWidth="1"/>
+    <col min="619" max="621" width="10.83203125" customWidth="1"/>
+    <col min="628" max="628" width="10.83203125" customWidth="1"/>
+    <col min="630" max="630" width="10.83203125" customWidth="1"/>
+    <col min="632" max="640" width="10.83203125" customWidth="1"/>
+    <col min="644" max="645" width="10.83203125" customWidth="1"/>
+    <col min="648" max="648" width="10.83203125" customWidth="1"/>
+    <col min="650" max="652" width="10.83203125" customWidth="1"/>
+    <col min="654" max="656" width="10.83203125" customWidth="1"/>
+    <col min="665" max="673" width="10.83203125" customWidth="1"/>
+    <col min="684" max="685" width="10.83203125" customWidth="1"/>
+    <col min="687" max="687" width="10.83203125" customWidth="1"/>
+    <col min="689" max="689" width="10.83203125" customWidth="1"/>
+    <col min="692" max="694" width="10.83203125" customWidth="1"/>
+    <col min="696" max="705" width="10.83203125" customWidth="1"/>
+    <col min="708" max="711" width="10.83203125" customWidth="1"/>
+    <col min="715" max="716" width="10.83203125" customWidth="1"/>
+    <col min="718" max="718" width="10.83203125" customWidth="1"/>
+    <col min="720" max="720" width="10.83203125" customWidth="1"/>
+    <col min="724" max="724" width="10.83203125" customWidth="1"/>
+    <col min="726" max="726" width="10.83203125" customWidth="1"/>
+    <col min="728" max="737" width="10.83203125" customWidth="1"/>
+    <col min="739" max="741" width="10.83203125" customWidth="1"/>
+    <col min="743" max="743" width="10.83203125" customWidth="1"/>
+    <col min="746" max="746" width="10.83203125" customWidth="1"/>
+    <col min="751" max="751" width="10.83203125" customWidth="1"/>
+    <col min="753" max="756" width="10.83203125" customWidth="1"/>
+    <col min="758" max="759" width="10.83203125" customWidth="1"/>
+    <col min="761" max="768" width="10.83203125" customWidth="1"/>
+    <col min="771" max="773" width="10.83203125" customWidth="1"/>
+    <col min="776" max="777" width="10.83203125" customWidth="1"/>
+    <col min="779" max="779" width="10.83203125" customWidth="1"/>
+    <col min="781" max="781" width="10.83203125" customWidth="1"/>
+    <col min="783" max="783" width="10.83203125" customWidth="1"/>
+    <col min="785" max="785" width="10.83203125" customWidth="1"/>
+    <col min="793" max="800" width="10.83203125" customWidth="1"/>
+    <col min="802" max="802" width="10.83203125" customWidth="1"/>
+    <col min="806" max="806" width="10.83203125" customWidth="1"/>
+    <col min="810" max="810" width="10.83203125" customWidth="1"/>
+    <col min="813" max="813" width="10.83203125" customWidth="1"/>
+    <col min="815" max="817" width="10.83203125" customWidth="1"/>
+    <col min="819" max="820" width="10.83203125" customWidth="1"/>
+    <col min="823" max="832" width="10.83203125" customWidth="1"/>
+    <col min="842" max="842" width="10.83203125" customWidth="1"/>
+    <col min="844" max="844" width="10.83203125" customWidth="1"/>
+    <col min="849" max="850" width="10.83203125" customWidth="1"/>
+    <col min="853" max="855" width="10.83203125" customWidth="1"/>
+    <col min="857" max="865" width="10.83203125" customWidth="1"/>
+    <col min="869" max="870" width="10.83203125" customWidth="1"/>
+    <col min="872" max="873" width="10.83203125" customWidth="1"/>
+    <col min="875" max="877" width="10.83203125" customWidth="1"/>
+    <col min="884" max="884" width="10.83203125" customWidth="1"/>
+    <col min="886" max="886" width="10.83203125" customWidth="1"/>
+    <col min="888" max="896" width="10.83203125" customWidth="1"/>
+    <col min="900" max="901" width="10.83203125" customWidth="1"/>
+    <col min="904" max="904" width="10.83203125" customWidth="1"/>
+    <col min="906" max="908" width="10.83203125" customWidth="1"/>
+    <col min="910" max="912" width="10.83203125" customWidth="1"/>
+    <col min="921" max="929" width="10.83203125" customWidth="1"/>
+    <col min="940" max="941" width="10.83203125" customWidth="1"/>
+    <col min="943" max="943" width="10.83203125" customWidth="1"/>
+    <col min="945" max="945" width="10.83203125" customWidth="1"/>
+    <col min="948" max="950" width="10.83203125" customWidth="1"/>
+    <col min="952" max="961" width="10.83203125" customWidth="1"/>
+    <col min="964" max="967" width="10.83203125" customWidth="1"/>
+    <col min="971" max="972" width="10.83203125" customWidth="1"/>
+    <col min="974" max="974" width="10.83203125" customWidth="1"/>
+    <col min="976" max="976" width="10.83203125" customWidth="1"/>
+    <col min="980" max="980" width="10.83203125" customWidth="1"/>
+    <col min="982" max="982" width="10.83203125" customWidth="1"/>
+    <col min="984" max="993" width="10.83203125" customWidth="1"/>
+    <col min="995" max="997" width="10.83203125" customWidth="1"/>
+    <col min="999" max="999" width="10.83203125" customWidth="1"/>
+    <col min="1002" max="1002" width="10.83203125" customWidth="1"/>
+    <col min="1007" max="1007" width="10.83203125" customWidth="1"/>
+    <col min="1009" max="1012" width="10.83203125" customWidth="1"/>
+    <col min="1014" max="1015" width="10.83203125" customWidth="1"/>
+    <col min="1017" max="1034" width="10.83203125" customWidth="1"/>
+    <col min="1037" max="1038" width="10.83203125" customWidth="1"/>
+    <col min="1049" max="1058" width="10.83203125" customWidth="1"/>
+    <col min="1061" max="1062" width="10.83203125" customWidth="1"/>
+    <col min="1081" max="1090" width="10.83203125" customWidth="1"/>
+    <col min="1093" max="1094" width="10.83203125" customWidth="1"/>
+    <col min="1105" max="1106" width="10.83203125" customWidth="1"/>
+    <col min="1109" max="1110" width="10.83203125" customWidth="1"/>
+    <col min="1113" max="1120" width="10.83203125" customWidth="1"/>
+    <col min="1138" max="1139" width="10.83203125" customWidth="1"/>
+    <col min="1142" max="1143" width="10.83203125" customWidth="1"/>
+    <col min="1145" max="1152" width="10.83203125" customWidth="1"/>
+    <col min="1154" max="1155" width="10.83203125" customWidth="1"/>
+    <col min="1158" max="1159" width="10.83203125" customWidth="1"/>
+    <col min="1161" max="1162" width="10.83203125" customWidth="1"/>
+    <col min="1165" max="1166" width="10.83203125" customWidth="1"/>
+    <col min="1177" max="1184" width="10.83203125" customWidth="1"/>
+    <col min="1194" max="1195" width="10.83203125" customWidth="1"/>
+    <col min="1198" max="1199" width="10.83203125" customWidth="1"/>
+    <col min="1201" max="1202" width="10.83203125" customWidth="1"/>
+    <col min="1205" max="1206" width="10.83203125" customWidth="1"/>
+    <col min="1209" max="1218" width="10.83203125" customWidth="1"/>
+    <col min="1221" max="1222" width="10.83203125" customWidth="1"/>
+    <col min="1226" max="1227" width="10.83203125" customWidth="1"/>
+    <col min="1230" max="1231" width="10.83203125" customWidth="1"/>
+    <col min="1241" max="1248" width="10.83203125" customWidth="1"/>
+    <col min="1251" max="1253" width="10.83203125" customWidth="1"/>
+    <col min="1259" max="1261" width="10.83203125" customWidth="1"/>
+    <col min="1267" max="1269" width="10.83203125" customWidth="1"/>
+    <col min="1273" max="1280" width="10.83203125" customWidth="1"/>
+    <col min="1283" max="1284" width="10.83203125" customWidth="1"/>
+    <col min="1287" max="1289" width="10.83203125" customWidth="1"/>
+    <col min="1292" max="1293" width="10.83203125" customWidth="1"/>
+    <col min="1296" max="1296" width="10.83203125" customWidth="1"/>
+    <col min="1305" max="1312" width="10.83203125" customWidth="1"/>
+    <col min="1315" max="1316" width="10.83203125" customWidth="1"/>
+    <col min="1319" max="1322" width="10.83203125" customWidth="1"/>
+    <col min="1325" max="1326" width="10.83203125" customWidth="1"/>
+    <col min="1329" max="1330" width="10.83203125" customWidth="1"/>
+    <col min="1333" max="1334" width="10.83203125" customWidth="1"/>
+    <col min="1337" max="1344" width="10.83203125" customWidth="1"/>
+    <col min="1346" max="1347" width="10.83203125" customWidth="1"/>
+    <col min="1350" max="1351" width="10.83203125" customWidth="1"/>
+    <col min="1353" max="1354" width="10.83203125" customWidth="1"/>
+    <col min="1357" max="1358" width="10.83203125" customWidth="1"/>
+    <col min="1361" max="1376" width="10.83203125" customWidth="1"/>
+    <col min="1385" max="1386" width="10.83203125" customWidth="1"/>
+    <col min="1389" max="1390" width="10.83203125" customWidth="1"/>
+    <col min="1393" max="1408" width="10.83203125" customWidth="1"/>
+    <col min="1418" max="1419" width="10.83203125" customWidth="1"/>
+    <col min="1422" max="1423" width="10.83203125" customWidth="1"/>
+    <col min="1425" max="1440" width="10.83203125" customWidth="1"/>
+    <col min="1449" max="1449" width="10.83203125" customWidth="1"/>
+    <col min="1452" max="1453" width="10.83203125" customWidth="1"/>
+    <col min="1456" max="1473" width="10.83203125" customWidth="1"/>
+    <col min="1476" max="1477" width="10.83203125" customWidth="1"/>
+    <col min="1480" max="1481" width="10.83203125" customWidth="1"/>
+    <col min="1484" max="1485" width="10.83203125" customWidth="1"/>
+    <col min="1488" max="1488" width="10.83203125" customWidth="1"/>
+    <col min="1490" max="1491" width="10.83203125" customWidth="1"/>
+    <col min="1494" max="1495" width="10.83203125" customWidth="1"/>
+    <col min="1497" max="1505" width="10.83203125" customWidth="1"/>
+    <col min="1508" max="1508" width="10.83203125" customWidth="1"/>
+    <col min="1510" max="1511" width="10.83203125" customWidth="1"/>
+    <col min="1513" max="1513" width="10.83203125" customWidth="1"/>
+    <col min="1516" max="1516" width="10.83203125" customWidth="1"/>
+    <col min="1518" max="1519" width="10.83203125" customWidth="1"/>
+    <col min="1521" max="1521" width="10.83203125" customWidth="1"/>
+    <col min="1524" max="1524" width="10.83203125" customWidth="1"/>
+    <col min="1526" max="1527" width="10.83203125" customWidth="1"/>
+    <col min="1529" max="1544" width="10.83203125" customWidth="1"/>
+    <col min="1547" max="1548" width="10.83203125" customWidth="1"/>
+    <col min="1551" max="1553" width="10.83203125" customWidth="1"/>
+    <col min="1556" max="1557" width="10.83203125" customWidth="1"/>
+    <col min="1560" max="1568" width="10.83203125" customWidth="1"/>
+    <col min="1571" max="1572" width="10.83203125" customWidth="1"/>
+    <col min="1575" max="1576" width="10.83203125" customWidth="1"/>
+    <col min="1578" max="1579" width="10.83203125" customWidth="1"/>
+    <col min="1582" max="1583" width="10.83203125" customWidth="1"/>
+    <col min="1585" max="1585" width="10.83203125" customWidth="1"/>
+    <col min="1588" max="1589" width="10.83203125" customWidth="1"/>
+    <col min="1592" max="1608" width="10.83203125" customWidth="1"/>
+    <col min="1611" max="1612" width="10.83203125" customWidth="1"/>
+    <col min="1615" max="1632" width="10.83203125" customWidth="1"/>
+    <col min="1635" max="1636" width="10.83203125" customWidth="1"/>
+    <col min="1639" max="1640" width="10.83203125" customWidth="1"/>
+    <col min="1643" max="1644" width="10.83203125" customWidth="1"/>
+    <col min="1647" max="1664" width="10.83203125" customWidth="1"/>
+    <col min="1666" max="1667" width="10.83203125" customWidth="1"/>
+    <col min="1670" max="1671" width="10.83203125" customWidth="1"/>
+    <col min="1675" max="1676" width="10.83203125" customWidth="1"/>
+    <col min="1679" max="1696" width="10.83203125" customWidth="1"/>
+    <col min="1698" max="1699" width="10.83203125" customWidth="1"/>
+    <col min="1702" max="1703" width="10.83203125" customWidth="1"/>
+    <col min="1707" max="1708" width="10.83203125" customWidth="1"/>
+    <col min="1711" max="1713" width="10.83203125" customWidth="1"/>
+    <col min="1716" max="1717" width="10.83203125" customWidth="1"/>
+    <col min="1720" max="1728" width="10.83203125" customWidth="1"/>
+    <col min="1731" max="1732" width="10.83203125" customWidth="1"/>
+    <col min="1735" max="1736" width="10.83203125" customWidth="1"/>
+    <col min="1739" max="1740" width="10.83203125" customWidth="1"/>
+    <col min="1743" max="1744" width="10.83203125" customWidth="1"/>
+    <col min="1746" max="1747" width="10.83203125" customWidth="1"/>
+    <col min="1750" max="1751" width="10.83203125" customWidth="1"/>
+    <col min="1753" max="1760" width="10.83203125" customWidth="1"/>
+    <col min="1763" max="1764" width="10.83203125" customWidth="1"/>
+    <col min="1767" max="1768" width="10.83203125" customWidth="1"/>
+    <col min="1771" max="1772" width="10.83203125" customWidth="1"/>
+    <col min="1775" max="1776" width="10.83203125" customWidth="1"/>
+    <col min="1779" max="1780" width="10.83203125" customWidth="1"/>
+    <col min="1783" max="1793" width="10.83203125" customWidth="1"/>
+    <col min="1802" max="1804" width="10.83203125" customWidth="1"/>
+    <col min="1807" max="1807" width="10.83203125" customWidth="1"/>
+    <col min="1824" max="1905" width="10.83203125" customWidth="1"/>
+    <col min="1907" max="1908" width="10.83203125" customWidth="1"/>
+    <col min="1910" max="1910" width="10.83203125" customWidth="1"/>
+    <col min="1912" max="1912" width="10.83203125" customWidth="1"/>
+    <col min="1914" max="1914" width="10.83203125" customWidth="1"/>
+    <col min="1917" max="1918" width="10.83203125" customWidth="1"/>
+    <col min="1922" max="1924" width="10.83203125" customWidth="1"/>
+    <col min="1926" max="1928" width="10.83203125" customWidth="1"/>
+    <col min="1930" max="1932" width="10.83203125" customWidth="1"/>
+    <col min="1934" max="1934" width="10.83203125" customWidth="1"/>
+    <col min="1936" max="1936" width="10.83203125" customWidth="1"/>
+    <col min="1952" max="1968" width="10.83203125" customWidth="1"/>
+    <col min="1971" max="2038" width="10.83203125" customWidth="1"/>
+    <col min="2040" max="2040" width="10.83203125" customWidth="1"/>
+    <col min="2042" max="2042" width="10.83203125" customWidth="1"/>
+    <col min="2044" max="2046" width="10.83203125" customWidth="1"/>
+    <col min="2050" max="2052" width="10.83203125" customWidth="1"/>
+    <col min="2054" max="2056" width="10.83203125" customWidth="1"/>
+    <col min="2058" max="2060" width="10.83203125" customWidth="1"/>
+    <col min="2062" max="2062" width="10.83203125" customWidth="1"/>
+    <col min="2064" max="2064" width="10.83203125" customWidth="1"/>
+    <col min="2080" max="2096" width="10.83203125" customWidth="1"/>
+    <col min="2099" max="2099" width="10.83203125" customWidth="1"/>
+    <col min="2101" max="2103" width="10.83203125" customWidth="1"/>
+    <col min="2106" max="2107" width="10.83203125" customWidth="1"/>
+    <col min="2111" max="2111" width="10.83203125" customWidth="1"/>
+    <col min="2113" max="2113" width="10.83203125" customWidth="1"/>
+    <col min="2115" max="2115" width="10.83203125" customWidth="1"/>
+    <col min="2122" max="2124" width="10.83203125" customWidth="1"/>
+    <col min="2127" max="2127" width="10.83203125" customWidth="1"/>
+    <col min="2144" max="2161" width="10.83203125" customWidth="1"/>
+    <col min="2163" max="2164" width="10.83203125" customWidth="1"/>
+    <col min="2168" max="2168" width="10.83203125" customWidth="1"/>
+    <col min="2170" max="2170" width="10.83203125" customWidth="1"/>
+    <col min="2173" max="2174" width="10.83203125" customWidth="1"/>
+    <col min="2178" max="2180" width="10.83203125" customWidth="1"/>
+    <col min="2182" max="2184" width="10.83203125" customWidth="1"/>
+    <col min="2186" max="2188" width="10.83203125" customWidth="1"/>
+    <col min="2190" max="2190" width="10.83203125" customWidth="1"/>
+    <col min="2192" max="2192" width="10.83203125" customWidth="1"/>
+    <col min="2208" max="2224" width="10.83203125" customWidth="1"/>
+    <col min="2227" max="2293" width="10.83203125" customWidth="1"/>
+    <col min="2296" max="2296" width="10.83203125" customWidth="1"/>
+    <col min="2298" max="2298" width="10.83203125" customWidth="1"/>
+    <col min="2300" max="2302" width="10.83203125" customWidth="1"/>
+    <col min="2306" max="2308" width="10.83203125" customWidth="1"/>
+    <col min="2310" max="2312" width="10.83203125" customWidth="1"/>
+    <col min="2314" max="2316" width="10.83203125" customWidth="1"/>
+    <col min="2318" max="2318" width="10.83203125" customWidth="1"/>
+    <col min="2320" max="2320" width="10.83203125" customWidth="1"/>
+    <col min="2336" max="2359" width="10.83203125" customWidth="1"/>
+    <col min="2361" max="2492" width="10.83203125" customWidth="1"/>
+    <col min="2494" max="2535" width="10.83203125" customWidth="1"/>
+    <col min="2561" max="2564" width="10.83203125" customWidth="1"/>
+    <col min="2566" max="2566" width="10.83203125" customWidth="1"/>
+    <col min="2568" max="2569" width="10.83203125" customWidth="1"/>
+    <col min="2574" max="2575" width="10.83203125" customWidth="1"/>
+    <col min="2592" max="2615" width="10.83203125" customWidth="1"/>
+    <col min="2617" max="2672" width="10.83203125" customWidth="1"/>
+    <col min="2674" max="2674" width="10.83203125" customWidth="1"/>
+    <col min="2676" max="2814" width="10.83203125" customWidth="1"/>
+    <col min="2819" max="2822" width="10.83203125" customWidth="1"/>
+    <col min="2824" max="2827" width="10.83203125" customWidth="1"/>
+    <col min="2830" max="2832" width="10.83203125" customWidth="1"/>
+    <col min="2834" max="2871" width="10.83203125" customWidth="1"/>
+    <col min="2873" max="2933" width="10.83203125" customWidth="1"/>
+    <col min="2938" max="2942" width="10.83203125" customWidth="1"/>
+    <col min="2946" max="2948" width="10.83203125" customWidth="1"/>
+    <col min="2950" max="2952" width="10.83203125" customWidth="1"/>
+    <col min="2954" max="2956" width="10.83203125" customWidth="1"/>
+    <col min="2958" max="2958" width="10.83203125" customWidth="1"/>
+    <col min="2960" max="2960" width="10.83203125" customWidth="1"/>
+    <col min="2976" max="2992" width="10.83203125" customWidth="1"/>
+    <col min="2999" max="2999" width="10.83203125" customWidth="1"/>
+    <col min="3003" max="3004" width="10.83203125" customWidth="1"/>
+    <col min="3006" max="3006" width="10.83203125" customWidth="1"/>
+    <col min="3008" max="3008" width="10.83203125" customWidth="1"/>
+    <col min="3011" max="3011" width="10.83203125" customWidth="1"/>
+    <col min="3013" max="3017" width="10.83203125" customWidth="1"/>
+    <col min="3019" max="3020" width="10.83203125" customWidth="1"/>
+    <col min="3023" max="3023" width="10.83203125" customWidth="1"/>
+    <col min="3040" max="3134" width="10.83203125" customWidth="1"/>
+    <col min="3139" max="3141" width="10.83203125" customWidth="1"/>
+    <col min="3145" max="3145" width="10.83203125" customWidth="1"/>
+    <col min="3147" max="3147" width="10.83203125" customWidth="1"/>
+    <col min="3151" max="3151" width="10.83203125" customWidth="1"/>
+    <col min="3168" max="3188" width="10.83203125" customWidth="1"/>
+    <col min="3190" max="3193" width="10.83203125" customWidth="1"/>
+    <col min="3195" max="3198" width="10.83203125" customWidth="1"/>
+    <col min="3202" max="3204" width="10.83203125" customWidth="1"/>
+    <col min="3206" max="3208" width="10.83203125" customWidth="1"/>
+    <col min="3210" max="3212" width="10.83203125" customWidth="1"/>
+    <col min="3214" max="3214" width="10.83203125" customWidth="1"/>
+    <col min="3216" max="3216" width="10.83203125" customWidth="1"/>
+    <col min="3232" max="3249" width="10.83203125" customWidth="1"/>
+    <col min="3251" max="3255" width="10.83203125" customWidth="1"/>
+    <col min="3257" max="3257" width="10.83203125" customWidth="1"/>
+    <col min="3259" max="3261" width="10.83203125" customWidth="1"/>
+    <col min="3265" max="3265" width="10.83203125" customWidth="1"/>
+    <col min="3267" max="3267" width="10.83203125" customWidth="1"/>
+    <col min="3269" max="3273" width="10.83203125" customWidth="1"/>
+    <col min="3275" max="3276" width="10.83203125" customWidth="1"/>
+    <col min="3279" max="3279" width="10.83203125" customWidth="1"/>
+    <col min="3296" max="3319" width="10.83203125" customWidth="1"/>
+    <col min="3321" max="3383" width="10.83203125" customWidth="1"/>
+    <col min="3385" max="3440" width="10.83203125" customWidth="1"/>
+    <col min="3443" max="3509" width="10.83203125" customWidth="1"/>
+    <col min="3511" max="3511" width="10.83203125" customWidth="1"/>
+    <col min="3513" max="3514" width="10.83203125" customWidth="1"/>
+    <col min="3516" max="3518" width="10.83203125" customWidth="1"/>
+    <col min="3522" max="3524" width="10.83203125" customWidth="1"/>
+    <col min="3526" max="3528" width="10.83203125" customWidth="1"/>
+    <col min="3530" max="3532" width="10.83203125" customWidth="1"/>
+    <col min="3534" max="3534" width="10.83203125" customWidth="1"/>
+    <col min="3536" max="3536" width="10.83203125" customWidth="1"/>
+    <col min="3552" max="3572" width="10.83203125" customWidth="1"/>
+    <col min="3576" max="3578" width="10.83203125" customWidth="1"/>
+    <col min="3580" max="3582" width="10.83203125" customWidth="1"/>
+    <col min="3586" max="3588" width="10.83203125" customWidth="1"/>
+    <col min="3590" max="3592" width="10.83203125" customWidth="1"/>
+    <col min="3594" max="3596" width="10.83203125" customWidth="1"/>
+    <col min="3598" max="3598" width="10.83203125" customWidth="1"/>
+    <col min="3600" max="3600" width="10.83203125" customWidth="1"/>
+    <col min="3616" max="3639" width="10.83203125" customWidth="1"/>
+    <col min="3642" max="3643" width="10.83203125" customWidth="1"/>
+    <col min="3647" max="3650" width="10.83203125" customWidth="1"/>
+    <col min="3652" max="3652" width="10.83203125" customWidth="1"/>
+    <col min="3656" max="3658" width="10.83203125" customWidth="1"/>
+    <col min="3662" max="3663" width="10.83203125" customWidth="1"/>
+    <col min="3680" max="3696" width="10.83203125" customWidth="1"/>
+    <col min="3699" max="3728" width="10.83203125" customWidth="1"/>
+    <col min="3730" max="3763" width="10.83203125" customWidth="1"/>
+    <col min="3765" max="3766" width="10.83203125" customWidth="1"/>
+    <col min="3768" max="3769" width="10.83203125" customWidth="1"/>
+    <col min="3772" max="3774" width="10.83203125" customWidth="1"/>
+    <col min="3778" max="3780" width="10.83203125" customWidth="1"/>
+    <col min="3782" max="3784" width="10.83203125" customWidth="1"/>
+    <col min="3786" max="3788" width="10.83203125" customWidth="1"/>
+    <col min="3790" max="3790" width="10.83203125" customWidth="1"/>
+    <col min="3792" max="3792" width="10.83203125" customWidth="1"/>
+    <col min="3808" max="3888" width="10.83203125" customWidth="1"/>
+    <col min="3936" max="4019" width="10.83203125" customWidth="1"/>
+    <col min="4021" max="4021" width="10.83203125" customWidth="1"/>
+    <col min="4024" max="4025" width="10.83203125" customWidth="1"/>
+    <col min="4028" max="4030" width="10.83203125" customWidth="1"/>
+    <col min="4034" max="4036" width="10.83203125" customWidth="1"/>
+    <col min="4038" max="4040" width="10.83203125" customWidth="1"/>
+    <col min="4042" max="4044" width="10.83203125" customWidth="1"/>
+    <col min="4046" max="4046" width="10.83203125" customWidth="1"/>
+    <col min="4048" max="4049" width="10.83203125" customWidth="1"/>
+    <col min="4051" max="4080" width="10.83203125" customWidth="1"/>
+    <col min="4083" max="4148" width="10.83203125" customWidth="1"/>
+    <col min="4150" max="4150" width="10.83203125" customWidth="1"/>
+    <col min="4152" max="4152" width="10.83203125" customWidth="1"/>
+    <col min="4154" max="4154" width="10.83203125" customWidth="1"/>
+    <col min="4157" max="4158" width="10.83203125" customWidth="1"/>
+    <col min="4162" max="4164" width="10.83203125" customWidth="1"/>
+    <col min="4166" max="4168" width="10.83203125" customWidth="1"/>
+    <col min="4170" max="4172" width="10.83203125" customWidth="1"/>
+    <col min="4174" max="4174" width="10.83203125" customWidth="1"/>
+    <col min="4176" max="4176" width="10.83203125" customWidth="1"/>
+    <col min="4192" max="4208" width="10.83203125" customWidth="1"/>
+    <col min="4210" max="4210" width="10.83203125" customWidth="1"/>
+    <col min="4216" max="4218" width="10.83203125" customWidth="1"/>
+    <col min="4220" max="4222" width="10.83203125" customWidth="1"/>
+    <col min="4226" max="4228" width="10.83203125" customWidth="1"/>
+    <col min="4230" max="4232" width="10.83203125" customWidth="1"/>
+    <col min="4234" max="4236" width="10.83203125" customWidth="1"/>
+    <col min="4238" max="4238" width="10.83203125" customWidth="1"/>
+    <col min="4240" max="4240" width="10.83203125" customWidth="1"/>
+    <col min="4256" max="4305" width="10.83203125" customWidth="1"/>
+    <col min="4307" max="4343" width="10.83203125" customWidth="1"/>
+    <col min="4345" max="4345" width="10.83203125" customWidth="1"/>
+    <col min="4347" max="4348" width="10.83203125" customWidth="1"/>
+    <col min="4357" max="4360" width="10.83203125" customWidth="1"/>
+    <col min="4362" max="4381" width="10.83203125" customWidth="1"/>
+    <col min="4384" max="4404" width="10.83203125" customWidth="1"/>
+    <col min="4408" max="4408" width="10.83203125" customWidth="1"/>
+    <col min="4410" max="4410" width="10.83203125" customWidth="1"/>
+    <col min="4413" max="4414" width="10.83203125" customWidth="1"/>
+    <col min="4418" max="4420" width="10.83203125" customWidth="1"/>
+    <col min="4422" max="4424" width="10.83203125" customWidth="1"/>
+    <col min="4426" max="4428" width="10.83203125" customWidth="1"/>
+    <col min="4430" max="4430" width="10.83203125" customWidth="1"/>
+    <col min="4432" max="4432" width="10.83203125" customWidth="1"/>
+    <col min="4448" max="4468" width="10.83203125" customWidth="1"/>
+    <col min="4473" max="4476" width="10.83203125" customWidth="1"/>
+    <col min="4478" max="4479" width="10.83203125" customWidth="1"/>
+    <col min="4481" max="4481" width="10.83203125" customWidth="1"/>
+    <col min="4483" max="4485" width="10.83203125" customWidth="1"/>
+    <col min="4489" max="4489" width="10.83203125" customWidth="1"/>
+    <col min="4491" max="4491" width="10.83203125" customWidth="1"/>
+    <col min="4495" max="4495" width="10.83203125" customWidth="1"/>
+    <col min="4512" max="4532" width="10.83203125" customWidth="1"/>
+    <col min="4534" max="4534" width="10.83203125" customWidth="1"/>
+    <col min="4537" max="4537" width="10.83203125" customWidth="1"/>
+    <col min="4541" max="4542" width="10.83203125" customWidth="1"/>
+    <col min="4544" max="4544" width="10.83203125" customWidth="1"/>
+    <col min="4548" max="4550" width="10.83203125" customWidth="1"/>
+    <col min="4552" max="4553" width="10.83203125" customWidth="1"/>
+    <col min="4555" max="4573" width="10.83203125" customWidth="1"/>
+    <col min="4576" max="4599" width="10.83203125" customWidth="1"/>
+    <col min="4601" max="4601" width="10.83203125" customWidth="1"/>
+    <col min="4603" max="4604" width="10.83203125" customWidth="1"/>
+    <col min="4613" max="4616" width="10.83203125" customWidth="1"/>
+    <col min="4618" max="4624" width="10.83203125" customWidth="1"/>
+    <col min="4627" max="4784" width="10.83203125" customWidth="1"/>
+    <col min="4787" max="4912" width="10.83203125" customWidth="1"/>
+    <col min="4914" max="5046" width="10.83203125" customWidth="1"/>
+    <col min="5049" max="5049" width="10.83203125" customWidth="1"/>
+    <col min="5053" max="5054" width="10.83203125" customWidth="1"/>
+    <col min="5056" max="5056" width="10.83203125" customWidth="1"/>
+    <col min="5060" max="5062" width="10.83203125" customWidth="1"/>
+    <col min="5064" max="5065" width="10.83203125" customWidth="1"/>
+    <col min="5067" max="5085" width="10.83203125" customWidth="1"/>
+    <col min="5088" max="5168" width="10.83203125" customWidth="1"/>
+    <col min="5170" max="5232" width="10.83203125" customWidth="1"/>
+    <col min="5234" max="5302" width="10.83203125" customWidth="1"/>
+    <col min="5305" max="5305" width="10.83203125" customWidth="1"/>
+    <col min="5309" max="5310" width="10.83203125" customWidth="1"/>
+    <col min="5312" max="5312" width="10.83203125" customWidth="1"/>
+    <col min="5316" max="5318" width="10.83203125" customWidth="1"/>
+    <col min="5320" max="5321" width="10.83203125" customWidth="1"/>
+    <col min="5323" max="5341" width="10.83203125" customWidth="1"/>
+    <col min="5344" max="5367" width="10.83203125" customWidth="1"/>
+    <col min="5369" max="5424" width="10.83203125" customWidth="1"/>
+    <col min="5429" max="5429" width="10.83203125" customWidth="1"/>
+    <col min="5431" max="5440" width="10.83203125" customWidth="1"/>
+    <col min="5442" max="5442" width="10.83203125" customWidth="1"/>
+    <col min="5445" max="5446" width="10.83203125" customWidth="1"/>
+    <col min="5448" max="5456" width="10.83203125" customWidth="1"/>
+    <col min="5458" max="5458" width="10.83203125" customWidth="1"/>
+    <col min="5460" max="5461" width="10.83203125" customWidth="1"/>
+    <col min="5464" max="5473" width="10.83203125" customWidth="1"/>
+    <col min="5475" max="5476" width="10.83203125" customWidth="1"/>
+    <col min="5480" max="5488" width="10.83203125" customWidth="1"/>
+    <col min="5490" max="5490" width="10.83203125" customWidth="1"/>
+    <col min="5492" max="5553" width="10.83203125" customWidth="1"/>
+    <col min="5555" max="5558" width="10.83203125" customWidth="1"/>
+    <col min="5560" max="5568" width="10.83203125" customWidth="1"/>
+    <col min="5570" max="5570" width="10.83203125" customWidth="1"/>
+    <col min="5572" max="5572" width="10.83203125" customWidth="1"/>
+    <col min="5576" max="5586" width="10.83203125" customWidth="1"/>
+    <col min="5589" max="5589" width="10.83203125" customWidth="1"/>
+    <col min="5592" max="5600" width="10.83203125" customWidth="1"/>
+    <col min="5603" max="5603" width="10.83203125" customWidth="1"/>
+    <col min="5605" max="5605" width="10.83203125" customWidth="1"/>
+    <col min="5608" max="5623" width="10.83203125" customWidth="1"/>
+    <col min="5625" max="5681" width="10.83203125" customWidth="1"/>
+    <col min="5684" max="5685" width="10.83203125" customWidth="1"/>
+    <col min="5688" max="5696" width="10.83203125" customWidth="1"/>
+    <col min="5698" max="5699" width="10.83203125" customWidth="1"/>
+    <col min="5701" max="5701" width="10.83203125" customWidth="1"/>
+    <col min="5704" max="5712" width="10.83203125" customWidth="1"/>
+    <col min="5716" max="5717" width="10.83203125" customWidth="1"/>
+    <col min="5720" max="5728" width="10.83203125" customWidth="1"/>
+    <col min="5730" max="5730" width="10.83203125" customWidth="1"/>
+    <col min="5732" max="5732" width="10.83203125" customWidth="1"/>
+    <col min="5736" max="5744" width="10.83203125" customWidth="1"/>
+    <col min="5746" max="5746" width="10.83203125" customWidth="1"/>
+    <col min="5748" max="5808" width="10.83203125" customWidth="1"/>
+    <col min="5813" max="5813" width="10.83203125" customWidth="1"/>
+    <col min="5816" max="5825" width="10.83203125" customWidth="1"/>
+    <col min="5829" max="5829" width="10.83203125" customWidth="1"/>
+    <col min="5832" max="5840" width="10.83203125" customWidth="1"/>
+    <col min="5842" max="5842" width="10.83203125" customWidth="1"/>
+    <col min="5845" max="5845" width="10.83203125" customWidth="1"/>
+    <col min="5847" max="5858" width="10.83203125" customWidth="1"/>
+    <col min="5860" max="5860" width="10.83203125" customWidth="1"/>
+    <col min="5862" max="5862" width="10.83203125" customWidth="1"/>
+    <col min="5864" max="5872" width="10.83203125" customWidth="1"/>
+    <col min="5877" max="5877" width="10.83203125" customWidth="1"/>
+    <col min="5880" max="5888" width="10.83203125" customWidth="1"/>
+    <col min="5893" max="5893" width="10.83203125" customWidth="1"/>
+    <col min="5896" max="5906" width="10.83203125" customWidth="1"/>
+    <col min="5909" max="5909" width="10.83203125" customWidth="1"/>
+    <col min="5912" max="5920" width="10.83203125" customWidth="1"/>
+    <col min="5922" max="5922" width="10.83203125" customWidth="1"/>
+    <col min="5925" max="5925" width="10.83203125" customWidth="1"/>
+    <col min="5927" max="5936" width="10.83203125" customWidth="1"/>
+    <col min="5938" max="5938" width="10.83203125" customWidth="1"/>
+    <col min="5941" max="5941" width="10.83203125" customWidth="1"/>
+    <col min="5944" max="5952" width="10.83203125" customWidth="1"/>
+    <col min="5954" max="5957" width="10.83203125" customWidth="1"/>
+    <col min="5960" max="5968" width="10.83203125" customWidth="1"/>
+    <col min="5971" max="5972" width="10.83203125" customWidth="1"/>
+    <col min="5976" max="5986" width="10.83203125" customWidth="1"/>
+    <col min="5988" max="5988" width="10.83203125" customWidth="1"/>
+    <col min="5992" max="6000" width="10.83203125" customWidth="1"/>
+    <col min="6002" max="6002" width="10.83203125" customWidth="1"/>
+    <col min="6004" max="6005" width="10.83203125" customWidth="1"/>
+    <col min="6008" max="6017" width="10.83203125" customWidth="1"/>
+    <col min="6019" max="6020" width="10.83203125" customWidth="1"/>
+    <col min="6024" max="6032" width="10.83203125" customWidth="1"/>
+    <col min="6037" max="6037" width="10.83203125" customWidth="1"/>
+    <col min="6039" max="6050" width="10.83203125" customWidth="1"/>
+    <col min="6052" max="6052" width="10.83203125" customWidth="1"/>
+    <col min="6056" max="6064" width="10.83203125" customWidth="1"/>
+    <col min="6066" max="6066" width="10.83203125" customWidth="1"/>
+    <col min="6068" max="6069" width="10.83203125" customWidth="1"/>
+    <col min="6072" max="6080" width="10.83203125" customWidth="1"/>
+    <col min="6082" max="6082" width="10.83203125" customWidth="1"/>
+    <col min="6085" max="6085" width="10.83203125" customWidth="1"/>
+    <col min="6088" max="6100" width="10.83203125" customWidth="1"/>
+    <col min="6104" max="6114" width="10.83203125" customWidth="1"/>
+    <col min="6117" max="6117" width="10.83203125" customWidth="1"/>
+    <col min="6120" max="6123" width="10.83203125" customWidth="1"/>
+    <col min="6126" max="6126" width="10.83203125" customWidth="1"/>
+    <col min="6128" max="6128" width="10.83203125" customWidth="1"/>
+    <col min="6130" max="6133" width="10.83203125" customWidth="1"/>
+    <col min="6136" max="6146" width="10.83203125" customWidth="1"/>
+    <col min="6148" max="6148" width="10.83203125" customWidth="1"/>
+    <col min="6152" max="6160" width="10.83203125" customWidth="1"/>
+    <col min="6162" max="6162" width="10.83203125" customWidth="1"/>
+    <col min="6164" max="6165" width="10.83203125" customWidth="1"/>
+    <col min="6168" max="6177" width="10.83203125" customWidth="1"/>
+    <col min="6181" max="6181" width="10.83203125" customWidth="1"/>
+    <col min="6183" max="6195" width="10.83203125" customWidth="1"/>
+    <col min="6200" max="6210" width="10.83203125" customWidth="1"/>
+    <col min="6213" max="6213" width="10.83203125" customWidth="1"/>
+    <col min="6216" max="6224" width="10.83203125" customWidth="1"/>
+    <col min="6227" max="6228" width="10.83203125" customWidth="1"/>
+    <col min="6232" max="6262" width="10.83203125" customWidth="1"/>
+    <col min="6264" max="6264" width="10.83203125" customWidth="1"/>
+    <col min="6266" max="6329" width="10.83203125" customWidth="1"/>
+    <col min="6331" max="6331" width="10.83203125" customWidth="1"/>
+    <col min="6337" max="6342" width="10.83203125" customWidth="1"/>
+    <col min="6344" max="6347" width="10.83203125" customWidth="1"/>
+    <col min="6350" max="6352" width="10.83203125" customWidth="1"/>
+    <col min="6354" max="6379" width="10.83203125" customWidth="1"/>
+    <col min="6382" max="6382" width="10.83203125" customWidth="1"/>
+    <col min="6384" max="6404" width="10.83203125" customWidth="1"/>
+    <col min="6409" max="6410" width="10.83203125" customWidth="1"/>
+    <col min="6412" max="6414" width="10.83203125" customWidth="1"/>
+    <col min="6418" max="6418" width="10.83203125" customWidth="1"/>
+    <col min="6420" max="6420" width="10.83203125" customWidth="1"/>
+    <col min="6432" max="6480" width="10.83203125" customWidth="1"/>
+    <col min="6482" max="6521" width="10.83203125" customWidth="1"/>
+    <col min="6523" max="6523" width="10.83203125" customWidth="1"/>
+    <col min="6529" max="6534" width="10.83203125" customWidth="1"/>
+    <col min="6536" max="6539" width="10.83203125" customWidth="1"/>
+    <col min="6542" max="6544" width="10.83203125" customWidth="1"/>
+    <col min="6546" max="6580" width="10.83203125" customWidth="1"/>
+    <col min="6583" max="6644" width="10.83203125" customWidth="1"/>
+    <col min="6648" max="6650" width="10.83203125" customWidth="1"/>
+    <col min="6652" max="6654" width="10.83203125" customWidth="1"/>
+    <col min="6658" max="6660" width="10.83203125" customWidth="1"/>
+    <col min="6662" max="6664" width="10.83203125" customWidth="1"/>
+    <col min="6666" max="6668" width="10.83203125" customWidth="1"/>
+    <col min="6670" max="6670" width="10.83203125" customWidth="1"/>
+    <col min="6672" max="6672" width="10.83203125" customWidth="1"/>
+    <col min="6688" max="6768" width="10.83203125" customWidth="1"/>
+    <col min="6786" max="6788" width="10.83203125" customWidth="1"/>
+    <col min="6790" max="6792" width="10.83203125" customWidth="1"/>
+    <col min="6794" max="6796" width="10.83203125" customWidth="1"/>
+    <col min="6798" max="6798" width="10.83203125" customWidth="1"/>
+    <col min="6800" max="6800" width="10.83203125" customWidth="1"/>
+    <col min="6816" max="6835" width="10.83203125" customWidth="1"/>
+    <col min="6837" max="6837" width="10.83203125" customWidth="1"/>
+    <col min="6839" max="6899" width="10.83203125" customWidth="1"/>
+    <col min="6901" max="6901" width="10.83203125" customWidth="1"/>
+    <col min="6903" max="7029" width="10.83203125" customWidth="1"/>
+    <col min="7031" max="7060" width="10.83203125" customWidth="1"/>
+    <col min="7063" max="7096" width="10.83203125" customWidth="1"/>
+    <col min="7098" max="7099" width="10.83203125" customWidth="1"/>
+    <col min="7101" max="7102" width="10.83203125" customWidth="1"/>
+    <col min="7106" max="7108" width="10.83203125" customWidth="1"/>
+    <col min="7110" max="7112" width="10.83203125" customWidth="1"/>
+    <col min="7114" max="7116" width="10.83203125" customWidth="1"/>
+    <col min="7118" max="7118" width="10.83203125" customWidth="1"/>
+    <col min="7120" max="7120" width="10.83203125" customWidth="1"/>
+    <col min="7136" max="7156" width="10.83203125" customWidth="1"/>
+    <col min="7158" max="7163" width="10.83203125" customWidth="1"/>
+    <col min="7165" max="7166" width="10.83203125" customWidth="1"/>
+    <col min="7170" max="7172" width="10.83203125" customWidth="1"/>
+    <col min="7174" max="7176" width="10.83203125" customWidth="1"/>
+    <col min="7178" max="7180" width="10.83203125" customWidth="1"/>
+    <col min="7182" max="7182" width="10.83203125" customWidth="1"/>
+    <col min="7184" max="7184" width="10.83203125" customWidth="1"/>
+    <col min="7200" max="7220" width="10.83203125" customWidth="1"/>
+    <col min="7223" max="7225" width="10.83203125" customWidth="1"/>
+    <col min="7228" max="7228" width="10.83203125" customWidth="1"/>
+    <col min="7230" max="7230" width="10.83203125" customWidth="1"/>
+    <col min="7232" max="7232" width="10.83203125" customWidth="1"/>
+    <col min="7234" max="7234" width="10.83203125" customWidth="1"/>
+    <col min="7236" max="7237" width="10.83203125" customWidth="1"/>
+    <col min="7241" max="7243" width="10.83203125" customWidth="1"/>
+    <col min="7245" max="7261" width="10.83203125" customWidth="1"/>
+    <col min="7264" max="7285" width="10.83203125" customWidth="1"/>
+    <col min="7287" max="7316" width="10.83203125" customWidth="1"/>
+    <col min="7319" max="7349" width="10.83203125" customWidth="1"/>
+    <col min="7351" max="7352" width="10.83203125" customWidth="1"/>
+    <col min="7354" max="7355" width="10.83203125" customWidth="1"/>
+    <col min="7357" max="7358" width="10.83203125" customWidth="1"/>
+    <col min="7362" max="7364" width="10.83203125" customWidth="1"/>
+    <col min="7366" max="7368" width="10.83203125" customWidth="1"/>
+    <col min="7370" max="7372" width="10.83203125" customWidth="1"/>
+    <col min="7374" max="7374" width="10.83203125" customWidth="1"/>
+    <col min="7376" max="7376" width="10.83203125" customWidth="1"/>
+    <col min="7392" max="7412" width="10.83203125" customWidth="1"/>
+    <col min="7415" max="7419" width="10.83203125" customWidth="1"/>
+    <col min="7421" max="7422" width="10.83203125" customWidth="1"/>
+    <col min="7426" max="7428" width="10.83203125" customWidth="1"/>
+    <col min="7430" max="7432" width="10.83203125" customWidth="1"/>
+    <col min="7434" max="7436" width="10.83203125" customWidth="1"/>
+    <col min="7438" max="7438" width="10.83203125" customWidth="1"/>
+    <col min="7440" max="7440" width="10.83203125" customWidth="1"/>
+    <col min="7456" max="7486" width="10.83203125" customWidth="1"/>
+    <col min="7491" max="7494" width="10.83203125" customWidth="1"/>
+    <col min="7496" max="7499" width="10.83203125" customWidth="1"/>
+    <col min="7502" max="7504" width="10.83203125" customWidth="1"/>
+    <col min="7506" max="7536" width="10.83203125" customWidth="1"/>
+    <col min="7540" max="7542" width="10.83203125" customWidth="1"/>
+    <col min="7544" max="7605" width="10.83203125" customWidth="1"/>
+    <col min="7607" max="7607" width="10.83203125" customWidth="1"/>
+    <col min="7610" max="7611" width="10.83203125" customWidth="1"/>
+    <col min="7613" max="7614" width="10.83203125" customWidth="1"/>
+    <col min="7618" max="7620" width="10.83203125" customWidth="1"/>
+    <col min="7622" max="7624" width="10.83203125" customWidth="1"/>
+    <col min="7626" max="7628" width="10.83203125" customWidth="1"/>
+    <col min="7630" max="7630" width="10.83203125" customWidth="1"/>
+    <col min="7632" max="7632" width="10.83203125" customWidth="1"/>
+    <col min="7648" max="7668" width="10.83203125" customWidth="1"/>
+    <col min="7671" max="7673" width="10.83203125" customWidth="1"/>
+    <col min="7676" max="7676" width="10.83203125" customWidth="1"/>
+    <col min="7678" max="7678" width="10.83203125" customWidth="1"/>
+    <col min="7680" max="7680" width="10.83203125" customWidth="1"/>
+    <col min="7682" max="7682" width="10.83203125" customWidth="1"/>
+    <col min="7684" max="7685" width="10.83203125" customWidth="1"/>
+    <col min="7689" max="7691" width="10.83203125" customWidth="1"/>
+    <col min="7693" max="7709" width="10.83203125" customWidth="1"/>
+    <col min="7712" max="7728" width="10.83203125" customWidth="1"/>
+    <col min="7730" max="7737" width="10.83203125" customWidth="1"/>
+    <col min="7739" max="7740" width="10.83203125" customWidth="1"/>
+    <col min="7743" max="7744" width="10.83203125" customWidth="1"/>
+    <col min="7746" max="7760" width="10.83203125" customWidth="1"/>
+    <col min="7762" max="7793" width="10.83203125" customWidth="1"/>
+    <col min="7796" max="7797" width="10.83203125" customWidth="1"/>
+    <col min="7800" max="7809" width="10.83203125" customWidth="1"/>
+    <col min="7811" max="7815" width="10.83203125" customWidth="1"/>
+    <col min="7817" max="7819" width="10.83203125" customWidth="1"/>
+    <col min="7822" max="7822" width="10.83203125" customWidth="1"/>
+    <col min="7824" max="7825" width="10.83203125" customWidth="1"/>
+    <col min="7829" max="7829" width="10.83203125" customWidth="1"/>
+    <col min="7831" max="7832" width="10.83203125" customWidth="1"/>
+    <col min="7834" max="7834" width="10.83203125" customWidth="1"/>
+    <col min="7836" max="7836" width="10.83203125" customWidth="1"/>
+    <col min="7839" max="7841" width="10.83203125" customWidth="1"/>
+    <col min="7844" max="7846" width="10.83203125" customWidth="1"/>
+    <col min="7852" max="7852" width="10.83203125" customWidth="1"/>
+    <col min="7854" max="7860" width="10.83203125" customWidth="1"/>
+    <col min="7863" max="7996" width="10.83203125" customWidth="1"/>
+    <col min="7998" max="8039" width="10.83203125" customWidth="1"/>
+    <col min="8049" max="8049" width="10.83203125" customWidth="1"/>
+    <col min="8052" max="8053" width="10.83203125" customWidth="1"/>
+    <col min="8056" max="8065" width="10.83203125" customWidth="1"/>
+    <col min="8067" max="8071" width="10.83203125" customWidth="1"/>
+    <col min="8073" max="8075" width="10.83203125" customWidth="1"/>
+    <col min="8078" max="8078" width="10.83203125" customWidth="1"/>
+    <col min="8080" max="8081" width="10.83203125" customWidth="1"/>
+    <col min="8085" max="8085" width="10.83203125" customWidth="1"/>
+    <col min="8087" max="8088" width="10.83203125" customWidth="1"/>
+    <col min="8090" max="8090" width="10.83203125" customWidth="1"/>
+    <col min="8092" max="8092" width="10.83203125" customWidth="1"/>
+    <col min="8095" max="8097" width="10.83203125" customWidth="1"/>
+    <col min="8100" max="8102" width="10.83203125" customWidth="1"/>
+    <col min="8108" max="8108" width="10.83203125" customWidth="1"/>
+    <col min="8110" max="8176" width="10.83203125" customWidth="1"/>
+    <col min="8179" max="8374" width="10.83203125" customWidth="1"/>
+    <col min="8377" max="8377" width="10.83203125" customWidth="1"/>
+    <col min="8381" max="8382" width="10.83203125" customWidth="1"/>
+    <col min="8384" max="8384" width="10.83203125" customWidth="1"/>
+    <col min="8388" max="8390" width="10.83203125" customWidth="1"/>
+    <col min="8392" max="8393" width="10.83203125" customWidth="1"/>
+    <col min="8395" max="8413" width="10.83203125" customWidth="1"/>
+    <col min="8416" max="8436" width="10.83203125" customWidth="1"/>
+    <col min="8441" max="8443" width="10.83203125" customWidth="1"/>
+    <col min="8445" max="8446" width="10.83203125" customWidth="1"/>
+    <col min="8450" max="8452" width="10.83203125" customWidth="1"/>
+    <col min="8454" max="8456" width="10.83203125" customWidth="1"/>
+    <col min="8458" max="8460" width="10.83203125" customWidth="1"/>
+    <col min="8462" max="8462" width="10.83203125" customWidth="1"/>
+    <col min="8464" max="8464" width="10.83203125" customWidth="1"/>
+    <col min="8480" max="8496" width="10.83203125" customWidth="1"/>
+    <col min="8500" max="8501" width="10.83203125" customWidth="1"/>
+    <col min="8505" max="8506" width="10.83203125" customWidth="1"/>
+    <col min="8509" max="8510" width="10.83203125" customWidth="1"/>
+    <col min="8512" max="8513" width="10.83203125" customWidth="1"/>
+    <col min="8516" max="8516" width="10.83203125" customWidth="1"/>
+    <col min="8520" max="8522" width="10.83203125" customWidth="1"/>
+    <col min="8526" max="8527" width="10.83203125" customWidth="1"/>
+    <col min="8544" max="8630" width="10.83203125" customWidth="1"/>
+    <col min="8633" max="8633" width="10.83203125" customWidth="1"/>
+    <col min="8637" max="8638" width="10.83203125" customWidth="1"/>
+    <col min="8640" max="8640" width="10.83203125" customWidth="1"/>
+    <col min="8644" max="8646" width="10.83203125" customWidth="1"/>
+    <col min="8648" max="8649" width="10.83203125" customWidth="1"/>
+    <col min="8651" max="8669" width="10.83203125" customWidth="1"/>
+    <col min="8672" max="8696" width="10.83203125" customWidth="1"/>
+    <col min="8698" max="8699" width="10.83203125" customWidth="1"/>
+    <col min="8701" max="8702" width="10.83203125" customWidth="1"/>
+    <col min="8706" max="8708" width="10.83203125" customWidth="1"/>
+    <col min="8710" max="8712" width="10.83203125" customWidth="1"/>
+    <col min="8714" max="8716" width="10.83203125" customWidth="1"/>
+    <col min="8718" max="8718" width="10.83203125" customWidth="1"/>
+    <col min="8720" max="8720" width="10.83203125" customWidth="1"/>
+    <col min="8736" max="8752" width="10.83203125" customWidth="1"/>
+    <col min="8756" max="8757" width="10.83203125" customWidth="1"/>
+    <col min="8761" max="8762" width="10.83203125" customWidth="1"/>
+    <col min="8765" max="8766" width="10.83203125" customWidth="1"/>
+    <col min="8768" max="8769" width="10.83203125" customWidth="1"/>
+    <col min="8772" max="8772" width="10.83203125" customWidth="1"/>
+    <col min="8776" max="8778" width="10.83203125" customWidth="1"/>
+    <col min="8782" max="8783" width="10.83203125" customWidth="1"/>
+    <col min="8785" max="8949" width="10.83203125" customWidth="1"/>
+    <col min="8951" max="8952" width="10.83203125" customWidth="1"/>
+    <col min="8954" max="8955" width="10.83203125" customWidth="1"/>
+    <col min="8957" max="8958" width="10.83203125" customWidth="1"/>
+    <col min="8962" max="8964" width="10.83203125" customWidth="1"/>
+    <col min="8966" max="8968" width="10.83203125" customWidth="1"/>
+    <col min="8970" max="8972" width="10.83203125" customWidth="1"/>
+    <col min="8974" max="8974" width="10.83203125" customWidth="1"/>
+    <col min="8976" max="8976" width="10.83203125" customWidth="1"/>
+    <col min="8992" max="9008" width="10.83203125" customWidth="1"/>
+    <col min="9010" max="9017" width="10.83203125" customWidth="1"/>
+    <col min="9019" max="9020" width="10.83203125" customWidth="1"/>
+    <col min="9023" max="9024" width="10.83203125" customWidth="1"/>
+    <col min="9026" max="9201" width="10.83203125" customWidth="1"/>
+    <col min="9204" max="9205" width="10.83203125" customWidth="1"/>
+    <col min="9208" max="9217" width="10.83203125" customWidth="1"/>
+    <col min="9219" max="9223" width="10.83203125" customWidth="1"/>
+    <col min="9225" max="9227" width="10.83203125" customWidth="1"/>
+    <col min="9230" max="9230" width="10.83203125" customWidth="1"/>
+    <col min="9232" max="9233" width="10.83203125" customWidth="1"/>
+    <col min="9237" max="9237" width="10.83203125" customWidth="1"/>
+    <col min="9239" max="9240" width="10.83203125" customWidth="1"/>
+    <col min="9242" max="9242" width="10.83203125" customWidth="1"/>
+    <col min="9244" max="9244" width="10.83203125" customWidth="1"/>
+    <col min="9247" max="9249" width="10.83203125" customWidth="1"/>
+    <col min="9252" max="9254" width="10.83203125" customWidth="1"/>
+    <col min="9260" max="9260" width="10.83203125" customWidth="1"/>
+    <col min="9262" max="9268" width="10.83203125" customWidth="1"/>
+    <col min="9271" max="9273" width="10.83203125" customWidth="1"/>
+    <col min="9276" max="9276" width="10.83203125" customWidth="1"/>
+    <col min="9278" max="9278" width="10.83203125" customWidth="1"/>
+    <col min="9280" max="9280" width="10.83203125" customWidth="1"/>
+    <col min="9282" max="9282" width="10.83203125" customWidth="1"/>
+    <col min="9284" max="9285" width="10.83203125" customWidth="1"/>
+    <col min="9289" max="9291" width="10.83203125" customWidth="1"/>
+    <col min="9293" max="9309" width="10.83203125" customWidth="1"/>
+    <col min="9312" max="9328" width="10.83203125" customWidth="1"/>
+    <col min="9332" max="9334" width="10.83203125" customWidth="1"/>
+    <col min="9336" max="9396" width="10.83203125" customWidth="1"/>
+    <col min="9399" max="9401" width="10.83203125" customWidth="1"/>
+    <col min="9404" max="9404" width="10.83203125" customWidth="1"/>
+    <col min="9406" max="9406" width="10.83203125" customWidth="1"/>
+    <col min="9408" max="9408" width="10.83203125" customWidth="1"/>
+    <col min="9410" max="9410" width="10.83203125" customWidth="1"/>
+    <col min="9412" max="9413" width="10.83203125" customWidth="1"/>
+    <col min="9417" max="9419" width="10.83203125" customWidth="1"/>
+    <col min="9421" max="9437" width="10.83203125" customWidth="1"/>
+    <col min="9440" max="9456" width="10.83203125" customWidth="1"/>
+    <col min="9460" max="9462" width="10.83203125" customWidth="1"/>
+    <col min="9464" max="9526" width="10.83203125" customWidth="1"/>
+    <col min="9528" max="9529" width="10.83203125" customWidth="1"/>
+    <col min="9531" max="9531" width="10.83203125" customWidth="1"/>
+    <col min="9533" max="9534" width="10.83203125" customWidth="1"/>
+    <col min="9538" max="9540" width="10.83203125" customWidth="1"/>
+    <col min="9542" max="9544" width="10.83203125" customWidth="1"/>
+    <col min="9546" max="9548" width="10.83203125" customWidth="1"/>
+    <col min="9550" max="9550" width="10.83203125" customWidth="1"/>
+    <col min="9552" max="9552" width="10.83203125" customWidth="1"/>
+    <col min="9568" max="9588" width="10.83203125" customWidth="1"/>
+    <col min="9591" max="9593" width="10.83203125" customWidth="1"/>
+    <col min="9596" max="9596" width="10.83203125" customWidth="1"/>
+    <col min="9598" max="9598" width="10.83203125" customWidth="1"/>
+    <col min="9600" max="9600" width="10.83203125" customWidth="1"/>
+    <col min="9602" max="9602" width="10.83203125" customWidth="1"/>
+    <col min="9604" max="9605" width="10.83203125" customWidth="1"/>
+    <col min="9609" max="9611" width="10.83203125" customWidth="1"/>
+    <col min="9613" max="9629" width="10.83203125" customWidth="1"/>
+    <col min="9632" max="9654" width="10.83203125" customWidth="1"/>
+    <col min="9656" max="9660" width="10.83203125" customWidth="1"/>
+    <col min="9662" max="9663" width="10.83203125" customWidth="1"/>
+    <col min="9667" max="9669" width="10.83203125" customWidth="1"/>
+    <col min="9672" max="9672" width="10.83203125" customWidth="1"/>
+    <col min="9674" max="9676" width="10.83203125" customWidth="1"/>
+    <col min="9679" max="9679" width="10.83203125" customWidth="1"/>
+    <col min="9696" max="9713" width="10.83203125" customWidth="1"/>
+    <col min="9716" max="9717" width="10.83203125" customWidth="1"/>
+    <col min="9720" max="9729" width="10.83203125" customWidth="1"/>
+    <col min="9731" max="9735" width="10.83203125" customWidth="1"/>
+    <col min="9737" max="9739" width="10.83203125" customWidth="1"/>
+    <col min="9742" max="9742" width="10.83203125" customWidth="1"/>
+    <col min="9744" max="9745" width="10.83203125" customWidth="1"/>
+    <col min="9749" max="9749" width="10.83203125" customWidth="1"/>
+    <col min="9751" max="9752" width="10.83203125" customWidth="1"/>
+    <col min="9754" max="9754" width="10.83203125" customWidth="1"/>
+    <col min="9756" max="9756" width="10.83203125" customWidth="1"/>
+    <col min="9759" max="9761" width="10.83203125" customWidth="1"/>
+    <col min="9764" max="9766" width="10.83203125" customWidth="1"/>
+    <col min="9772" max="9772" width="10.83203125" customWidth="1"/>
+    <col min="9774" max="9777" width="10.83203125" customWidth="1"/>
+    <col min="9780" max="9781" width="10.83203125" customWidth="1"/>
+    <col min="9784" max="9793" width="10.83203125" customWidth="1"/>
+    <col min="9795" max="9799" width="10.83203125" customWidth="1"/>
+    <col min="9801" max="9803" width="10.83203125" customWidth="1"/>
+    <col min="9806" max="9806" width="10.83203125" customWidth="1"/>
+    <col min="9808" max="9809" width="10.83203125" customWidth="1"/>
+    <col min="9813" max="9813" width="10.83203125" customWidth="1"/>
+    <col min="9815" max="9816" width="10.83203125" customWidth="1"/>
+    <col min="9818" max="9818" width="10.83203125" customWidth="1"/>
+    <col min="9820" max="9820" width="10.83203125" customWidth="1"/>
+    <col min="9823" max="9825" width="10.83203125" customWidth="1"/>
+    <col min="9828" max="9830" width="10.83203125" customWidth="1"/>
+    <col min="9836" max="9836" width="10.83203125" customWidth="1"/>
+    <col min="9838" max="9844" width="10.83203125" customWidth="1"/>
+    <col min="9849" max="9852" width="10.83203125" customWidth="1"/>
+    <col min="9854" max="9855" width="10.83203125" customWidth="1"/>
+    <col min="9857" max="9857" width="10.83203125" customWidth="1"/>
+    <col min="9859" max="9861" width="10.83203125" customWidth="1"/>
+    <col min="9865" max="9865" width="10.83203125" customWidth="1"/>
+    <col min="9867" max="9867" width="10.83203125" customWidth="1"/>
+    <col min="9871" max="9871" width="10.83203125" customWidth="1"/>
+    <col min="9888" max="9908" width="10.83203125" customWidth="1"/>
+    <col min="9910" max="9910" width="10.83203125" customWidth="1"/>
+    <col min="9912" max="9912" width="10.83203125" customWidth="1"/>
+    <col min="9914" max="9914" width="10.83203125" customWidth="1"/>
+    <col min="9917" max="9918" width="10.83203125" customWidth="1"/>
+    <col min="9922" max="9924" width="10.83203125" customWidth="1"/>
+    <col min="9926" max="9928" width="10.83203125" customWidth="1"/>
+    <col min="9930" max="9932" width="10.83203125" customWidth="1"/>
+    <col min="9934" max="9934" width="10.83203125" customWidth="1"/>
+    <col min="9936" max="9936" width="10.83203125" customWidth="1"/>
+    <col min="9952" max="9968" width="10.83203125" customWidth="1"/>
+    <col min="10033" max="10035" width="10.83203125" customWidth="1"/>
+    <col min="10037" max="10038" width="10.83203125" customWidth="1"/>
+    <col min="10040" max="10041" width="10.83203125" customWidth="1"/>
+    <col min="10044" max="10046" width="10.83203125" customWidth="1"/>
+    <col min="10050" max="10052" width="10.83203125" customWidth="1"/>
+    <col min="10054" max="10056" width="10.83203125" customWidth="1"/>
+    <col min="10058" max="10060" width="10.83203125" customWidth="1"/>
+    <col min="10062" max="10062" width="10.83203125" customWidth="1"/>
+    <col min="10064" max="10064" width="10.83203125" customWidth="1"/>
+    <col min="10080" max="10100" width="10.83203125" customWidth="1"/>
+    <col min="10103" max="10105" width="10.83203125" customWidth="1"/>
+    <col min="10108" max="10110" width="10.83203125" customWidth="1"/>
+    <col min="10114" max="10116" width="10.83203125" customWidth="1"/>
+    <col min="10118" max="10120" width="10.83203125" customWidth="1"/>
+    <col min="10122" max="10124" width="10.83203125" customWidth="1"/>
+    <col min="10126" max="10126" width="10.83203125" customWidth="1"/>
+    <col min="10128" max="10128" width="10.83203125" customWidth="1"/>
+    <col min="10144" max="10160" width="10.83203125" customWidth="1"/>
+    <col min="10163" max="10165" width="10.83203125" customWidth="1"/>
+    <col min="10167" max="10170" width="10.83203125" customWidth="1"/>
+    <col min="10172" max="10172" width="10.83203125" customWidth="1"/>
+    <col min="10174" max="10176" width="10.83203125" customWidth="1"/>
+    <col min="10178" max="10178" width="10.83203125" customWidth="1"/>
+    <col min="10186" max="10188" width="10.83203125" customWidth="1"/>
+    <col min="10191" max="10191" width="10.83203125" customWidth="1"/>
+    <col min="10208" max="10224" width="10.83203125" customWidth="1"/>
+    <col min="10289" max="10294" width="10.83203125" customWidth="1"/>
+    <col min="10297" max="10299" width="10.83203125" customWidth="1"/>
+    <col min="10301" max="10302" width="10.83203125" customWidth="1"/>
+    <col min="10306" max="10308" width="10.83203125" customWidth="1"/>
+    <col min="10310" max="10312" width="10.83203125" customWidth="1"/>
+    <col min="10314" max="10316" width="10.83203125" customWidth="1"/>
+    <col min="10318" max="10318" width="10.83203125" customWidth="1"/>
+    <col min="10320" max="10320" width="10.83203125" customWidth="1"/>
+    <col min="10336" max="10356" width="10.83203125" customWidth="1"/>
+    <col min="10358" max="10358" width="10.83203125" customWidth="1"/>
+    <col min="10360" max="10361" width="10.83203125" customWidth="1"/>
+    <col min="10364" max="10366" width="10.83203125" customWidth="1"/>
+    <col min="10370" max="10372" width="10.83203125" customWidth="1"/>
+    <col min="10374" max="10376" width="10.83203125" customWidth="1"/>
+    <col min="10378" max="10380" width="10.83203125" customWidth="1"/>
+    <col min="10382" max="10382" width="10.83203125" customWidth="1"/>
+    <col min="10384" max="10384" width="10.83203125" customWidth="1"/>
+    <col min="10400" max="10416" width="10.83203125" customWidth="1"/>
+    <col min="10419" max="10421" width="10.83203125" customWidth="1"/>
+    <col min="10423" max="10426" width="10.83203125" customWidth="1"/>
+    <col min="10428" max="10428" width="10.83203125" customWidth="1"/>
+    <col min="10430" max="10432" width="10.83203125" customWidth="1"/>
+    <col min="10434" max="10434" width="10.83203125" customWidth="1"/>
+    <col min="10442" max="10444" width="10.83203125" customWidth="1"/>
+    <col min="10447" max="10447" width="10.83203125" customWidth="1"/>
+    <col min="10464" max="10480" width="10.83203125" customWidth="1"/>
+    <col min="10483" max="10483" width="10.83203125" customWidth="1"/>
+    <col min="10485" max="10485" width="10.83203125" customWidth="1"/>
+    <col min="10488" max="10490" width="10.83203125" customWidth="1"/>
+    <col min="10492" max="10492" width="10.83203125" customWidth="1"/>
+    <col min="10496" max="10496" width="10.83203125" customWidth="1"/>
+    <col min="10501" max="10501" width="10.83203125" customWidth="1"/>
+    <col min="10504" max="10508" width="10.83203125" customWidth="1"/>
+    <col min="10512" max="10512" width="10.83203125" customWidth="1"/>
+    <col min="10517" max="10517" width="10.83203125" customWidth="1"/>
+    <col min="10519" max="10520" width="10.83203125" customWidth="1"/>
+    <col min="10522" max="10522" width="10.83203125" customWidth="1"/>
+    <col min="10525" max="10526" width="10.83203125" customWidth="1"/>
+    <col min="10528" max="10528" width="10.83203125" customWidth="1"/>
+    <col min="10530" max="10530" width="10.83203125" customWidth="1"/>
+    <col min="10532" max="10533" width="10.83203125" customWidth="1"/>
+    <col min="10536" max="10537" width="10.83203125" customWidth="1"/>
+    <col min="10539" max="10540" width="10.83203125" customWidth="1"/>
+    <col min="10544" max="10549" width="10.83203125" customWidth="1"/>
+    <col min="10553" max="10555" width="10.83203125" customWidth="1"/>
+    <col min="10557" max="10558" width="10.83203125" customWidth="1"/>
+    <col min="10562" max="10564" width="10.83203125" customWidth="1"/>
+    <col min="10566" max="10568" width="10.83203125" customWidth="1"/>
+    <col min="10570" max="10572" width="10.83203125" customWidth="1"/>
+    <col min="10574" max="10574" width="10.83203125" customWidth="1"/>
+    <col min="10576" max="10576" width="10.83203125" customWidth="1"/>
+    <col min="10592" max="10608" width="10.83203125" customWidth="1"/>
+    <col min="10610" max="10610" width="10.83203125" customWidth="1"/>
+    <col min="10613" max="10613" width="10.83203125" customWidth="1"/>
+    <col min="10615" max="10616" width="10.83203125" customWidth="1"/>
+    <col min="10619" max="10622" width="10.83203125" customWidth="1"/>
+    <col min="10624" max="10624" width="10.83203125" customWidth="1"/>
+    <col min="10629" max="10629" width="10.83203125" customWidth="1"/>
+    <col min="10632" max="10633" width="10.83203125" customWidth="1"/>
+    <col min="10637" max="10637" width="10.83203125" customWidth="1"/>
+    <col min="10640" max="10641" width="10.83203125" customWidth="1"/>
+    <col min="10644" max="10645" width="10.83203125" customWidth="1"/>
+    <col min="10648" max="10648" width="10.83203125" customWidth="1"/>
+    <col min="10650" max="10651" width="10.83203125" customWidth="1"/>
+    <col min="10653" max="10653" width="10.83203125" customWidth="1"/>
+    <col min="10656" max="10656" width="10.83203125" customWidth="1"/>
+    <col min="10660" max="10661" width="10.83203125" customWidth="1"/>
+    <col min="10664" max="10664" width="10.83203125" customWidth="1"/>
+    <col min="10666" max="10666" width="10.83203125" customWidth="1"/>
+    <col min="10668" max="10668" width="10.83203125" customWidth="1"/>
+    <col min="10672" max="10673" width="10.83203125" customWidth="1"/>
+    <col min="10675" max="10676" width="10.83203125" customWidth="1"/>
+    <col min="10680" max="10680" width="10.83203125" customWidth="1"/>
+    <col min="10682" max="10685" width="10.83203125" customWidth="1"/>
+    <col min="10688" max="10690" width="10.83203125" customWidth="1"/>
+    <col min="10692" max="10692" width="10.83203125" customWidth="1"/>
+    <col min="10696" max="10696" width="10.83203125" customWidth="1"/>
+    <col min="10698" max="10699" width="10.83203125" customWidth="1"/>
+    <col min="10701" max="10701" width="10.83203125" customWidth="1"/>
+    <col min="10704" max="10704" width="10.83203125" customWidth="1"/>
+    <col min="10709" max="10709" width="10.83203125" customWidth="1"/>
+    <col min="10712" max="10713" width="10.83203125" customWidth="1"/>
+    <col min="10717" max="10717" width="10.83203125" customWidth="1"/>
+    <col min="10720" max="10720" width="10.83203125" customWidth="1"/>
+    <col min="10722" max="10722" width="10.83203125" customWidth="1"/>
+    <col min="10725" max="10725" width="10.83203125" customWidth="1"/>
+    <col min="10727" max="10730" width="10.83203125" customWidth="1"/>
+    <col min="10732" max="10732" width="10.83203125" customWidth="1"/>
+    <col min="10734" max="10734" width="10.83203125" customWidth="1"/>
+    <col min="10736" max="10736" width="10.83203125" customWidth="1"/>
+    <col min="10741" max="10741" width="10.83203125" customWidth="1"/>
+    <col min="10744" max="10744" width="10.83203125" customWidth="1"/>
+    <col min="10749" max="10749" width="10.83203125" customWidth="1"/>
+    <col min="10752" max="10754" width="10.83203125" customWidth="1"/>
+    <col min="10757" max="10757" width="10.83203125" customWidth="1"/>
+    <col min="10760" max="10760" width="10.83203125" customWidth="1"/>
+    <col min="10762" max="10762" width="10.83203125" customWidth="1"/>
+    <col min="10765" max="10765" width="10.83203125" customWidth="1"/>
+    <col min="10767" max="10768" width="10.83203125" customWidth="1"/>
+    <col min="10770" max="10770" width="10.83203125" customWidth="1"/>
+    <col min="10773" max="10773" width="10.83203125" customWidth="1"/>
+    <col min="10776" max="10776" width="10.83203125" customWidth="1"/>
+    <col min="10778" max="10781" width="10.83203125" customWidth="1"/>
+    <col min="10784" max="10784" width="10.83203125" customWidth="1"/>
+    <col min="10787" max="10788" width="10.83203125" customWidth="1"/>
+    <col min="10792" max="10794" width="10.83203125" customWidth="1"/>
+    <col min="10796" max="10796" width="10.83203125" customWidth="1"/>
+    <col min="10800" max="10800" width="10.83203125" customWidth="1"/>
+    <col min="10802" max="10802" width="10.83203125" customWidth="1"/>
+    <col min="10804" max="10805" width="10.83203125" customWidth="1"/>
+    <col min="10808" max="10809" width="10.83203125" customWidth="1"/>
+    <col min="10811" max="10812" width="10.83203125" customWidth="1"/>
+    <col min="10816" max="10816" width="10.83203125" customWidth="1"/>
+    <col min="10821" max="10821" width="10.83203125" customWidth="1"/>
+    <col min="10823" max="10826" width="10.83203125" customWidth="1"/>
+    <col min="10828" max="10828" width="10.83203125" customWidth="1"/>
+    <col min="10832" max="10832" width="10.83203125" customWidth="1"/>
+    <col min="10834" max="10834" width="10.83203125" customWidth="1"/>
+    <col min="10836" max="10837" width="10.83203125" customWidth="1"/>
+    <col min="10840" max="10840" width="10.83203125" customWidth="1"/>
+    <col min="10842" max="10842" width="10.83203125" customWidth="1"/>
+    <col min="10845" max="10845" width="10.83203125" customWidth="1"/>
+    <col min="10848" max="10852" width="10.83203125" customWidth="1"/>
+    <col min="10856" max="10858" width="10.83203125" customWidth="1"/>
+    <col min="10861" max="10861" width="10.83203125" customWidth="1"/>
+    <col min="10864" max="10864" width="10.83203125" customWidth="1"/>
+    <col min="10866" max="10869" width="10.83203125" customWidth="1"/>
+    <col min="10872" max="10874" width="10.83203125" customWidth="1"/>
+    <col min="10876" max="10876" width="10.83203125" customWidth="1"/>
+    <col min="10880" max="10880" width="10.83203125" customWidth="1"/>
+    <col min="10882" max="10882" width="10.83203125" customWidth="1"/>
+    <col min="10884" max="10885" width="10.83203125" customWidth="1"/>
+    <col min="10888" max="10889" width="10.83203125" customWidth="1"/>
+    <col min="10893" max="10893" width="10.83203125" customWidth="1"/>
+    <col min="10895" max="10899" width="10.83203125" customWidth="1"/>
+    <col min="10904" max="10906" width="10.83203125" customWidth="1"/>
+    <col min="10909" max="10909" width="10.83203125" customWidth="1"/>
+    <col min="10912" max="10912" width="10.83203125" customWidth="1"/>
+    <col min="10915" max="10916" width="10.83203125" customWidth="1"/>
+    <col min="10920" max="10928" width="10.83203125" customWidth="1"/>
+    <col min="10930" max="10931" width="10.83203125" customWidth="1"/>
+    <col min="10934" max="10997" width="10.83203125" customWidth="1"/>
+    <col min="10999" max="10999" width="10.83203125" customWidth="1"/>
+    <col min="11002" max="11003" width="10.83203125" customWidth="1"/>
+    <col min="11005" max="11006" width="10.83203125" customWidth="1"/>
+    <col min="11010" max="11012" width="10.83203125" customWidth="1"/>
+    <col min="11014" max="11016" width="10.83203125" customWidth="1"/>
+    <col min="11018" max="11020" width="10.83203125" customWidth="1"/>
+    <col min="11022" max="11022" width="10.83203125" customWidth="1"/>
+    <col min="11024" max="11024" width="10.83203125" customWidth="1"/>
+    <col min="11040" max="11056" width="10.83203125" customWidth="1"/>
+    <col min="11059" max="11059" width="10.83203125" customWidth="1"/>
+    <col min="11061" max="11063" width="10.83203125" customWidth="1"/>
+    <col min="11066" max="11067" width="10.83203125" customWidth="1"/>
+    <col min="11071" max="11071" width="10.83203125" customWidth="1"/>
+    <col min="11073" max="11073" width="10.83203125" customWidth="1"/>
+    <col min="11075" max="11075" width="10.83203125" customWidth="1"/>
+    <col min="11082" max="11084" width="10.83203125" customWidth="1"/>
+    <col min="11087" max="11087" width="10.83203125" customWidth="1"/>
+    <col min="11104" max="11122" width="10.83203125" customWidth="1"/>
+    <col min="11124" max="11187" width="10.83203125" customWidth="1"/>
+    <col min="11191" max="11195" width="10.83203125" customWidth="1"/>
+    <col min="11197" max="11198" width="10.83203125" customWidth="1"/>
+    <col min="11200" max="11201" width="10.83203125" customWidth="1"/>
+    <col min="11203" max="11204" width="10.83203125" customWidth="1"/>
+    <col min="11209" max="11214" width="10.83203125" customWidth="1"/>
+    <col min="11218" max="11218" width="10.83203125" customWidth="1"/>
+    <col min="11220" max="11220" width="10.83203125" customWidth="1"/>
+    <col min="11232" max="11253" width="10.83203125" customWidth="1"/>
+    <col min="11255" max="11255" width="10.83203125" customWidth="1"/>
+    <col min="11257" max="11259" width="10.83203125" customWidth="1"/>
+    <col min="11261" max="11262" width="10.83203125" customWidth="1"/>
+    <col min="11266" max="11268" width="10.83203125" customWidth="1"/>
+    <col min="11270" max="11272" width="10.83203125" customWidth="1"/>
+    <col min="11274" max="11276" width="10.83203125" customWidth="1"/>
+    <col min="11278" max="11278" width="10.83203125" customWidth="1"/>
+    <col min="11280" max="11280" width="10.83203125" customWidth="1"/>
+    <col min="11296" max="11376" width="10.83203125" customWidth="1"/>
+    <col min="11380" max="11443" width="10.83203125" customWidth="1"/>
+    <col min="11445" max="11508" width="10.83203125" customWidth="1"/>
+    <col min="11513" max="11513" width="10.83203125" customWidth="1"/>
+    <col min="11515" max="11515" width="10.83203125" customWidth="1"/>
+    <col min="11517" max="11518" width="10.83203125" customWidth="1"/>
+    <col min="11522" max="11524" width="10.83203125" customWidth="1"/>
+    <col min="11526" max="11528" width="10.83203125" customWidth="1"/>
+    <col min="11530" max="11532" width="10.83203125" customWidth="1"/>
+    <col min="11534" max="11534" width="10.83203125" customWidth="1"/>
+    <col min="11536" max="11536" width="10.83203125" customWidth="1"/>
+    <col min="11552" max="11571" width="10.83203125" customWidth="1"/>
+    <col min="11573" max="11573" width="10.83203125" customWidth="1"/>
+    <col min="11575" max="11575" width="10.83203125" customWidth="1"/>
+    <col min="11578" max="11578" width="10.83203125" customWidth="1"/>
+    <col min="11580" max="11580" width="10.83203125" customWidth="1"/>
+    <col min="11583" max="11583" width="10.83203125" customWidth="1"/>
+    <col min="11587" max="11588" width="10.83203125" customWidth="1"/>
+    <col min="11592" max="11594" width="10.83203125" customWidth="1"/>
+    <col min="11598" max="11599" width="10.83203125" customWidth="1"/>
+    <col min="11616" max="11633" width="10.83203125" customWidth="1"/>
+    <col min="11636" max="11637" width="10.83203125" customWidth="1"/>
+    <col min="11640" max="11649" width="10.83203125" customWidth="1"/>
+    <col min="11651" max="11655" width="10.83203125" customWidth="1"/>
+    <col min="11657" max="11659" width="10.83203125" customWidth="1"/>
+    <col min="11662" max="11662" width="10.83203125" customWidth="1"/>
+    <col min="11664" max="11665" width="10.83203125" customWidth="1"/>
+    <col min="11669" max="11669" width="10.83203125" customWidth="1"/>
+    <col min="11671" max="11672" width="10.83203125" customWidth="1"/>
+    <col min="11674" max="11674" width="10.83203125" customWidth="1"/>
+    <col min="11676" max="11676" width="10.83203125" customWidth="1"/>
+    <col min="11679" max="11681" width="10.83203125" customWidth="1"/>
+    <col min="11684" max="11686" width="10.83203125" customWidth="1"/>
+    <col min="11692" max="11692" width="10.83203125" customWidth="1"/>
+    <col min="11694" max="11704" width="10.83203125" customWidth="1"/>
+    <col min="11706" max="11707" width="10.83203125" customWidth="1"/>
+    <col min="11709" max="11710" width="10.83203125" customWidth="1"/>
+    <col min="11714" max="11716" width="10.83203125" customWidth="1"/>
+    <col min="11718" max="11720" width="10.83203125" customWidth="1"/>
+    <col min="11722" max="11724" width="10.83203125" customWidth="1"/>
+    <col min="11726" max="11726" width="10.83203125" customWidth="1"/>
+    <col min="11728" max="11728" width="10.83203125" customWidth="1"/>
+    <col min="11744" max="11761" width="10.83203125" customWidth="1"/>
+    <col min="11770" max="11831" width="10.83203125" customWidth="1"/>
+    <col min="11836" max="11836" width="10.83203125" customWidth="1"/>
+    <col min="11838" max="11838" width="10.83203125" customWidth="1"/>
+    <col min="11842" max="11844" width="10.83203125" customWidth="1"/>
+    <col min="11846" max="11848" width="10.83203125" customWidth="1"/>
+    <col min="11850" max="11852" width="10.83203125" customWidth="1"/>
+    <col min="11854" max="11854" width="10.83203125" customWidth="1"/>
+    <col min="11856" max="11856" width="10.83203125" customWidth="1"/>
+    <col min="11872" max="11889" width="10.83203125" customWidth="1"/>
+    <col min="11892" max="11893" width="10.83203125" customWidth="1"/>
+    <col min="11896" max="11905" width="10.83203125" customWidth="1"/>
+    <col min="11907" max="11911" width="10.83203125" customWidth="1"/>
+    <col min="11913" max="11915" width="10.83203125" customWidth="1"/>
+    <col min="11918" max="11918" width="10.83203125" customWidth="1"/>
+    <col min="11920" max="11921" width="10.83203125" customWidth="1"/>
+    <col min="11925" max="11925" width="10.83203125" customWidth="1"/>
+    <col min="11927" max="11928" width="10.83203125" customWidth="1"/>
+    <col min="11930" max="11930" width="10.83203125" customWidth="1"/>
+    <col min="11932" max="11932" width="10.83203125" customWidth="1"/>
+    <col min="11935" max="11937" width="10.83203125" customWidth="1"/>
+    <col min="11940" max="11942" width="10.83203125" customWidth="1"/>
+    <col min="11948" max="11948" width="10.83203125" customWidth="1"/>
+    <col min="11950" max="11952" width="10.83203125" customWidth="1"/>
+    <col min="11962" max="12021" width="10.83203125" customWidth="1"/>
+    <col min="12028" max="12030" width="10.83203125" customWidth="1"/>
+    <col min="12034" max="12036" width="10.83203125" customWidth="1"/>
+    <col min="12038" max="12040" width="10.83203125" customWidth="1"/>
+    <col min="12042" max="12044" width="10.83203125" customWidth="1"/>
+    <col min="12046" max="12046" width="10.83203125" customWidth="1"/>
+    <col min="12048" max="12048" width="10.83203125" customWidth="1"/>
+    <col min="12064" max="12081" width="10.83203125" customWidth="1"/>
+    <col min="12083" max="12083" width="10.83203125" customWidth="1"/>
+    <col min="12085" max="12085" width="10.83203125" customWidth="1"/>
+    <col min="12087" max="12088" width="10.83203125" customWidth="1"/>
+    <col min="12090" max="12091" width="10.83203125" customWidth="1"/>
+    <col min="12094" max="12094" width="10.83203125" customWidth="1"/>
+    <col min="12096" max="12096" width="10.83203125" customWidth="1"/>
+    <col min="12099" max="12099" width="10.83203125" customWidth="1"/>
+    <col min="12106" max="12108" width="10.83203125" customWidth="1"/>
+    <col min="12111" max="12111" width="10.83203125" customWidth="1"/>
+    <col min="12128" max="12145" width="10.83203125" customWidth="1"/>
+    <col min="12148" max="12149" width="10.83203125" customWidth="1"/>
+    <col min="12152" max="12161" width="10.83203125" customWidth="1"/>
+    <col min="12163" max="12167" width="10.83203125" customWidth="1"/>
+    <col min="12169" max="12171" width="10.83203125" customWidth="1"/>
+    <col min="12174" max="12174" width="10.83203125" customWidth="1"/>
+    <col min="12176" max="12177" width="10.83203125" customWidth="1"/>
+    <col min="12181" max="12181" width="10.83203125" customWidth="1"/>
+    <col min="12183" max="12184" width="10.83203125" customWidth="1"/>
+    <col min="12186" max="12186" width="10.83203125" customWidth="1"/>
+    <col min="12188" max="12188" width="10.83203125" customWidth="1"/>
+    <col min="12191" max="12193" width="10.83203125" customWidth="1"/>
+    <col min="12196" max="12198" width="10.83203125" customWidth="1"/>
+    <col min="12204" max="12204" width="10.83203125" customWidth="1"/>
+    <col min="12206" max="12208" width="10.83203125" customWidth="1"/>
+    <col min="12211" max="12216" width="10.83203125" customWidth="1"/>
+    <col min="12218" max="12219" width="10.83203125" customWidth="1"/>
+    <col min="12221" max="12222" width="10.83203125" customWidth="1"/>
+    <col min="12226" max="12228" width="10.83203125" customWidth="1"/>
+    <col min="12230" max="12232" width="10.83203125" customWidth="1"/>
+    <col min="12234" max="12236" width="10.83203125" customWidth="1"/>
+    <col min="12238" max="12238" width="10.83203125" customWidth="1"/>
+    <col min="12240" max="12240" width="10.83203125" customWidth="1"/>
+    <col min="12256" max="12283" width="10.83203125" customWidth="1"/>
+    <col min="12285" max="12286" width="10.83203125" customWidth="1"/>
+    <col min="12290" max="12292" width="10.83203125" customWidth="1"/>
+    <col min="12294" max="12296" width="10.83203125" customWidth="1"/>
+    <col min="12298" max="12300" width="10.83203125" customWidth="1"/>
+    <col min="12302" max="12302" width="10.83203125" customWidth="1"/>
+    <col min="12304" max="12304" width="10.83203125" customWidth="1"/>
+    <col min="12307" max="12307" width="10.83203125" customWidth="1"/>
+    <col min="12314" max="12339" width="10.83203125" customWidth="1"/>
+    <col min="12341" max="12345" width="10.83203125" customWidth="1"/>
+    <col min="12347" max="12352" width="10.83203125" customWidth="1"/>
+    <col min="12384" max="12408" width="10.83203125" customWidth="1"/>
+    <col min="12410" max="12411" width="10.83203125" customWidth="1"/>
+    <col min="12413" max="12414" width="10.83203125" customWidth="1"/>
+    <col min="12418" max="12420" width="10.83203125" customWidth="1"/>
+    <col min="12422" max="12424" width="10.83203125" customWidth="1"/>
+    <col min="12426" max="12428" width="10.83203125" customWidth="1"/>
+    <col min="12430" max="12430" width="10.83203125" customWidth="1"/>
+    <col min="12432" max="12432" width="10.83203125" customWidth="1"/>
+    <col min="12448" max="12465" width="10.83203125" customWidth="1"/>
+    <col min="12474" max="12496" width="10.83203125" customWidth="1"/>
+    <col min="12512" max="12528" width="10.83203125" customWidth="1"/>
+    <col min="12532" max="12533" width="10.83203125" customWidth="1"/>
+    <col min="12535" max="12537" width="10.83203125" customWidth="1"/>
+    <col min="12540" max="12540" width="10.83203125" customWidth="1"/>
+    <col min="12544" max="12544" width="10.83203125" customWidth="1"/>
+    <col min="12546" max="12546" width="10.83203125" customWidth="1"/>
+    <col min="12548" max="12548" width="10.83203125" customWidth="1"/>
+    <col min="12550" max="12560" width="10.83203125" customWidth="1"/>
+    <col min="12563" max="12563" width="10.83203125" customWidth="1"/>
+    <col min="12570" max="12595" width="10.83203125" customWidth="1"/>
+    <col min="12597" max="12601" width="10.83203125" customWidth="1"/>
+    <col min="12603" max="12608" width="10.83203125" customWidth="1"/>
+    <col min="12640" max="12661" width="10.83203125" customWidth="1"/>
+    <col min="12663" max="12664" width="10.83203125" customWidth="1"/>
+    <col min="12666" max="12667" width="10.83203125" customWidth="1"/>
+    <col min="12669" max="12670" width="10.83203125" customWidth="1"/>
+    <col min="12674" max="12676" width="10.83203125" customWidth="1"/>
+    <col min="12678" max="12680" width="10.83203125" customWidth="1"/>
+    <col min="12682" max="12684" width="10.83203125" customWidth="1"/>
+    <col min="12686" max="12686" width="10.83203125" customWidth="1"/>
+    <col min="12688" max="12688" width="10.83203125" customWidth="1"/>
+    <col min="12704" max="12721" width="10.83203125" customWidth="1"/>
+    <col min="12730" max="12752" width="10.83203125" customWidth="1"/>
+    <col min="12768" max="12784" width="10.83203125" customWidth="1"/>
+    <col min="12786" max="12880" width="10.83203125" customWidth="1"/>
+    <col min="12896" max="12915" width="10.83203125" customWidth="1"/>
+    <col min="12917" max="12976" width="10.83203125" customWidth="1"/>
+    <col min="12980" max="13043" width="10.83203125" customWidth="1"/>
+    <col min="13045" max="13045" width="10.83203125" customWidth="1"/>
+    <col min="13049" max="13049" width="10.83203125" customWidth="1"/>
+    <col min="13052" max="13054" width="10.83203125" customWidth="1"/>
+    <col min="13058" max="13060" width="10.83203125" customWidth="1"/>
+    <col min="13062" max="13064" width="10.83203125" customWidth="1"/>
+    <col min="13066" max="13068" width="10.83203125" customWidth="1"/>
+    <col min="13070" max="13070" width="10.83203125" customWidth="1"/>
+    <col min="13072" max="13072" width="10.83203125" customWidth="1"/>
+    <col min="13088" max="13232" width="10.83203125" customWidth="1"/>
+    <col min="13234" max="13277" width="10.83203125" customWidth="1"/>
+    <col min="13280" max="13299" width="10.83203125" customWidth="1"/>
+    <col min="13301" max="13304" width="10.83203125" customWidth="1"/>
+    <col min="13308" max="13310" width="10.83203125" customWidth="1"/>
+    <col min="13314" max="13316" width="10.83203125" customWidth="1"/>
+    <col min="13318" max="13320" width="10.83203125" customWidth="1"/>
+    <col min="13322" max="13324" width="10.83203125" customWidth="1"/>
+    <col min="13326" max="13326" width="10.83203125" customWidth="1"/>
+    <col min="13328" max="13328" width="10.83203125" customWidth="1"/>
+    <col min="13344" max="13438" width="10.83203125" customWidth="1"/>
+    <col min="13443" max="13446" width="10.83203125" customWidth="1"/>
+    <col min="13448" max="13451" width="10.83203125" customWidth="1"/>
+    <col min="13454" max="13456" width="10.83203125" customWidth="1"/>
+    <col min="13458" max="13553" width="10.83203125" customWidth="1"/>
+    <col min="13555" max="13557" width="10.83203125" customWidth="1"/>
+    <col min="13559" max="13559" width="10.83203125" customWidth="1"/>
+    <col min="13563" max="13563" width="10.83203125" customWidth="1"/>
+    <col min="13565" max="13565" width="10.83203125" customWidth="1"/>
+    <col min="13567" max="13567" width="10.83203125" customWidth="1"/>
+    <col min="13569" max="13569" width="10.83203125" customWidth="1"/>
+    <col min="13571" max="13571" width="10.83203125" customWidth="1"/>
+    <col min="13573" max="13573" width="10.83203125" customWidth="1"/>
+    <col min="13575" max="13575" width="10.83203125" customWidth="1"/>
+    <col min="13577" max="13577" width="10.83203125" customWidth="1"/>
+    <col min="13579" max="13580" width="10.83203125" customWidth="1"/>
+    <col min="13583" max="14064" width="10.83203125" customWidth="1"/>
+    <col min="14067" max="15153" width="10.83203125" customWidth="1"/>
+    <col min="15156" max="15157" width="10.83203125" customWidth="1"/>
+    <col min="15160" max="15169" width="10.83203125" customWidth="1"/>
+    <col min="15171" max="15175" width="10.83203125" customWidth="1"/>
+    <col min="15177" max="15179" width="10.83203125" customWidth="1"/>
+    <col min="15182" max="15182" width="10.83203125" customWidth="1"/>
+    <col min="15184" max="15185" width="10.83203125" customWidth="1"/>
+    <col min="15189" max="15189" width="10.83203125" customWidth="1"/>
+    <col min="15191" max="15192" width="10.83203125" customWidth="1"/>
+    <col min="15194" max="15194" width="10.83203125" customWidth="1"/>
+    <col min="15196" max="15196" width="10.83203125" customWidth="1"/>
+    <col min="15199" max="15201" width="10.83203125" customWidth="1"/>
+    <col min="15204" max="15206" width="10.83203125" customWidth="1"/>
+    <col min="15212" max="15212" width="10.83203125" customWidth="1"/>
+    <col min="15214" max="15217" width="10.83203125" customWidth="1"/>
+    <col min="15220" max="15221" width="10.83203125" customWidth="1"/>
+    <col min="15224" max="15233" width="10.83203125" customWidth="1"/>
+    <col min="15235" max="15239" width="10.83203125" customWidth="1"/>
+    <col min="15241" max="15243" width="10.83203125" customWidth="1"/>
+    <col min="15246" max="15246" width="10.83203125" customWidth="1"/>
+    <col min="15248" max="15249" width="10.83203125" customWidth="1"/>
+    <col min="15253" max="15253" width="10.83203125" customWidth="1"/>
+    <col min="15255" max="15256" width="10.83203125" customWidth="1"/>
+    <col min="15258" max="15258" width="10.83203125" customWidth="1"/>
+    <col min="15260" max="15260" width="10.83203125" customWidth="1"/>
+    <col min="15263" max="15265" width="10.83203125" customWidth="1"/>
+    <col min="15268" max="15270" width="10.83203125" customWidth="1"/>
+    <col min="15276" max="15276" width="10.83203125" customWidth="1"/>
+    <col min="15278" max="15283" width="10.83203125" customWidth="1"/>
+    <col min="15285" max="15286" width="10.83203125" customWidth="1"/>
+    <col min="15288" max="15289" width="10.83203125" customWidth="1"/>
+    <col min="15291" max="15291" width="10.83203125" customWidth="1"/>
+    <col min="15293" max="15294" width="10.83203125" customWidth="1"/>
+    <col min="15296" max="15297" width="10.83203125" customWidth="1"/>
+    <col min="15300" max="15304" width="10.83203125" customWidth="1"/>
+    <col min="15307" max="15308" width="10.83203125" customWidth="1"/>
+    <col min="15310" max="15312" width="10.83203125" customWidth="1"/>
+    <col min="15314" max="15483" width="10.83203125" customWidth="1"/>
+    <col min="15485" max="15486" width="10.83203125" customWidth="1"/>
+    <col min="15490" max="15492" width="10.83203125" customWidth="1"/>
+    <col min="15494" max="15496" width="10.83203125" customWidth="1"/>
+    <col min="15498" max="15500" width="10.83203125" customWidth="1"/>
+    <col min="15502" max="15502" width="10.83203125" customWidth="1"/>
+    <col min="15504" max="15504" width="10.83203125" customWidth="1"/>
+    <col min="15520" max="15536" width="10.83203125" customWidth="1"/>
+    <col min="15538" max="15538" width="10.83203125" customWidth="1"/>
+    <col min="15544" max="15544" width="10.83203125" customWidth="1"/>
+    <col min="15546" max="15547" width="10.83203125" customWidth="1"/>
+    <col min="15550" max="15550" width="10.83203125" customWidth="1"/>
+    <col min="15552" max="15552" width="10.83203125" customWidth="1"/>
+    <col min="15555" max="15555" width="10.83203125" customWidth="1"/>
+    <col min="15562" max="15564" width="10.83203125" customWidth="1"/>
+    <col min="15567" max="15567" width="10.83203125" customWidth="1"/>
+    <col min="15584" max="15606" width="10.83203125" customWidth="1"/>
+    <col min="15609" max="15611" width="10.83203125" customWidth="1"/>
+    <col min="15613" max="15614" width="10.83203125" customWidth="1"/>
+    <col min="15618" max="15620" width="10.83203125" customWidth="1"/>
+    <col min="15622" max="15624" width="10.83203125" customWidth="1"/>
+    <col min="15626" max="15628" width="10.83203125" customWidth="1"/>
+    <col min="15630" max="15630" width="10.83203125" customWidth="1"/>
+    <col min="15632" max="15632" width="10.83203125" customWidth="1"/>
+    <col min="15648" max="15732" width="10.83203125" customWidth="1"/>
+    <col min="15737" max="15739" width="10.83203125" customWidth="1"/>
+    <col min="15741" max="15742" width="10.83203125" customWidth="1"/>
+    <col min="15746" max="15748" width="10.83203125" customWidth="1"/>
+    <col min="15750" max="15752" width="10.83203125" customWidth="1"/>
+    <col min="15754" max="15756" width="10.83203125" customWidth="1"/>
+    <col min="15758" max="15758" width="10.83203125" customWidth="1"/>
+    <col min="15760" max="15760" width="10.83203125" customWidth="1"/>
+    <col min="15776" max="15792" width="10.83203125" customWidth="1"/>
+    <col min="15794" max="15794" width="10.83203125" customWidth="1"/>
+    <col min="15798" max="15801" width="10.83203125" customWidth="1"/>
+    <col min="15806" max="15806" width="10.83203125" customWidth="1"/>
+    <col min="15808" max="15809" width="10.83203125" customWidth="1"/>
+    <col min="15811" max="15811" width="10.83203125" customWidth="1"/>
+    <col min="15818" max="15820" width="10.83203125" customWidth="1"/>
+    <col min="15823" max="15823" width="10.83203125" customWidth="1"/>
+    <col min="15840" max="15861" width="10.83203125" customWidth="1"/>
+    <col min="15865" max="15867" width="10.83203125" customWidth="1"/>
+    <col min="15869" max="15870" width="10.83203125" customWidth="1"/>
+    <col min="15874" max="15876" width="10.83203125" customWidth="1"/>
+    <col min="15878" max="15880" width="10.83203125" customWidth="1"/>
+    <col min="15882" max="15884" width="10.83203125" customWidth="1"/>
+    <col min="15886" max="15886" width="10.83203125" customWidth="1"/>
+    <col min="15888" max="15888" width="10.83203125" customWidth="1"/>
+    <col min="15904" max="15921" width="10.83203125" customWidth="1"/>
+    <col min="15926" max="15927" width="10.83203125" customWidth="1"/>
+    <col min="15931" max="15933" width="10.83203125" customWidth="1"/>
+    <col min="15937" max="15937" width="10.83203125" customWidth="1"/>
+    <col min="15939" max="15940" width="10.83203125" customWidth="1"/>
+    <col min="15944" max="15946" width="10.83203125" customWidth="1"/>
+    <col min="15950" max="15951" width="10.83203125" customWidth="1"/>
+    <col min="15968" max="15988" width="10.83203125" customWidth="1"/>
+    <col min="15990" max="15992" width="10.83203125" customWidth="1"/>
+    <col min="15994" max="15995" width="10.83203125" customWidth="1"/>
+    <col min="15997" max="15998" width="10.83203125" customWidth="1"/>
+    <col min="16002" max="16004" width="10.83203125" customWidth="1"/>
+    <col min="16006" max="16008" width="10.83203125" customWidth="1"/>
+    <col min="16010" max="16012" width="10.83203125" customWidth="1"/>
+    <col min="16014" max="16014" width="10.83203125" customWidth="1"/>
+    <col min="16016" max="16016" width="10.83203125" customWidth="1"/>
+    <col min="16032" max="16048" width="10.83203125" customWidth="1"/>
+    <col min="16050" max="16050" width="10.83203125" customWidth="1"/>
+    <col min="16054" max="16057" width="10.83203125" customWidth="1"/>
+    <col min="16062" max="16062" width="10.83203125" customWidth="1"/>
+    <col min="16064" max="16065" width="10.83203125" customWidth="1"/>
+    <col min="16067" max="16067" width="10.83203125" customWidth="1"/>
+    <col min="16074" max="16076" width="10.83203125" customWidth="1"/>
+    <col min="16079" max="16079" width="10.83203125" customWidth="1"/>
+    <col min="16096" max="16112" width="10.83203125" customWidth="1"/>
+    <col min="16114" max="16114" width="10.83203125" customWidth="1"/>
+    <col min="16118" max="16118" width="10.83203125" customWidth="1"/>
+    <col min="16120" max="16120" width="10.83203125" customWidth="1"/>
+    <col min="16122" max="16176" width="10.83203125" customWidth="1"/>
+    <col min="16178" max="16178" width="10.83203125" customWidth="1"/>
+    <col min="16182" max="16182" width="10.83203125" customWidth="1"/>
+    <col min="16184" max="16184" width="10.83203125" customWidth="1"/>
+    <col min="16186" max="16245" width="10.83203125" customWidth="1"/>
+    <col min="16247" max="16248" width="10.83203125" customWidth="1"/>
+    <col min="16250" max="16251" width="10.83203125" customWidth="1"/>
+    <col min="16253" max="16254" width="10.83203125" customWidth="1"/>
+    <col min="16258" max="16260" width="10.83203125" customWidth="1"/>
+    <col min="16262" max="16264" width="10.83203125" customWidth="1"/>
+    <col min="16266" max="16268" width="10.83203125" customWidth="1"/>
+    <col min="16270" max="16270" width="10.83203125" customWidth="1"/>
+    <col min="16272" max="16272" width="10.83203125" customWidth="1"/>
+    <col min="16288" max="16304" width="10.83203125" customWidth="1"/>
+    <col min="16306" max="16307" width="10.83203125" customWidth="1"/>
+    <col min="16310" max="16312" width="10.83203125" customWidth="1"/>
+    <col min="16314" max="16315" width="10.83203125" customWidth="1"/>
+    <col min="16318" max="16318" width="10.83203125" customWidth="1"/>
+    <col min="16320" max="16320" width="10.83203125" customWidth="1"/>
+    <col min="16323" max="16323" width="10.83203125" customWidth="1"/>
+    <col min="16325" max="16329" width="10.83203125" customWidth="1"/>
+    <col min="16331" max="16332" width="10.83203125" customWidth="1"/>
+    <col min="16335" max="16335" width="10.83203125" customWidth="1"/>
+    <col min="16352" max="16368" width="10.83203125" customWidth="1"/>
+    <col min="16372" max="16374" width="10.83203125" customWidth="1"/>
+    <col min="16376" max="16376" width="10.83203125" customWidth="1"/>
+    <col min="16379" max="16384" width="10.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M11"/>
   <sheetViews>
@@ -2244,1439 +3682,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="12.6640625" customWidth="1"/>
-    <col min="257" max="260" width="10.83203125" customWidth="1"/>
-    <col min="262" max="263" width="10.83203125" customWidth="1"/>
-    <col min="265" max="298" width="10.83203125" customWidth="1"/>
-    <col min="300" max="301" width="10.83203125" customWidth="1"/>
-    <col min="304" max="304" width="10.83203125" customWidth="1"/>
-    <col min="306" max="308" width="10.83203125" customWidth="1"/>
-    <col min="310" max="340" width="10.83203125" customWidth="1"/>
-    <col min="342" max="343" width="10.83203125" customWidth="1"/>
-    <col min="345" max="356" width="10.83203125" customWidth="1"/>
-    <col min="358" max="359" width="10.83203125" customWidth="1"/>
-    <col min="362" max="364" width="10.83203125" customWidth="1"/>
-    <col min="368" max="369" width="10.83203125" customWidth="1"/>
-    <col min="371" max="371" width="10.83203125" customWidth="1"/>
-    <col min="375" max="385" width="10.83203125" customWidth="1"/>
-    <col min="388" max="390" width="10.83203125" customWidth="1"/>
-    <col min="392" max="400" width="10.83203125" customWidth="1"/>
-    <col min="402" max="402" width="10.83203125" customWidth="1"/>
-    <col min="404" max="405" width="10.83203125" customWidth="1"/>
-    <col min="407" max="407" width="10.83203125" customWidth="1"/>
-    <col min="409" max="431" width="10.83203125" customWidth="1"/>
-    <col min="433" max="439" width="10.83203125" customWidth="1"/>
-    <col min="441" max="454" width="10.83203125" customWidth="1"/>
-    <col min="457" max="462" width="10.83203125" customWidth="1"/>
-    <col min="465" max="470" width="10.83203125" customWidth="1"/>
-    <col min="473" max="487" width="10.83203125" customWidth="1"/>
-    <col min="489" max="495" width="10.83203125" customWidth="1"/>
-    <col min="497" max="503" width="10.83203125" customWidth="1"/>
-    <col min="505" max="512" width="10.83203125" customWidth="1"/>
-    <col min="515" max="517" width="10.83203125" customWidth="1"/>
-    <col min="520" max="521" width="10.83203125" customWidth="1"/>
-    <col min="523" max="523" width="10.83203125" customWidth="1"/>
-    <col min="525" max="525" width="10.83203125" customWidth="1"/>
-    <col min="527" max="527" width="10.83203125" customWidth="1"/>
-    <col min="529" max="529" width="10.83203125" customWidth="1"/>
-    <col min="537" max="544" width="10.83203125" customWidth="1"/>
-    <col min="546" max="546" width="10.83203125" customWidth="1"/>
-    <col min="550" max="550" width="10.83203125" customWidth="1"/>
-    <col min="554" max="554" width="10.83203125" customWidth="1"/>
-    <col min="557" max="557" width="10.83203125" customWidth="1"/>
-    <col min="559" max="561" width="10.83203125" customWidth="1"/>
-    <col min="563" max="564" width="10.83203125" customWidth="1"/>
-    <col min="567" max="576" width="10.83203125" customWidth="1"/>
-    <col min="586" max="586" width="10.83203125" customWidth="1"/>
-    <col min="588" max="588" width="10.83203125" customWidth="1"/>
-    <col min="593" max="594" width="10.83203125" customWidth="1"/>
-    <col min="597" max="599" width="10.83203125" customWidth="1"/>
-    <col min="601" max="609" width="10.83203125" customWidth="1"/>
-    <col min="613" max="614" width="10.83203125" customWidth="1"/>
-    <col min="616" max="617" width="10.83203125" customWidth="1"/>
-    <col min="619" max="621" width="10.83203125" customWidth="1"/>
-    <col min="628" max="628" width="10.83203125" customWidth="1"/>
-    <col min="630" max="630" width="10.83203125" customWidth="1"/>
-    <col min="632" max="640" width="10.83203125" customWidth="1"/>
-    <col min="644" max="645" width="10.83203125" customWidth="1"/>
-    <col min="648" max="648" width="10.83203125" customWidth="1"/>
-    <col min="650" max="652" width="10.83203125" customWidth="1"/>
-    <col min="654" max="656" width="10.83203125" customWidth="1"/>
-    <col min="665" max="673" width="10.83203125" customWidth="1"/>
-    <col min="684" max="685" width="10.83203125" customWidth="1"/>
-    <col min="687" max="687" width="10.83203125" customWidth="1"/>
-    <col min="689" max="689" width="10.83203125" customWidth="1"/>
-    <col min="692" max="694" width="10.83203125" customWidth="1"/>
-    <col min="696" max="705" width="10.83203125" customWidth="1"/>
-    <col min="708" max="711" width="10.83203125" customWidth="1"/>
-    <col min="715" max="716" width="10.83203125" customWidth="1"/>
-    <col min="718" max="718" width="10.83203125" customWidth="1"/>
-    <col min="720" max="720" width="10.83203125" customWidth="1"/>
-    <col min="724" max="724" width="10.83203125" customWidth="1"/>
-    <col min="726" max="726" width="10.83203125" customWidth="1"/>
-    <col min="728" max="737" width="10.83203125" customWidth="1"/>
-    <col min="739" max="741" width="10.83203125" customWidth="1"/>
-    <col min="743" max="743" width="10.83203125" customWidth="1"/>
-    <col min="746" max="746" width="10.83203125" customWidth="1"/>
-    <col min="751" max="751" width="10.83203125" customWidth="1"/>
-    <col min="753" max="756" width="10.83203125" customWidth="1"/>
-    <col min="758" max="759" width="10.83203125" customWidth="1"/>
-    <col min="761" max="768" width="10.83203125" customWidth="1"/>
-    <col min="771" max="773" width="10.83203125" customWidth="1"/>
-    <col min="776" max="777" width="10.83203125" customWidth="1"/>
-    <col min="779" max="779" width="10.83203125" customWidth="1"/>
-    <col min="781" max="781" width="10.83203125" customWidth="1"/>
-    <col min="783" max="783" width="10.83203125" customWidth="1"/>
-    <col min="785" max="785" width="10.83203125" customWidth="1"/>
-    <col min="793" max="800" width="10.83203125" customWidth="1"/>
-    <col min="802" max="802" width="10.83203125" customWidth="1"/>
-    <col min="806" max="806" width="10.83203125" customWidth="1"/>
-    <col min="810" max="810" width="10.83203125" customWidth="1"/>
-    <col min="813" max="813" width="10.83203125" customWidth="1"/>
-    <col min="815" max="817" width="10.83203125" customWidth="1"/>
-    <col min="819" max="820" width="10.83203125" customWidth="1"/>
-    <col min="823" max="832" width="10.83203125" customWidth="1"/>
-    <col min="842" max="842" width="10.83203125" customWidth="1"/>
-    <col min="844" max="844" width="10.83203125" customWidth="1"/>
-    <col min="849" max="850" width="10.83203125" customWidth="1"/>
-    <col min="853" max="855" width="10.83203125" customWidth="1"/>
-    <col min="857" max="865" width="10.83203125" customWidth="1"/>
-    <col min="869" max="870" width="10.83203125" customWidth="1"/>
-    <col min="872" max="873" width="10.83203125" customWidth="1"/>
-    <col min="875" max="877" width="10.83203125" customWidth="1"/>
-    <col min="884" max="884" width="10.83203125" customWidth="1"/>
-    <col min="886" max="886" width="10.83203125" customWidth="1"/>
-    <col min="888" max="896" width="10.83203125" customWidth="1"/>
-    <col min="900" max="901" width="10.83203125" customWidth="1"/>
-    <col min="904" max="904" width="10.83203125" customWidth="1"/>
-    <col min="906" max="908" width="10.83203125" customWidth="1"/>
-    <col min="910" max="912" width="10.83203125" customWidth="1"/>
-    <col min="921" max="929" width="10.83203125" customWidth="1"/>
-    <col min="940" max="941" width="10.83203125" customWidth="1"/>
-    <col min="943" max="943" width="10.83203125" customWidth="1"/>
-    <col min="945" max="945" width="10.83203125" customWidth="1"/>
-    <col min="948" max="950" width="10.83203125" customWidth="1"/>
-    <col min="952" max="961" width="10.83203125" customWidth="1"/>
-    <col min="964" max="967" width="10.83203125" customWidth="1"/>
-    <col min="971" max="972" width="10.83203125" customWidth="1"/>
-    <col min="974" max="974" width="10.83203125" customWidth="1"/>
-    <col min="976" max="976" width="10.83203125" customWidth="1"/>
-    <col min="980" max="980" width="10.83203125" customWidth="1"/>
-    <col min="982" max="982" width="10.83203125" customWidth="1"/>
-    <col min="984" max="993" width="10.83203125" customWidth="1"/>
-    <col min="995" max="997" width="10.83203125" customWidth="1"/>
-    <col min="999" max="999" width="10.83203125" customWidth="1"/>
-    <col min="1002" max="1002" width="10.83203125" customWidth="1"/>
-    <col min="1007" max="1007" width="10.83203125" customWidth="1"/>
-    <col min="1009" max="1012" width="10.83203125" customWidth="1"/>
-    <col min="1014" max="1015" width="10.83203125" customWidth="1"/>
-    <col min="1017" max="1034" width="10.83203125" customWidth="1"/>
-    <col min="1037" max="1038" width="10.83203125" customWidth="1"/>
-    <col min="1049" max="1058" width="10.83203125" customWidth="1"/>
-    <col min="1061" max="1062" width="10.83203125" customWidth="1"/>
-    <col min="1081" max="1090" width="10.83203125" customWidth="1"/>
-    <col min="1093" max="1094" width="10.83203125" customWidth="1"/>
-    <col min="1105" max="1106" width="10.83203125" customWidth="1"/>
-    <col min="1109" max="1110" width="10.83203125" customWidth="1"/>
-    <col min="1113" max="1120" width="10.83203125" customWidth="1"/>
-    <col min="1138" max="1139" width="10.83203125" customWidth="1"/>
-    <col min="1142" max="1143" width="10.83203125" customWidth="1"/>
-    <col min="1145" max="1152" width="10.83203125" customWidth="1"/>
-    <col min="1154" max="1155" width="10.83203125" customWidth="1"/>
-    <col min="1158" max="1159" width="10.83203125" customWidth="1"/>
-    <col min="1161" max="1162" width="10.83203125" customWidth="1"/>
-    <col min="1165" max="1166" width="10.83203125" customWidth="1"/>
-    <col min="1177" max="1184" width="10.83203125" customWidth="1"/>
-    <col min="1194" max="1195" width="10.83203125" customWidth="1"/>
-    <col min="1198" max="1199" width="10.83203125" customWidth="1"/>
-    <col min="1201" max="1202" width="10.83203125" customWidth="1"/>
-    <col min="1205" max="1206" width="10.83203125" customWidth="1"/>
-    <col min="1209" max="1218" width="10.83203125" customWidth="1"/>
-    <col min="1221" max="1222" width="10.83203125" customWidth="1"/>
-    <col min="1226" max="1227" width="10.83203125" customWidth="1"/>
-    <col min="1230" max="1231" width="10.83203125" customWidth="1"/>
-    <col min="1241" max="1248" width="10.83203125" customWidth="1"/>
-    <col min="1251" max="1253" width="10.83203125" customWidth="1"/>
-    <col min="1259" max="1261" width="10.83203125" customWidth="1"/>
-    <col min="1267" max="1269" width="10.83203125" customWidth="1"/>
-    <col min="1273" max="1280" width="10.83203125" customWidth="1"/>
-    <col min="1283" max="1284" width="10.83203125" customWidth="1"/>
-    <col min="1287" max="1289" width="10.83203125" customWidth="1"/>
-    <col min="1292" max="1293" width="10.83203125" customWidth="1"/>
-    <col min="1296" max="1296" width="10.83203125" customWidth="1"/>
-    <col min="1305" max="1312" width="10.83203125" customWidth="1"/>
-    <col min="1315" max="1316" width="10.83203125" customWidth="1"/>
-    <col min="1319" max="1322" width="10.83203125" customWidth="1"/>
-    <col min="1325" max="1326" width="10.83203125" customWidth="1"/>
-    <col min="1329" max="1330" width="10.83203125" customWidth="1"/>
-    <col min="1333" max="1334" width="10.83203125" customWidth="1"/>
-    <col min="1337" max="1344" width="10.83203125" customWidth="1"/>
-    <col min="1346" max="1347" width="10.83203125" customWidth="1"/>
-    <col min="1350" max="1351" width="10.83203125" customWidth="1"/>
-    <col min="1353" max="1354" width="10.83203125" customWidth="1"/>
-    <col min="1357" max="1358" width="10.83203125" customWidth="1"/>
-    <col min="1361" max="1376" width="10.83203125" customWidth="1"/>
-    <col min="1385" max="1386" width="10.83203125" customWidth="1"/>
-    <col min="1389" max="1390" width="10.83203125" customWidth="1"/>
-    <col min="1393" max="1408" width="10.83203125" customWidth="1"/>
-    <col min="1418" max="1419" width="10.83203125" customWidth="1"/>
-    <col min="1422" max="1423" width="10.83203125" customWidth="1"/>
-    <col min="1425" max="1440" width="10.83203125" customWidth="1"/>
-    <col min="1449" max="1449" width="10.83203125" customWidth="1"/>
-    <col min="1452" max="1453" width="10.83203125" customWidth="1"/>
-    <col min="1456" max="1473" width="10.83203125" customWidth="1"/>
-    <col min="1476" max="1477" width="10.83203125" customWidth="1"/>
-    <col min="1480" max="1481" width="10.83203125" customWidth="1"/>
-    <col min="1484" max="1485" width="10.83203125" customWidth="1"/>
-    <col min="1488" max="1488" width="10.83203125" customWidth="1"/>
-    <col min="1490" max="1491" width="10.83203125" customWidth="1"/>
-    <col min="1494" max="1495" width="10.83203125" customWidth="1"/>
-    <col min="1497" max="1505" width="10.83203125" customWidth="1"/>
-    <col min="1508" max="1508" width="10.83203125" customWidth="1"/>
-    <col min="1510" max="1511" width="10.83203125" customWidth="1"/>
-    <col min="1513" max="1513" width="10.83203125" customWidth="1"/>
-    <col min="1516" max="1516" width="10.83203125" customWidth="1"/>
-    <col min="1518" max="1519" width="10.83203125" customWidth="1"/>
-    <col min="1521" max="1521" width="10.83203125" customWidth="1"/>
-    <col min="1524" max="1524" width="10.83203125" customWidth="1"/>
-    <col min="1526" max="1527" width="10.83203125" customWidth="1"/>
-    <col min="1529" max="1544" width="10.83203125" customWidth="1"/>
-    <col min="1547" max="1548" width="10.83203125" customWidth="1"/>
-    <col min="1551" max="1553" width="10.83203125" customWidth="1"/>
-    <col min="1556" max="1557" width="10.83203125" customWidth="1"/>
-    <col min="1560" max="1568" width="10.83203125" customWidth="1"/>
-    <col min="1571" max="1572" width="10.83203125" customWidth="1"/>
-    <col min="1575" max="1576" width="10.83203125" customWidth="1"/>
-    <col min="1578" max="1579" width="10.83203125" customWidth="1"/>
-    <col min="1582" max="1583" width="10.83203125" customWidth="1"/>
-    <col min="1585" max="1585" width="10.83203125" customWidth="1"/>
-    <col min="1588" max="1589" width="10.83203125" customWidth="1"/>
-    <col min="1592" max="1608" width="10.83203125" customWidth="1"/>
-    <col min="1611" max="1612" width="10.83203125" customWidth="1"/>
-    <col min="1615" max="1632" width="10.83203125" customWidth="1"/>
-    <col min="1635" max="1636" width="10.83203125" customWidth="1"/>
-    <col min="1639" max="1640" width="10.83203125" customWidth="1"/>
-    <col min="1643" max="1644" width="10.83203125" customWidth="1"/>
-    <col min="1647" max="1664" width="10.83203125" customWidth="1"/>
-    <col min="1666" max="1667" width="10.83203125" customWidth="1"/>
-    <col min="1670" max="1671" width="10.83203125" customWidth="1"/>
-    <col min="1675" max="1676" width="10.83203125" customWidth="1"/>
-    <col min="1679" max="1696" width="10.83203125" customWidth="1"/>
-    <col min="1698" max="1699" width="10.83203125" customWidth="1"/>
-    <col min="1702" max="1703" width="10.83203125" customWidth="1"/>
-    <col min="1707" max="1708" width="10.83203125" customWidth="1"/>
-    <col min="1711" max="1713" width="10.83203125" customWidth="1"/>
-    <col min="1716" max="1717" width="10.83203125" customWidth="1"/>
-    <col min="1720" max="1728" width="10.83203125" customWidth="1"/>
-    <col min="1731" max="1732" width="10.83203125" customWidth="1"/>
-    <col min="1735" max="1736" width="10.83203125" customWidth="1"/>
-    <col min="1739" max="1740" width="10.83203125" customWidth="1"/>
-    <col min="1743" max="1744" width="10.83203125" customWidth="1"/>
-    <col min="1746" max="1747" width="10.83203125" customWidth="1"/>
-    <col min="1750" max="1751" width="10.83203125" customWidth="1"/>
-    <col min="1753" max="1760" width="10.83203125" customWidth="1"/>
-    <col min="1763" max="1764" width="10.83203125" customWidth="1"/>
-    <col min="1767" max="1768" width="10.83203125" customWidth="1"/>
-    <col min="1771" max="1772" width="10.83203125" customWidth="1"/>
-    <col min="1775" max="1776" width="10.83203125" customWidth="1"/>
-    <col min="1779" max="1780" width="10.83203125" customWidth="1"/>
-    <col min="1783" max="1793" width="10.83203125" customWidth="1"/>
-    <col min="1802" max="1804" width="10.83203125" customWidth="1"/>
-    <col min="1807" max="1807" width="10.83203125" customWidth="1"/>
-    <col min="1824" max="1905" width="10.83203125" customWidth="1"/>
-    <col min="1907" max="1908" width="10.83203125" customWidth="1"/>
-    <col min="1910" max="1910" width="10.83203125" customWidth="1"/>
-    <col min="1912" max="1912" width="10.83203125" customWidth="1"/>
-    <col min="1914" max="1914" width="10.83203125" customWidth="1"/>
-    <col min="1917" max="1918" width="10.83203125" customWidth="1"/>
-    <col min="1922" max="1924" width="10.83203125" customWidth="1"/>
-    <col min="1926" max="1928" width="10.83203125" customWidth="1"/>
-    <col min="1930" max="1932" width="10.83203125" customWidth="1"/>
-    <col min="1934" max="1934" width="10.83203125" customWidth="1"/>
-    <col min="1936" max="1936" width="10.83203125" customWidth="1"/>
-    <col min="1952" max="1968" width="10.83203125" customWidth="1"/>
-    <col min="1971" max="2038" width="10.83203125" customWidth="1"/>
-    <col min="2040" max="2040" width="10.83203125" customWidth="1"/>
-    <col min="2042" max="2042" width="10.83203125" customWidth="1"/>
-    <col min="2044" max="2046" width="10.83203125" customWidth="1"/>
-    <col min="2050" max="2052" width="10.83203125" customWidth="1"/>
-    <col min="2054" max="2056" width="10.83203125" customWidth="1"/>
-    <col min="2058" max="2060" width="10.83203125" customWidth="1"/>
-    <col min="2062" max="2062" width="10.83203125" customWidth="1"/>
-    <col min="2064" max="2064" width="10.83203125" customWidth="1"/>
-    <col min="2080" max="2096" width="10.83203125" customWidth="1"/>
-    <col min="2099" max="2099" width="10.83203125" customWidth="1"/>
-    <col min="2101" max="2103" width="10.83203125" customWidth="1"/>
-    <col min="2106" max="2107" width="10.83203125" customWidth="1"/>
-    <col min="2111" max="2111" width="10.83203125" customWidth="1"/>
-    <col min="2113" max="2113" width="10.83203125" customWidth="1"/>
-    <col min="2115" max="2115" width="10.83203125" customWidth="1"/>
-    <col min="2122" max="2124" width="10.83203125" customWidth="1"/>
-    <col min="2127" max="2127" width="10.83203125" customWidth="1"/>
-    <col min="2144" max="2161" width="10.83203125" customWidth="1"/>
-    <col min="2163" max="2164" width="10.83203125" customWidth="1"/>
-    <col min="2168" max="2168" width="10.83203125" customWidth="1"/>
-    <col min="2170" max="2170" width="10.83203125" customWidth="1"/>
-    <col min="2173" max="2174" width="10.83203125" customWidth="1"/>
-    <col min="2178" max="2180" width="10.83203125" customWidth="1"/>
-    <col min="2182" max="2184" width="10.83203125" customWidth="1"/>
-    <col min="2186" max="2188" width="10.83203125" customWidth="1"/>
-    <col min="2190" max="2190" width="10.83203125" customWidth="1"/>
-    <col min="2192" max="2192" width="10.83203125" customWidth="1"/>
-    <col min="2208" max="2224" width="10.83203125" customWidth="1"/>
-    <col min="2227" max="2293" width="10.83203125" customWidth="1"/>
-    <col min="2296" max="2296" width="10.83203125" customWidth="1"/>
-    <col min="2298" max="2298" width="10.83203125" customWidth="1"/>
-    <col min="2300" max="2302" width="10.83203125" customWidth="1"/>
-    <col min="2306" max="2308" width="10.83203125" customWidth="1"/>
-    <col min="2310" max="2312" width="10.83203125" customWidth="1"/>
-    <col min="2314" max="2316" width="10.83203125" customWidth="1"/>
-    <col min="2318" max="2318" width="10.83203125" customWidth="1"/>
-    <col min="2320" max="2320" width="10.83203125" customWidth="1"/>
-    <col min="2336" max="2359" width="10.83203125" customWidth="1"/>
-    <col min="2361" max="2492" width="10.83203125" customWidth="1"/>
-    <col min="2494" max="2535" width="10.83203125" customWidth="1"/>
-    <col min="2561" max="2564" width="10.83203125" customWidth="1"/>
-    <col min="2566" max="2566" width="10.83203125" customWidth="1"/>
-    <col min="2568" max="2569" width="10.83203125" customWidth="1"/>
-    <col min="2574" max="2575" width="10.83203125" customWidth="1"/>
-    <col min="2592" max="2615" width="10.83203125" customWidth="1"/>
-    <col min="2617" max="2672" width="10.83203125" customWidth="1"/>
-    <col min="2674" max="2674" width="10.83203125" customWidth="1"/>
-    <col min="2676" max="2814" width="10.83203125" customWidth="1"/>
-    <col min="2819" max="2822" width="10.83203125" customWidth="1"/>
-    <col min="2824" max="2827" width="10.83203125" customWidth="1"/>
-    <col min="2830" max="2832" width="10.83203125" customWidth="1"/>
-    <col min="2834" max="2871" width="10.83203125" customWidth="1"/>
-    <col min="2873" max="2933" width="10.83203125" customWidth="1"/>
-    <col min="2938" max="2942" width="10.83203125" customWidth="1"/>
-    <col min="2946" max="2948" width="10.83203125" customWidth="1"/>
-    <col min="2950" max="2952" width="10.83203125" customWidth="1"/>
-    <col min="2954" max="2956" width="10.83203125" customWidth="1"/>
-    <col min="2958" max="2958" width="10.83203125" customWidth="1"/>
-    <col min="2960" max="2960" width="10.83203125" customWidth="1"/>
-    <col min="2976" max="2992" width="10.83203125" customWidth="1"/>
-    <col min="2999" max="2999" width="10.83203125" customWidth="1"/>
-    <col min="3003" max="3004" width="10.83203125" customWidth="1"/>
-    <col min="3006" max="3006" width="10.83203125" customWidth="1"/>
-    <col min="3008" max="3008" width="10.83203125" customWidth="1"/>
-    <col min="3011" max="3011" width="10.83203125" customWidth="1"/>
-    <col min="3013" max="3017" width="10.83203125" customWidth="1"/>
-    <col min="3019" max="3020" width="10.83203125" customWidth="1"/>
-    <col min="3023" max="3023" width="10.83203125" customWidth="1"/>
-    <col min="3040" max="3134" width="10.83203125" customWidth="1"/>
-    <col min="3139" max="3141" width="10.83203125" customWidth="1"/>
-    <col min="3145" max="3145" width="10.83203125" customWidth="1"/>
-    <col min="3147" max="3147" width="10.83203125" customWidth="1"/>
-    <col min="3151" max="3151" width="10.83203125" customWidth="1"/>
-    <col min="3168" max="3188" width="10.83203125" customWidth="1"/>
-    <col min="3190" max="3193" width="10.83203125" customWidth="1"/>
-    <col min="3195" max="3198" width="10.83203125" customWidth="1"/>
-    <col min="3202" max="3204" width="10.83203125" customWidth="1"/>
-    <col min="3206" max="3208" width="10.83203125" customWidth="1"/>
-    <col min="3210" max="3212" width="10.83203125" customWidth="1"/>
-    <col min="3214" max="3214" width="10.83203125" customWidth="1"/>
-    <col min="3216" max="3216" width="10.83203125" customWidth="1"/>
-    <col min="3232" max="3249" width="10.83203125" customWidth="1"/>
-    <col min="3251" max="3255" width="10.83203125" customWidth="1"/>
-    <col min="3257" max="3257" width="10.83203125" customWidth="1"/>
-    <col min="3259" max="3261" width="10.83203125" customWidth="1"/>
-    <col min="3265" max="3265" width="10.83203125" customWidth="1"/>
-    <col min="3267" max="3267" width="10.83203125" customWidth="1"/>
-    <col min="3269" max="3273" width="10.83203125" customWidth="1"/>
-    <col min="3275" max="3276" width="10.83203125" customWidth="1"/>
-    <col min="3279" max="3279" width="10.83203125" customWidth="1"/>
-    <col min="3296" max="3319" width="10.83203125" customWidth="1"/>
-    <col min="3321" max="3383" width="10.83203125" customWidth="1"/>
-    <col min="3385" max="3440" width="10.83203125" customWidth="1"/>
-    <col min="3443" max="3509" width="10.83203125" customWidth="1"/>
-    <col min="3511" max="3511" width="10.83203125" customWidth="1"/>
-    <col min="3513" max="3514" width="10.83203125" customWidth="1"/>
-    <col min="3516" max="3518" width="10.83203125" customWidth="1"/>
-    <col min="3522" max="3524" width="10.83203125" customWidth="1"/>
-    <col min="3526" max="3528" width="10.83203125" customWidth="1"/>
-    <col min="3530" max="3532" width="10.83203125" customWidth="1"/>
-    <col min="3534" max="3534" width="10.83203125" customWidth="1"/>
-    <col min="3536" max="3536" width="10.83203125" customWidth="1"/>
-    <col min="3552" max="3572" width="10.83203125" customWidth="1"/>
-    <col min="3576" max="3578" width="10.83203125" customWidth="1"/>
-    <col min="3580" max="3582" width="10.83203125" customWidth="1"/>
-    <col min="3586" max="3588" width="10.83203125" customWidth="1"/>
-    <col min="3590" max="3592" width="10.83203125" customWidth="1"/>
-    <col min="3594" max="3596" width="10.83203125" customWidth="1"/>
-    <col min="3598" max="3598" width="10.83203125" customWidth="1"/>
-    <col min="3600" max="3600" width="10.83203125" customWidth="1"/>
-    <col min="3616" max="3639" width="10.83203125" customWidth="1"/>
-    <col min="3642" max="3643" width="10.83203125" customWidth="1"/>
-    <col min="3647" max="3650" width="10.83203125" customWidth="1"/>
-    <col min="3652" max="3652" width="10.83203125" customWidth="1"/>
-    <col min="3656" max="3658" width="10.83203125" customWidth="1"/>
-    <col min="3662" max="3663" width="10.83203125" customWidth="1"/>
-    <col min="3680" max="3696" width="10.83203125" customWidth="1"/>
-    <col min="3699" max="3728" width="10.83203125" customWidth="1"/>
-    <col min="3730" max="3763" width="10.83203125" customWidth="1"/>
-    <col min="3765" max="3766" width="10.83203125" customWidth="1"/>
-    <col min="3768" max="3769" width="10.83203125" customWidth="1"/>
-    <col min="3772" max="3774" width="10.83203125" customWidth="1"/>
-    <col min="3778" max="3780" width="10.83203125" customWidth="1"/>
-    <col min="3782" max="3784" width="10.83203125" customWidth="1"/>
-    <col min="3786" max="3788" width="10.83203125" customWidth="1"/>
-    <col min="3790" max="3790" width="10.83203125" customWidth="1"/>
-    <col min="3792" max="3792" width="10.83203125" customWidth="1"/>
-    <col min="3808" max="3888" width="10.83203125" customWidth="1"/>
-    <col min="3936" max="4019" width="10.83203125" customWidth="1"/>
-    <col min="4021" max="4021" width="10.83203125" customWidth="1"/>
-    <col min="4024" max="4025" width="10.83203125" customWidth="1"/>
-    <col min="4028" max="4030" width="10.83203125" customWidth="1"/>
-    <col min="4034" max="4036" width="10.83203125" customWidth="1"/>
-    <col min="4038" max="4040" width="10.83203125" customWidth="1"/>
-    <col min="4042" max="4044" width="10.83203125" customWidth="1"/>
-    <col min="4046" max="4046" width="10.83203125" customWidth="1"/>
-    <col min="4048" max="4049" width="10.83203125" customWidth="1"/>
-    <col min="4051" max="4080" width="10.83203125" customWidth="1"/>
-    <col min="4083" max="4148" width="10.83203125" customWidth="1"/>
-    <col min="4150" max="4150" width="10.83203125" customWidth="1"/>
-    <col min="4152" max="4152" width="10.83203125" customWidth="1"/>
-    <col min="4154" max="4154" width="10.83203125" customWidth="1"/>
-    <col min="4157" max="4158" width="10.83203125" customWidth="1"/>
-    <col min="4162" max="4164" width="10.83203125" customWidth="1"/>
-    <col min="4166" max="4168" width="10.83203125" customWidth="1"/>
-    <col min="4170" max="4172" width="10.83203125" customWidth="1"/>
-    <col min="4174" max="4174" width="10.83203125" customWidth="1"/>
-    <col min="4176" max="4176" width="10.83203125" customWidth="1"/>
-    <col min="4192" max="4208" width="10.83203125" customWidth="1"/>
-    <col min="4210" max="4210" width="10.83203125" customWidth="1"/>
-    <col min="4216" max="4218" width="10.83203125" customWidth="1"/>
-    <col min="4220" max="4222" width="10.83203125" customWidth="1"/>
-    <col min="4226" max="4228" width="10.83203125" customWidth="1"/>
-    <col min="4230" max="4232" width="10.83203125" customWidth="1"/>
-    <col min="4234" max="4236" width="10.83203125" customWidth="1"/>
-    <col min="4238" max="4238" width="10.83203125" customWidth="1"/>
-    <col min="4240" max="4240" width="10.83203125" customWidth="1"/>
-    <col min="4256" max="4305" width="10.83203125" customWidth="1"/>
-    <col min="4307" max="4343" width="10.83203125" customWidth="1"/>
-    <col min="4345" max="4345" width="10.83203125" customWidth="1"/>
-    <col min="4347" max="4348" width="10.83203125" customWidth="1"/>
-    <col min="4357" max="4360" width="10.83203125" customWidth="1"/>
-    <col min="4362" max="4381" width="10.83203125" customWidth="1"/>
-    <col min="4384" max="4404" width="10.83203125" customWidth="1"/>
-    <col min="4408" max="4408" width="10.83203125" customWidth="1"/>
-    <col min="4410" max="4410" width="10.83203125" customWidth="1"/>
-    <col min="4413" max="4414" width="10.83203125" customWidth="1"/>
-    <col min="4418" max="4420" width="10.83203125" customWidth="1"/>
-    <col min="4422" max="4424" width="10.83203125" customWidth="1"/>
-    <col min="4426" max="4428" width="10.83203125" customWidth="1"/>
-    <col min="4430" max="4430" width="10.83203125" customWidth="1"/>
-    <col min="4432" max="4432" width="10.83203125" customWidth="1"/>
-    <col min="4448" max="4468" width="10.83203125" customWidth="1"/>
-    <col min="4473" max="4476" width="10.83203125" customWidth="1"/>
-    <col min="4478" max="4479" width="10.83203125" customWidth="1"/>
-    <col min="4481" max="4481" width="10.83203125" customWidth="1"/>
-    <col min="4483" max="4485" width="10.83203125" customWidth="1"/>
-    <col min="4489" max="4489" width="10.83203125" customWidth="1"/>
-    <col min="4491" max="4491" width="10.83203125" customWidth="1"/>
-    <col min="4495" max="4495" width="10.83203125" customWidth="1"/>
-    <col min="4512" max="4532" width="10.83203125" customWidth="1"/>
-    <col min="4534" max="4534" width="10.83203125" customWidth="1"/>
-    <col min="4537" max="4537" width="10.83203125" customWidth="1"/>
-    <col min="4541" max="4542" width="10.83203125" customWidth="1"/>
-    <col min="4544" max="4544" width="10.83203125" customWidth="1"/>
-    <col min="4548" max="4550" width="10.83203125" customWidth="1"/>
-    <col min="4552" max="4553" width="10.83203125" customWidth="1"/>
-    <col min="4555" max="4573" width="10.83203125" customWidth="1"/>
-    <col min="4576" max="4599" width="10.83203125" customWidth="1"/>
-    <col min="4601" max="4601" width="10.83203125" customWidth="1"/>
-    <col min="4603" max="4604" width="10.83203125" customWidth="1"/>
-    <col min="4613" max="4616" width="10.83203125" customWidth="1"/>
-    <col min="4618" max="4624" width="10.83203125" customWidth="1"/>
-    <col min="4627" max="4784" width="10.83203125" customWidth="1"/>
-    <col min="4787" max="4912" width="10.83203125" customWidth="1"/>
-    <col min="4914" max="5046" width="10.83203125" customWidth="1"/>
-    <col min="5049" max="5049" width="10.83203125" customWidth="1"/>
-    <col min="5053" max="5054" width="10.83203125" customWidth="1"/>
-    <col min="5056" max="5056" width="10.83203125" customWidth="1"/>
-    <col min="5060" max="5062" width="10.83203125" customWidth="1"/>
-    <col min="5064" max="5065" width="10.83203125" customWidth="1"/>
-    <col min="5067" max="5085" width="10.83203125" customWidth="1"/>
-    <col min="5088" max="5168" width="10.83203125" customWidth="1"/>
-    <col min="5170" max="5232" width="10.83203125" customWidth="1"/>
-    <col min="5234" max="5302" width="10.83203125" customWidth="1"/>
-    <col min="5305" max="5305" width="10.83203125" customWidth="1"/>
-    <col min="5309" max="5310" width="10.83203125" customWidth="1"/>
-    <col min="5312" max="5312" width="10.83203125" customWidth="1"/>
-    <col min="5316" max="5318" width="10.83203125" customWidth="1"/>
-    <col min="5320" max="5321" width="10.83203125" customWidth="1"/>
-    <col min="5323" max="5341" width="10.83203125" customWidth="1"/>
-    <col min="5344" max="5367" width="10.83203125" customWidth="1"/>
-    <col min="5369" max="5424" width="10.83203125" customWidth="1"/>
-    <col min="5429" max="5429" width="10.83203125" customWidth="1"/>
-    <col min="5431" max="5440" width="10.83203125" customWidth="1"/>
-    <col min="5442" max="5442" width="10.83203125" customWidth="1"/>
-    <col min="5445" max="5446" width="10.83203125" customWidth="1"/>
-    <col min="5448" max="5456" width="10.83203125" customWidth="1"/>
-    <col min="5458" max="5458" width="10.83203125" customWidth="1"/>
-    <col min="5460" max="5461" width="10.83203125" customWidth="1"/>
-    <col min="5464" max="5473" width="10.83203125" customWidth="1"/>
-    <col min="5475" max="5476" width="10.83203125" customWidth="1"/>
-    <col min="5480" max="5488" width="10.83203125" customWidth="1"/>
-    <col min="5490" max="5490" width="10.83203125" customWidth="1"/>
-    <col min="5492" max="5553" width="10.83203125" customWidth="1"/>
-    <col min="5555" max="5558" width="10.83203125" customWidth="1"/>
-    <col min="5560" max="5568" width="10.83203125" customWidth="1"/>
-    <col min="5570" max="5570" width="10.83203125" customWidth="1"/>
-    <col min="5572" max="5572" width="10.83203125" customWidth="1"/>
-    <col min="5576" max="5586" width="10.83203125" customWidth="1"/>
-    <col min="5589" max="5589" width="10.83203125" customWidth="1"/>
-    <col min="5592" max="5600" width="10.83203125" customWidth="1"/>
-    <col min="5603" max="5603" width="10.83203125" customWidth="1"/>
-    <col min="5605" max="5605" width="10.83203125" customWidth="1"/>
-    <col min="5608" max="5623" width="10.83203125" customWidth="1"/>
-    <col min="5625" max="5681" width="10.83203125" customWidth="1"/>
-    <col min="5684" max="5685" width="10.83203125" customWidth="1"/>
-    <col min="5688" max="5696" width="10.83203125" customWidth="1"/>
-    <col min="5698" max="5699" width="10.83203125" customWidth="1"/>
-    <col min="5701" max="5701" width="10.83203125" customWidth="1"/>
-    <col min="5704" max="5712" width="10.83203125" customWidth="1"/>
-    <col min="5716" max="5717" width="10.83203125" customWidth="1"/>
-    <col min="5720" max="5728" width="10.83203125" customWidth="1"/>
-    <col min="5730" max="5730" width="10.83203125" customWidth="1"/>
-    <col min="5732" max="5732" width="10.83203125" customWidth="1"/>
-    <col min="5736" max="5744" width="10.83203125" customWidth="1"/>
-    <col min="5746" max="5746" width="10.83203125" customWidth="1"/>
-    <col min="5748" max="5808" width="10.83203125" customWidth="1"/>
-    <col min="5813" max="5813" width="10.83203125" customWidth="1"/>
-    <col min="5816" max="5825" width="10.83203125" customWidth="1"/>
-    <col min="5829" max="5829" width="10.83203125" customWidth="1"/>
-    <col min="5832" max="5840" width="10.83203125" customWidth="1"/>
-    <col min="5842" max="5842" width="10.83203125" customWidth="1"/>
-    <col min="5845" max="5845" width="10.83203125" customWidth="1"/>
-    <col min="5847" max="5858" width="10.83203125" customWidth="1"/>
-    <col min="5860" max="5860" width="10.83203125" customWidth="1"/>
-    <col min="5862" max="5862" width="10.83203125" customWidth="1"/>
-    <col min="5864" max="5872" width="10.83203125" customWidth="1"/>
-    <col min="5877" max="5877" width="10.83203125" customWidth="1"/>
-    <col min="5880" max="5888" width="10.83203125" customWidth="1"/>
-    <col min="5893" max="5893" width="10.83203125" customWidth="1"/>
-    <col min="5896" max="5906" width="10.83203125" customWidth="1"/>
-    <col min="5909" max="5909" width="10.83203125" customWidth="1"/>
-    <col min="5912" max="5920" width="10.83203125" customWidth="1"/>
-    <col min="5922" max="5922" width="10.83203125" customWidth="1"/>
-    <col min="5925" max="5925" width="10.83203125" customWidth="1"/>
-    <col min="5927" max="5936" width="10.83203125" customWidth="1"/>
-    <col min="5938" max="5938" width="10.83203125" customWidth="1"/>
-    <col min="5941" max="5941" width="10.83203125" customWidth="1"/>
-    <col min="5944" max="5952" width="10.83203125" customWidth="1"/>
-    <col min="5954" max="5957" width="10.83203125" customWidth="1"/>
-    <col min="5960" max="5968" width="10.83203125" customWidth="1"/>
-    <col min="5971" max="5972" width="10.83203125" customWidth="1"/>
-    <col min="5976" max="5986" width="10.83203125" customWidth="1"/>
-    <col min="5988" max="5988" width="10.83203125" customWidth="1"/>
-    <col min="5992" max="6000" width="10.83203125" customWidth="1"/>
-    <col min="6002" max="6002" width="10.83203125" customWidth="1"/>
-    <col min="6004" max="6005" width="10.83203125" customWidth="1"/>
-    <col min="6008" max="6017" width="10.83203125" customWidth="1"/>
-    <col min="6019" max="6020" width="10.83203125" customWidth="1"/>
-    <col min="6024" max="6032" width="10.83203125" customWidth="1"/>
-    <col min="6037" max="6037" width="10.83203125" customWidth="1"/>
-    <col min="6039" max="6050" width="10.83203125" customWidth="1"/>
-    <col min="6052" max="6052" width="10.83203125" customWidth="1"/>
-    <col min="6056" max="6064" width="10.83203125" customWidth="1"/>
-    <col min="6066" max="6066" width="10.83203125" customWidth="1"/>
-    <col min="6068" max="6069" width="10.83203125" customWidth="1"/>
-    <col min="6072" max="6080" width="10.83203125" customWidth="1"/>
-    <col min="6082" max="6082" width="10.83203125" customWidth="1"/>
-    <col min="6085" max="6085" width="10.83203125" customWidth="1"/>
-    <col min="6088" max="6100" width="10.83203125" customWidth="1"/>
-    <col min="6104" max="6114" width="10.83203125" customWidth="1"/>
-    <col min="6117" max="6117" width="10.83203125" customWidth="1"/>
-    <col min="6120" max="6123" width="10.83203125" customWidth="1"/>
-    <col min="6126" max="6126" width="10.83203125" customWidth="1"/>
-    <col min="6128" max="6128" width="10.83203125" customWidth="1"/>
-    <col min="6130" max="6133" width="10.83203125" customWidth="1"/>
-    <col min="6136" max="6146" width="10.83203125" customWidth="1"/>
-    <col min="6148" max="6148" width="10.83203125" customWidth="1"/>
-    <col min="6152" max="6160" width="10.83203125" customWidth="1"/>
-    <col min="6162" max="6162" width="10.83203125" customWidth="1"/>
-    <col min="6164" max="6165" width="10.83203125" customWidth="1"/>
-    <col min="6168" max="6177" width="10.83203125" customWidth="1"/>
-    <col min="6181" max="6181" width="10.83203125" customWidth="1"/>
-    <col min="6183" max="6195" width="10.83203125" customWidth="1"/>
-    <col min="6200" max="6210" width="10.83203125" customWidth="1"/>
-    <col min="6213" max="6213" width="10.83203125" customWidth="1"/>
-    <col min="6216" max="6224" width="10.83203125" customWidth="1"/>
-    <col min="6227" max="6228" width="10.83203125" customWidth="1"/>
-    <col min="6232" max="6262" width="10.83203125" customWidth="1"/>
-    <col min="6264" max="6264" width="10.83203125" customWidth="1"/>
-    <col min="6266" max="6329" width="10.83203125" customWidth="1"/>
-    <col min="6331" max="6331" width="10.83203125" customWidth="1"/>
-    <col min="6337" max="6342" width="10.83203125" customWidth="1"/>
-    <col min="6344" max="6347" width="10.83203125" customWidth="1"/>
-    <col min="6350" max="6352" width="10.83203125" customWidth="1"/>
-    <col min="6354" max="6379" width="10.83203125" customWidth="1"/>
-    <col min="6382" max="6382" width="10.83203125" customWidth="1"/>
-    <col min="6384" max="6404" width="10.83203125" customWidth="1"/>
-    <col min="6409" max="6410" width="10.83203125" customWidth="1"/>
-    <col min="6412" max="6414" width="10.83203125" customWidth="1"/>
-    <col min="6418" max="6418" width="10.83203125" customWidth="1"/>
-    <col min="6420" max="6420" width="10.83203125" customWidth="1"/>
-    <col min="6432" max="6480" width="10.83203125" customWidth="1"/>
-    <col min="6482" max="6521" width="10.83203125" customWidth="1"/>
-    <col min="6523" max="6523" width="10.83203125" customWidth="1"/>
-    <col min="6529" max="6534" width="10.83203125" customWidth="1"/>
-    <col min="6536" max="6539" width="10.83203125" customWidth="1"/>
-    <col min="6542" max="6544" width="10.83203125" customWidth="1"/>
-    <col min="6546" max="6580" width="10.83203125" customWidth="1"/>
-    <col min="6583" max="6644" width="10.83203125" customWidth="1"/>
-    <col min="6648" max="6650" width="10.83203125" customWidth="1"/>
-    <col min="6652" max="6654" width="10.83203125" customWidth="1"/>
-    <col min="6658" max="6660" width="10.83203125" customWidth="1"/>
-    <col min="6662" max="6664" width="10.83203125" customWidth="1"/>
-    <col min="6666" max="6668" width="10.83203125" customWidth="1"/>
-    <col min="6670" max="6670" width="10.83203125" customWidth="1"/>
-    <col min="6672" max="6672" width="10.83203125" customWidth="1"/>
-    <col min="6688" max="6768" width="10.83203125" customWidth="1"/>
-    <col min="6786" max="6788" width="10.83203125" customWidth="1"/>
-    <col min="6790" max="6792" width="10.83203125" customWidth="1"/>
-    <col min="6794" max="6796" width="10.83203125" customWidth="1"/>
-    <col min="6798" max="6798" width="10.83203125" customWidth="1"/>
-    <col min="6800" max="6800" width="10.83203125" customWidth="1"/>
-    <col min="6816" max="6835" width="10.83203125" customWidth="1"/>
-    <col min="6837" max="6837" width="10.83203125" customWidth="1"/>
-    <col min="6839" max="6899" width="10.83203125" customWidth="1"/>
-    <col min="6901" max="6901" width="10.83203125" customWidth="1"/>
-    <col min="6903" max="7029" width="10.83203125" customWidth="1"/>
-    <col min="7031" max="7060" width="10.83203125" customWidth="1"/>
-    <col min="7063" max="7096" width="10.83203125" customWidth="1"/>
-    <col min="7098" max="7099" width="10.83203125" customWidth="1"/>
-    <col min="7101" max="7102" width="10.83203125" customWidth="1"/>
-    <col min="7106" max="7108" width="10.83203125" customWidth="1"/>
-    <col min="7110" max="7112" width="10.83203125" customWidth="1"/>
-    <col min="7114" max="7116" width="10.83203125" customWidth="1"/>
-    <col min="7118" max="7118" width="10.83203125" customWidth="1"/>
-    <col min="7120" max="7120" width="10.83203125" customWidth="1"/>
-    <col min="7136" max="7156" width="10.83203125" customWidth="1"/>
-    <col min="7158" max="7163" width="10.83203125" customWidth="1"/>
-    <col min="7165" max="7166" width="10.83203125" customWidth="1"/>
-    <col min="7170" max="7172" width="10.83203125" customWidth="1"/>
-    <col min="7174" max="7176" width="10.83203125" customWidth="1"/>
-    <col min="7178" max="7180" width="10.83203125" customWidth="1"/>
-    <col min="7182" max="7182" width="10.83203125" customWidth="1"/>
-    <col min="7184" max="7184" width="10.83203125" customWidth="1"/>
-    <col min="7200" max="7220" width="10.83203125" customWidth="1"/>
-    <col min="7223" max="7225" width="10.83203125" customWidth="1"/>
-    <col min="7228" max="7228" width="10.83203125" customWidth="1"/>
-    <col min="7230" max="7230" width="10.83203125" customWidth="1"/>
-    <col min="7232" max="7232" width="10.83203125" customWidth="1"/>
-    <col min="7234" max="7234" width="10.83203125" customWidth="1"/>
-    <col min="7236" max="7237" width="10.83203125" customWidth="1"/>
-    <col min="7241" max="7243" width="10.83203125" customWidth="1"/>
-    <col min="7245" max="7261" width="10.83203125" customWidth="1"/>
-    <col min="7264" max="7285" width="10.83203125" customWidth="1"/>
-    <col min="7287" max="7316" width="10.83203125" customWidth="1"/>
-    <col min="7319" max="7349" width="10.83203125" customWidth="1"/>
-    <col min="7351" max="7352" width="10.83203125" customWidth="1"/>
-    <col min="7354" max="7355" width="10.83203125" customWidth="1"/>
-    <col min="7357" max="7358" width="10.83203125" customWidth="1"/>
-    <col min="7362" max="7364" width="10.83203125" customWidth="1"/>
-    <col min="7366" max="7368" width="10.83203125" customWidth="1"/>
-    <col min="7370" max="7372" width="10.83203125" customWidth="1"/>
-    <col min="7374" max="7374" width="10.83203125" customWidth="1"/>
-    <col min="7376" max="7376" width="10.83203125" customWidth="1"/>
-    <col min="7392" max="7412" width="10.83203125" customWidth="1"/>
-    <col min="7415" max="7419" width="10.83203125" customWidth="1"/>
-    <col min="7421" max="7422" width="10.83203125" customWidth="1"/>
-    <col min="7426" max="7428" width="10.83203125" customWidth="1"/>
-    <col min="7430" max="7432" width="10.83203125" customWidth="1"/>
-    <col min="7434" max="7436" width="10.83203125" customWidth="1"/>
-    <col min="7438" max="7438" width="10.83203125" customWidth="1"/>
-    <col min="7440" max="7440" width="10.83203125" customWidth="1"/>
-    <col min="7456" max="7486" width="10.83203125" customWidth="1"/>
-    <col min="7491" max="7494" width="10.83203125" customWidth="1"/>
-    <col min="7496" max="7499" width="10.83203125" customWidth="1"/>
-    <col min="7502" max="7504" width="10.83203125" customWidth="1"/>
-    <col min="7506" max="7536" width="10.83203125" customWidth="1"/>
-    <col min="7540" max="7542" width="10.83203125" customWidth="1"/>
-    <col min="7544" max="7605" width="10.83203125" customWidth="1"/>
-    <col min="7607" max="7607" width="10.83203125" customWidth="1"/>
-    <col min="7610" max="7611" width="10.83203125" customWidth="1"/>
-    <col min="7613" max="7614" width="10.83203125" customWidth="1"/>
-    <col min="7618" max="7620" width="10.83203125" customWidth="1"/>
-    <col min="7622" max="7624" width="10.83203125" customWidth="1"/>
-    <col min="7626" max="7628" width="10.83203125" customWidth="1"/>
-    <col min="7630" max="7630" width="10.83203125" customWidth="1"/>
-    <col min="7632" max="7632" width="10.83203125" customWidth="1"/>
-    <col min="7648" max="7668" width="10.83203125" customWidth="1"/>
-    <col min="7671" max="7673" width="10.83203125" customWidth="1"/>
-    <col min="7676" max="7676" width="10.83203125" customWidth="1"/>
-    <col min="7678" max="7678" width="10.83203125" customWidth="1"/>
-    <col min="7680" max="7680" width="10.83203125" customWidth="1"/>
-    <col min="7682" max="7682" width="10.83203125" customWidth="1"/>
-    <col min="7684" max="7685" width="10.83203125" customWidth="1"/>
-    <col min="7689" max="7691" width="10.83203125" customWidth="1"/>
-    <col min="7693" max="7709" width="10.83203125" customWidth="1"/>
-    <col min="7712" max="7728" width="10.83203125" customWidth="1"/>
-    <col min="7730" max="7737" width="10.83203125" customWidth="1"/>
-    <col min="7739" max="7740" width="10.83203125" customWidth="1"/>
-    <col min="7743" max="7744" width="10.83203125" customWidth="1"/>
-    <col min="7746" max="7760" width="10.83203125" customWidth="1"/>
-    <col min="7762" max="7793" width="10.83203125" customWidth="1"/>
-    <col min="7796" max="7797" width="10.83203125" customWidth="1"/>
-    <col min="7800" max="7809" width="10.83203125" customWidth="1"/>
-    <col min="7811" max="7815" width="10.83203125" customWidth="1"/>
-    <col min="7817" max="7819" width="10.83203125" customWidth="1"/>
-    <col min="7822" max="7822" width="10.83203125" customWidth="1"/>
-    <col min="7824" max="7825" width="10.83203125" customWidth="1"/>
-    <col min="7829" max="7829" width="10.83203125" customWidth="1"/>
-    <col min="7831" max="7832" width="10.83203125" customWidth="1"/>
-    <col min="7834" max="7834" width="10.83203125" customWidth="1"/>
-    <col min="7836" max="7836" width="10.83203125" customWidth="1"/>
-    <col min="7839" max="7841" width="10.83203125" customWidth="1"/>
-    <col min="7844" max="7846" width="10.83203125" customWidth="1"/>
-    <col min="7852" max="7852" width="10.83203125" customWidth="1"/>
-    <col min="7854" max="7860" width="10.83203125" customWidth="1"/>
-    <col min="7863" max="7996" width="10.83203125" customWidth="1"/>
-    <col min="7998" max="8039" width="10.83203125" customWidth="1"/>
-    <col min="8049" max="8049" width="10.83203125" customWidth="1"/>
-    <col min="8052" max="8053" width="10.83203125" customWidth="1"/>
-    <col min="8056" max="8065" width="10.83203125" customWidth="1"/>
-    <col min="8067" max="8071" width="10.83203125" customWidth="1"/>
-    <col min="8073" max="8075" width="10.83203125" customWidth="1"/>
-    <col min="8078" max="8078" width="10.83203125" customWidth="1"/>
-    <col min="8080" max="8081" width="10.83203125" customWidth="1"/>
-    <col min="8085" max="8085" width="10.83203125" customWidth="1"/>
-    <col min="8087" max="8088" width="10.83203125" customWidth="1"/>
-    <col min="8090" max="8090" width="10.83203125" customWidth="1"/>
-    <col min="8092" max="8092" width="10.83203125" customWidth="1"/>
-    <col min="8095" max="8097" width="10.83203125" customWidth="1"/>
-    <col min="8100" max="8102" width="10.83203125" customWidth="1"/>
-    <col min="8108" max="8108" width="10.83203125" customWidth="1"/>
-    <col min="8110" max="8176" width="10.83203125" customWidth="1"/>
-    <col min="8179" max="8374" width="10.83203125" customWidth="1"/>
-    <col min="8377" max="8377" width="10.83203125" customWidth="1"/>
-    <col min="8381" max="8382" width="10.83203125" customWidth="1"/>
-    <col min="8384" max="8384" width="10.83203125" customWidth="1"/>
-    <col min="8388" max="8390" width="10.83203125" customWidth="1"/>
-    <col min="8392" max="8393" width="10.83203125" customWidth="1"/>
-    <col min="8395" max="8413" width="10.83203125" customWidth="1"/>
-    <col min="8416" max="8436" width="10.83203125" customWidth="1"/>
-    <col min="8441" max="8443" width="10.83203125" customWidth="1"/>
-    <col min="8445" max="8446" width="10.83203125" customWidth="1"/>
-    <col min="8450" max="8452" width="10.83203125" customWidth="1"/>
-    <col min="8454" max="8456" width="10.83203125" customWidth="1"/>
-    <col min="8458" max="8460" width="10.83203125" customWidth="1"/>
-    <col min="8462" max="8462" width="10.83203125" customWidth="1"/>
-    <col min="8464" max="8464" width="10.83203125" customWidth="1"/>
-    <col min="8480" max="8496" width="10.83203125" customWidth="1"/>
-    <col min="8500" max="8501" width="10.83203125" customWidth="1"/>
-    <col min="8505" max="8506" width="10.83203125" customWidth="1"/>
-    <col min="8509" max="8510" width="10.83203125" customWidth="1"/>
-    <col min="8512" max="8513" width="10.83203125" customWidth="1"/>
-    <col min="8516" max="8516" width="10.83203125" customWidth="1"/>
-    <col min="8520" max="8522" width="10.83203125" customWidth="1"/>
-    <col min="8526" max="8527" width="10.83203125" customWidth="1"/>
-    <col min="8544" max="8630" width="10.83203125" customWidth="1"/>
-    <col min="8633" max="8633" width="10.83203125" customWidth="1"/>
-    <col min="8637" max="8638" width="10.83203125" customWidth="1"/>
-    <col min="8640" max="8640" width="10.83203125" customWidth="1"/>
-    <col min="8644" max="8646" width="10.83203125" customWidth="1"/>
-    <col min="8648" max="8649" width="10.83203125" customWidth="1"/>
-    <col min="8651" max="8669" width="10.83203125" customWidth="1"/>
-    <col min="8672" max="8696" width="10.83203125" customWidth="1"/>
-    <col min="8698" max="8699" width="10.83203125" customWidth="1"/>
-    <col min="8701" max="8702" width="10.83203125" customWidth="1"/>
-    <col min="8706" max="8708" width="10.83203125" customWidth="1"/>
-    <col min="8710" max="8712" width="10.83203125" customWidth="1"/>
-    <col min="8714" max="8716" width="10.83203125" customWidth="1"/>
-    <col min="8718" max="8718" width="10.83203125" customWidth="1"/>
-    <col min="8720" max="8720" width="10.83203125" customWidth="1"/>
-    <col min="8736" max="8752" width="10.83203125" customWidth="1"/>
-    <col min="8756" max="8757" width="10.83203125" customWidth="1"/>
-    <col min="8761" max="8762" width="10.83203125" customWidth="1"/>
-    <col min="8765" max="8766" width="10.83203125" customWidth="1"/>
-    <col min="8768" max="8769" width="10.83203125" customWidth="1"/>
-    <col min="8772" max="8772" width="10.83203125" customWidth="1"/>
-    <col min="8776" max="8778" width="10.83203125" customWidth="1"/>
-    <col min="8782" max="8783" width="10.83203125" customWidth="1"/>
-    <col min="8785" max="8949" width="10.83203125" customWidth="1"/>
-    <col min="8951" max="8952" width="10.83203125" customWidth="1"/>
-    <col min="8954" max="8955" width="10.83203125" customWidth="1"/>
-    <col min="8957" max="8958" width="10.83203125" customWidth="1"/>
-    <col min="8962" max="8964" width="10.83203125" customWidth="1"/>
-    <col min="8966" max="8968" width="10.83203125" customWidth="1"/>
-    <col min="8970" max="8972" width="10.83203125" customWidth="1"/>
-    <col min="8974" max="8974" width="10.83203125" customWidth="1"/>
-    <col min="8976" max="8976" width="10.83203125" customWidth="1"/>
-    <col min="8992" max="9008" width="10.83203125" customWidth="1"/>
-    <col min="9010" max="9017" width="10.83203125" customWidth="1"/>
-    <col min="9019" max="9020" width="10.83203125" customWidth="1"/>
-    <col min="9023" max="9024" width="10.83203125" customWidth="1"/>
-    <col min="9026" max="9201" width="10.83203125" customWidth="1"/>
-    <col min="9204" max="9205" width="10.83203125" customWidth="1"/>
-    <col min="9208" max="9217" width="10.83203125" customWidth="1"/>
-    <col min="9219" max="9223" width="10.83203125" customWidth="1"/>
-    <col min="9225" max="9227" width="10.83203125" customWidth="1"/>
-    <col min="9230" max="9230" width="10.83203125" customWidth="1"/>
-    <col min="9232" max="9233" width="10.83203125" customWidth="1"/>
-    <col min="9237" max="9237" width="10.83203125" customWidth="1"/>
-    <col min="9239" max="9240" width="10.83203125" customWidth="1"/>
-    <col min="9242" max="9242" width="10.83203125" customWidth="1"/>
-    <col min="9244" max="9244" width="10.83203125" customWidth="1"/>
-    <col min="9247" max="9249" width="10.83203125" customWidth="1"/>
-    <col min="9252" max="9254" width="10.83203125" customWidth="1"/>
-    <col min="9260" max="9260" width="10.83203125" customWidth="1"/>
-    <col min="9262" max="9268" width="10.83203125" customWidth="1"/>
-    <col min="9271" max="9273" width="10.83203125" customWidth="1"/>
-    <col min="9276" max="9276" width="10.83203125" customWidth="1"/>
-    <col min="9278" max="9278" width="10.83203125" customWidth="1"/>
-    <col min="9280" max="9280" width="10.83203125" customWidth="1"/>
-    <col min="9282" max="9282" width="10.83203125" customWidth="1"/>
-    <col min="9284" max="9285" width="10.83203125" customWidth="1"/>
-    <col min="9289" max="9291" width="10.83203125" customWidth="1"/>
-    <col min="9293" max="9309" width="10.83203125" customWidth="1"/>
-    <col min="9312" max="9328" width="10.83203125" customWidth="1"/>
-    <col min="9332" max="9334" width="10.83203125" customWidth="1"/>
-    <col min="9336" max="9396" width="10.83203125" customWidth="1"/>
-    <col min="9399" max="9401" width="10.83203125" customWidth="1"/>
-    <col min="9404" max="9404" width="10.83203125" customWidth="1"/>
-    <col min="9406" max="9406" width="10.83203125" customWidth="1"/>
-    <col min="9408" max="9408" width="10.83203125" customWidth="1"/>
-    <col min="9410" max="9410" width="10.83203125" customWidth="1"/>
-    <col min="9412" max="9413" width="10.83203125" customWidth="1"/>
-    <col min="9417" max="9419" width="10.83203125" customWidth="1"/>
-    <col min="9421" max="9437" width="10.83203125" customWidth="1"/>
-    <col min="9440" max="9456" width="10.83203125" customWidth="1"/>
-    <col min="9460" max="9462" width="10.83203125" customWidth="1"/>
-    <col min="9464" max="9526" width="10.83203125" customWidth="1"/>
-    <col min="9528" max="9529" width="10.83203125" customWidth="1"/>
-    <col min="9531" max="9531" width="10.83203125" customWidth="1"/>
-    <col min="9533" max="9534" width="10.83203125" customWidth="1"/>
-    <col min="9538" max="9540" width="10.83203125" customWidth="1"/>
-    <col min="9542" max="9544" width="10.83203125" customWidth="1"/>
-    <col min="9546" max="9548" width="10.83203125" customWidth="1"/>
-    <col min="9550" max="9550" width="10.83203125" customWidth="1"/>
-    <col min="9552" max="9552" width="10.83203125" customWidth="1"/>
-    <col min="9568" max="9588" width="10.83203125" customWidth="1"/>
-    <col min="9591" max="9593" width="10.83203125" customWidth="1"/>
-    <col min="9596" max="9596" width="10.83203125" customWidth="1"/>
-    <col min="9598" max="9598" width="10.83203125" customWidth="1"/>
-    <col min="9600" max="9600" width="10.83203125" customWidth="1"/>
-    <col min="9602" max="9602" width="10.83203125" customWidth="1"/>
-    <col min="9604" max="9605" width="10.83203125" customWidth="1"/>
-    <col min="9609" max="9611" width="10.83203125" customWidth="1"/>
-    <col min="9613" max="9629" width="10.83203125" customWidth="1"/>
-    <col min="9632" max="9654" width="10.83203125" customWidth="1"/>
-    <col min="9656" max="9660" width="10.83203125" customWidth="1"/>
-    <col min="9662" max="9663" width="10.83203125" customWidth="1"/>
-    <col min="9667" max="9669" width="10.83203125" customWidth="1"/>
-    <col min="9672" max="9672" width="10.83203125" customWidth="1"/>
-    <col min="9674" max="9676" width="10.83203125" customWidth="1"/>
-    <col min="9679" max="9679" width="10.83203125" customWidth="1"/>
-    <col min="9696" max="9713" width="10.83203125" customWidth="1"/>
-    <col min="9716" max="9717" width="10.83203125" customWidth="1"/>
-    <col min="9720" max="9729" width="10.83203125" customWidth="1"/>
-    <col min="9731" max="9735" width="10.83203125" customWidth="1"/>
-    <col min="9737" max="9739" width="10.83203125" customWidth="1"/>
-    <col min="9742" max="9742" width="10.83203125" customWidth="1"/>
-    <col min="9744" max="9745" width="10.83203125" customWidth="1"/>
-    <col min="9749" max="9749" width="10.83203125" customWidth="1"/>
-    <col min="9751" max="9752" width="10.83203125" customWidth="1"/>
-    <col min="9754" max="9754" width="10.83203125" customWidth="1"/>
-    <col min="9756" max="9756" width="10.83203125" customWidth="1"/>
-    <col min="9759" max="9761" width="10.83203125" customWidth="1"/>
-    <col min="9764" max="9766" width="10.83203125" customWidth="1"/>
-    <col min="9772" max="9772" width="10.83203125" customWidth="1"/>
-    <col min="9774" max="9777" width="10.83203125" customWidth="1"/>
-    <col min="9780" max="9781" width="10.83203125" customWidth="1"/>
-    <col min="9784" max="9793" width="10.83203125" customWidth="1"/>
-    <col min="9795" max="9799" width="10.83203125" customWidth="1"/>
-    <col min="9801" max="9803" width="10.83203125" customWidth="1"/>
-    <col min="9806" max="9806" width="10.83203125" customWidth="1"/>
-    <col min="9808" max="9809" width="10.83203125" customWidth="1"/>
-    <col min="9813" max="9813" width="10.83203125" customWidth="1"/>
-    <col min="9815" max="9816" width="10.83203125" customWidth="1"/>
-    <col min="9818" max="9818" width="10.83203125" customWidth="1"/>
-    <col min="9820" max="9820" width="10.83203125" customWidth="1"/>
-    <col min="9823" max="9825" width="10.83203125" customWidth="1"/>
-    <col min="9828" max="9830" width="10.83203125" customWidth="1"/>
-    <col min="9836" max="9836" width="10.83203125" customWidth="1"/>
-    <col min="9838" max="9844" width="10.83203125" customWidth="1"/>
-    <col min="9849" max="9852" width="10.83203125" customWidth="1"/>
-    <col min="9854" max="9855" width="10.83203125" customWidth="1"/>
-    <col min="9857" max="9857" width="10.83203125" customWidth="1"/>
-    <col min="9859" max="9861" width="10.83203125" customWidth="1"/>
-    <col min="9865" max="9865" width="10.83203125" customWidth="1"/>
-    <col min="9867" max="9867" width="10.83203125" customWidth="1"/>
-    <col min="9871" max="9871" width="10.83203125" customWidth="1"/>
-    <col min="9888" max="9908" width="10.83203125" customWidth="1"/>
-    <col min="9910" max="9910" width="10.83203125" customWidth="1"/>
-    <col min="9912" max="9912" width="10.83203125" customWidth="1"/>
-    <col min="9914" max="9914" width="10.83203125" customWidth="1"/>
-    <col min="9917" max="9918" width="10.83203125" customWidth="1"/>
-    <col min="9922" max="9924" width="10.83203125" customWidth="1"/>
-    <col min="9926" max="9928" width="10.83203125" customWidth="1"/>
-    <col min="9930" max="9932" width="10.83203125" customWidth="1"/>
-    <col min="9934" max="9934" width="10.83203125" customWidth="1"/>
-    <col min="9936" max="9936" width="10.83203125" customWidth="1"/>
-    <col min="9952" max="9968" width="10.83203125" customWidth="1"/>
-    <col min="10033" max="10035" width="10.83203125" customWidth="1"/>
-    <col min="10037" max="10038" width="10.83203125" customWidth="1"/>
-    <col min="10040" max="10041" width="10.83203125" customWidth="1"/>
-    <col min="10044" max="10046" width="10.83203125" customWidth="1"/>
-    <col min="10050" max="10052" width="10.83203125" customWidth="1"/>
-    <col min="10054" max="10056" width="10.83203125" customWidth="1"/>
-    <col min="10058" max="10060" width="10.83203125" customWidth="1"/>
-    <col min="10062" max="10062" width="10.83203125" customWidth="1"/>
-    <col min="10064" max="10064" width="10.83203125" customWidth="1"/>
-    <col min="10080" max="10100" width="10.83203125" customWidth="1"/>
-    <col min="10103" max="10105" width="10.83203125" customWidth="1"/>
-    <col min="10108" max="10110" width="10.83203125" customWidth="1"/>
-    <col min="10114" max="10116" width="10.83203125" customWidth="1"/>
-    <col min="10118" max="10120" width="10.83203125" customWidth="1"/>
-    <col min="10122" max="10124" width="10.83203125" customWidth="1"/>
-    <col min="10126" max="10126" width="10.83203125" customWidth="1"/>
-    <col min="10128" max="10128" width="10.83203125" customWidth="1"/>
-    <col min="10144" max="10160" width="10.83203125" customWidth="1"/>
-    <col min="10163" max="10165" width="10.83203125" customWidth="1"/>
-    <col min="10167" max="10170" width="10.83203125" customWidth="1"/>
-    <col min="10172" max="10172" width="10.83203125" customWidth="1"/>
-    <col min="10174" max="10176" width="10.83203125" customWidth="1"/>
-    <col min="10178" max="10178" width="10.83203125" customWidth="1"/>
-    <col min="10186" max="10188" width="10.83203125" customWidth="1"/>
-    <col min="10191" max="10191" width="10.83203125" customWidth="1"/>
-    <col min="10208" max="10224" width="10.83203125" customWidth="1"/>
-    <col min="10289" max="10294" width="10.83203125" customWidth="1"/>
-    <col min="10297" max="10299" width="10.83203125" customWidth="1"/>
-    <col min="10301" max="10302" width="10.83203125" customWidth="1"/>
-    <col min="10306" max="10308" width="10.83203125" customWidth="1"/>
-    <col min="10310" max="10312" width="10.83203125" customWidth="1"/>
-    <col min="10314" max="10316" width="10.83203125" customWidth="1"/>
-    <col min="10318" max="10318" width="10.83203125" customWidth="1"/>
-    <col min="10320" max="10320" width="10.83203125" customWidth="1"/>
-    <col min="10336" max="10356" width="10.83203125" customWidth="1"/>
-    <col min="10358" max="10358" width="10.83203125" customWidth="1"/>
-    <col min="10360" max="10361" width="10.83203125" customWidth="1"/>
-    <col min="10364" max="10366" width="10.83203125" customWidth="1"/>
-    <col min="10370" max="10372" width="10.83203125" customWidth="1"/>
-    <col min="10374" max="10376" width="10.83203125" customWidth="1"/>
-    <col min="10378" max="10380" width="10.83203125" customWidth="1"/>
-    <col min="10382" max="10382" width="10.83203125" customWidth="1"/>
-    <col min="10384" max="10384" width="10.83203125" customWidth="1"/>
-    <col min="10400" max="10416" width="10.83203125" customWidth="1"/>
-    <col min="10419" max="10421" width="10.83203125" customWidth="1"/>
-    <col min="10423" max="10426" width="10.83203125" customWidth="1"/>
-    <col min="10428" max="10428" width="10.83203125" customWidth="1"/>
-    <col min="10430" max="10432" width="10.83203125" customWidth="1"/>
-    <col min="10434" max="10434" width="10.83203125" customWidth="1"/>
-    <col min="10442" max="10444" width="10.83203125" customWidth="1"/>
-    <col min="10447" max="10447" width="10.83203125" customWidth="1"/>
-    <col min="10464" max="10480" width="10.83203125" customWidth="1"/>
-    <col min="10483" max="10483" width="10.83203125" customWidth="1"/>
-    <col min="10485" max="10485" width="10.83203125" customWidth="1"/>
-    <col min="10488" max="10490" width="10.83203125" customWidth="1"/>
-    <col min="10492" max="10492" width="10.83203125" customWidth="1"/>
-    <col min="10496" max="10496" width="10.83203125" customWidth="1"/>
-    <col min="10501" max="10501" width="10.83203125" customWidth="1"/>
-    <col min="10504" max="10508" width="10.83203125" customWidth="1"/>
-    <col min="10512" max="10512" width="10.83203125" customWidth="1"/>
-    <col min="10517" max="10517" width="10.83203125" customWidth="1"/>
-    <col min="10519" max="10520" width="10.83203125" customWidth="1"/>
-    <col min="10522" max="10522" width="10.83203125" customWidth="1"/>
-    <col min="10525" max="10526" width="10.83203125" customWidth="1"/>
-    <col min="10528" max="10528" width="10.83203125" customWidth="1"/>
-    <col min="10530" max="10530" width="10.83203125" customWidth="1"/>
-    <col min="10532" max="10533" width="10.83203125" customWidth="1"/>
-    <col min="10536" max="10537" width="10.83203125" customWidth="1"/>
-    <col min="10539" max="10540" width="10.83203125" customWidth="1"/>
-    <col min="10544" max="10549" width="10.83203125" customWidth="1"/>
-    <col min="10553" max="10555" width="10.83203125" customWidth="1"/>
-    <col min="10557" max="10558" width="10.83203125" customWidth="1"/>
-    <col min="10562" max="10564" width="10.83203125" customWidth="1"/>
-    <col min="10566" max="10568" width="10.83203125" customWidth="1"/>
-    <col min="10570" max="10572" width="10.83203125" customWidth="1"/>
-    <col min="10574" max="10574" width="10.83203125" customWidth="1"/>
-    <col min="10576" max="10576" width="10.83203125" customWidth="1"/>
-    <col min="10592" max="10608" width="10.83203125" customWidth="1"/>
-    <col min="10610" max="10610" width="10.83203125" customWidth="1"/>
-    <col min="10613" max="10613" width="10.83203125" customWidth="1"/>
-    <col min="10615" max="10616" width="10.83203125" customWidth="1"/>
-    <col min="10619" max="10622" width="10.83203125" customWidth="1"/>
-    <col min="10624" max="10624" width="10.83203125" customWidth="1"/>
-    <col min="10629" max="10629" width="10.83203125" customWidth="1"/>
-    <col min="10632" max="10633" width="10.83203125" customWidth="1"/>
-    <col min="10637" max="10637" width="10.83203125" customWidth="1"/>
-    <col min="10640" max="10641" width="10.83203125" customWidth="1"/>
-    <col min="10644" max="10645" width="10.83203125" customWidth="1"/>
-    <col min="10648" max="10648" width="10.83203125" customWidth="1"/>
-    <col min="10650" max="10651" width="10.83203125" customWidth="1"/>
-    <col min="10653" max="10653" width="10.83203125" customWidth="1"/>
-    <col min="10656" max="10656" width="10.83203125" customWidth="1"/>
-    <col min="10660" max="10661" width="10.83203125" customWidth="1"/>
-    <col min="10664" max="10664" width="10.83203125" customWidth="1"/>
-    <col min="10666" max="10666" width="10.83203125" customWidth="1"/>
-    <col min="10668" max="10668" width="10.83203125" customWidth="1"/>
-    <col min="10672" max="10673" width="10.83203125" customWidth="1"/>
-    <col min="10675" max="10676" width="10.83203125" customWidth="1"/>
-    <col min="10680" max="10680" width="10.83203125" customWidth="1"/>
-    <col min="10682" max="10685" width="10.83203125" customWidth="1"/>
-    <col min="10688" max="10690" width="10.83203125" customWidth="1"/>
-    <col min="10692" max="10692" width="10.83203125" customWidth="1"/>
-    <col min="10696" max="10696" width="10.83203125" customWidth="1"/>
-    <col min="10698" max="10699" width="10.83203125" customWidth="1"/>
-    <col min="10701" max="10701" width="10.83203125" customWidth="1"/>
-    <col min="10704" max="10704" width="10.83203125" customWidth="1"/>
-    <col min="10709" max="10709" width="10.83203125" customWidth="1"/>
-    <col min="10712" max="10713" width="10.83203125" customWidth="1"/>
-    <col min="10717" max="10717" width="10.83203125" customWidth="1"/>
-    <col min="10720" max="10720" width="10.83203125" customWidth="1"/>
-    <col min="10722" max="10722" width="10.83203125" customWidth="1"/>
-    <col min="10725" max="10725" width="10.83203125" customWidth="1"/>
-    <col min="10727" max="10730" width="10.83203125" customWidth="1"/>
-    <col min="10732" max="10732" width="10.83203125" customWidth="1"/>
-    <col min="10734" max="10734" width="10.83203125" customWidth="1"/>
-    <col min="10736" max="10736" width="10.83203125" customWidth="1"/>
-    <col min="10741" max="10741" width="10.83203125" customWidth="1"/>
-    <col min="10744" max="10744" width="10.83203125" customWidth="1"/>
-    <col min="10749" max="10749" width="10.83203125" customWidth="1"/>
-    <col min="10752" max="10754" width="10.83203125" customWidth="1"/>
-    <col min="10757" max="10757" width="10.83203125" customWidth="1"/>
-    <col min="10760" max="10760" width="10.83203125" customWidth="1"/>
-    <col min="10762" max="10762" width="10.83203125" customWidth="1"/>
-    <col min="10765" max="10765" width="10.83203125" customWidth="1"/>
-    <col min="10767" max="10768" width="10.83203125" customWidth="1"/>
-    <col min="10770" max="10770" width="10.83203125" customWidth="1"/>
-    <col min="10773" max="10773" width="10.83203125" customWidth="1"/>
-    <col min="10776" max="10776" width="10.83203125" customWidth="1"/>
-    <col min="10778" max="10781" width="10.83203125" customWidth="1"/>
-    <col min="10784" max="10784" width="10.83203125" customWidth="1"/>
-    <col min="10787" max="10788" width="10.83203125" customWidth="1"/>
-    <col min="10792" max="10794" width="10.83203125" customWidth="1"/>
-    <col min="10796" max="10796" width="10.83203125" customWidth="1"/>
-    <col min="10800" max="10800" width="10.83203125" customWidth="1"/>
-    <col min="10802" max="10802" width="10.83203125" customWidth="1"/>
-    <col min="10804" max="10805" width="10.83203125" customWidth="1"/>
-    <col min="10808" max="10809" width="10.83203125" customWidth="1"/>
-    <col min="10811" max="10812" width="10.83203125" customWidth="1"/>
-    <col min="10816" max="10816" width="10.83203125" customWidth="1"/>
-    <col min="10821" max="10821" width="10.83203125" customWidth="1"/>
-    <col min="10823" max="10826" width="10.83203125" customWidth="1"/>
-    <col min="10828" max="10828" width="10.83203125" customWidth="1"/>
-    <col min="10832" max="10832" width="10.83203125" customWidth="1"/>
-    <col min="10834" max="10834" width="10.83203125" customWidth="1"/>
-    <col min="10836" max="10837" width="10.83203125" customWidth="1"/>
-    <col min="10840" max="10840" width="10.83203125" customWidth="1"/>
-    <col min="10842" max="10842" width="10.83203125" customWidth="1"/>
-    <col min="10845" max="10845" width="10.83203125" customWidth="1"/>
-    <col min="10848" max="10852" width="10.83203125" customWidth="1"/>
-    <col min="10856" max="10858" width="10.83203125" customWidth="1"/>
-    <col min="10861" max="10861" width="10.83203125" customWidth="1"/>
-    <col min="10864" max="10864" width="10.83203125" customWidth="1"/>
-    <col min="10866" max="10869" width="10.83203125" customWidth="1"/>
-    <col min="10872" max="10874" width="10.83203125" customWidth="1"/>
-    <col min="10876" max="10876" width="10.83203125" customWidth="1"/>
-    <col min="10880" max="10880" width="10.83203125" customWidth="1"/>
-    <col min="10882" max="10882" width="10.83203125" customWidth="1"/>
-    <col min="10884" max="10885" width="10.83203125" customWidth="1"/>
-    <col min="10888" max="10889" width="10.83203125" customWidth="1"/>
-    <col min="10893" max="10893" width="10.83203125" customWidth="1"/>
-    <col min="10895" max="10899" width="10.83203125" customWidth="1"/>
-    <col min="10904" max="10906" width="10.83203125" customWidth="1"/>
-    <col min="10909" max="10909" width="10.83203125" customWidth="1"/>
-    <col min="10912" max="10912" width="10.83203125" customWidth="1"/>
-    <col min="10915" max="10916" width="10.83203125" customWidth="1"/>
-    <col min="10920" max="10928" width="10.83203125" customWidth="1"/>
-    <col min="10930" max="10931" width="10.83203125" customWidth="1"/>
-    <col min="10934" max="10997" width="10.83203125" customWidth="1"/>
-    <col min="10999" max="10999" width="10.83203125" customWidth="1"/>
-    <col min="11002" max="11003" width="10.83203125" customWidth="1"/>
-    <col min="11005" max="11006" width="10.83203125" customWidth="1"/>
-    <col min="11010" max="11012" width="10.83203125" customWidth="1"/>
-    <col min="11014" max="11016" width="10.83203125" customWidth="1"/>
-    <col min="11018" max="11020" width="10.83203125" customWidth="1"/>
-    <col min="11022" max="11022" width="10.83203125" customWidth="1"/>
-    <col min="11024" max="11024" width="10.83203125" customWidth="1"/>
-    <col min="11040" max="11056" width="10.83203125" customWidth="1"/>
-    <col min="11059" max="11059" width="10.83203125" customWidth="1"/>
-    <col min="11061" max="11063" width="10.83203125" customWidth="1"/>
-    <col min="11066" max="11067" width="10.83203125" customWidth="1"/>
-    <col min="11071" max="11071" width="10.83203125" customWidth="1"/>
-    <col min="11073" max="11073" width="10.83203125" customWidth="1"/>
-    <col min="11075" max="11075" width="10.83203125" customWidth="1"/>
-    <col min="11082" max="11084" width="10.83203125" customWidth="1"/>
-    <col min="11087" max="11087" width="10.83203125" customWidth="1"/>
-    <col min="11104" max="11122" width="10.83203125" customWidth="1"/>
-    <col min="11124" max="11187" width="10.83203125" customWidth="1"/>
-    <col min="11191" max="11195" width="10.83203125" customWidth="1"/>
-    <col min="11197" max="11198" width="10.83203125" customWidth="1"/>
-    <col min="11200" max="11201" width="10.83203125" customWidth="1"/>
-    <col min="11203" max="11204" width="10.83203125" customWidth="1"/>
-    <col min="11209" max="11214" width="10.83203125" customWidth="1"/>
-    <col min="11218" max="11218" width="10.83203125" customWidth="1"/>
-    <col min="11220" max="11220" width="10.83203125" customWidth="1"/>
-    <col min="11232" max="11253" width="10.83203125" customWidth="1"/>
-    <col min="11255" max="11255" width="10.83203125" customWidth="1"/>
-    <col min="11257" max="11259" width="10.83203125" customWidth="1"/>
-    <col min="11261" max="11262" width="10.83203125" customWidth="1"/>
-    <col min="11266" max="11268" width="10.83203125" customWidth="1"/>
-    <col min="11270" max="11272" width="10.83203125" customWidth="1"/>
-    <col min="11274" max="11276" width="10.83203125" customWidth="1"/>
-    <col min="11278" max="11278" width="10.83203125" customWidth="1"/>
-    <col min="11280" max="11280" width="10.83203125" customWidth="1"/>
-    <col min="11296" max="11376" width="10.83203125" customWidth="1"/>
-    <col min="11380" max="11443" width="10.83203125" customWidth="1"/>
-    <col min="11445" max="11508" width="10.83203125" customWidth="1"/>
-    <col min="11513" max="11513" width="10.83203125" customWidth="1"/>
-    <col min="11515" max="11515" width="10.83203125" customWidth="1"/>
-    <col min="11517" max="11518" width="10.83203125" customWidth="1"/>
-    <col min="11522" max="11524" width="10.83203125" customWidth="1"/>
-    <col min="11526" max="11528" width="10.83203125" customWidth="1"/>
-    <col min="11530" max="11532" width="10.83203125" customWidth="1"/>
-    <col min="11534" max="11534" width="10.83203125" customWidth="1"/>
-    <col min="11536" max="11536" width="10.83203125" customWidth="1"/>
-    <col min="11552" max="11571" width="10.83203125" customWidth="1"/>
-    <col min="11573" max="11573" width="10.83203125" customWidth="1"/>
-    <col min="11575" max="11575" width="10.83203125" customWidth="1"/>
-    <col min="11578" max="11578" width="10.83203125" customWidth="1"/>
-    <col min="11580" max="11580" width="10.83203125" customWidth="1"/>
-    <col min="11583" max="11583" width="10.83203125" customWidth="1"/>
-    <col min="11587" max="11588" width="10.83203125" customWidth="1"/>
-    <col min="11592" max="11594" width="10.83203125" customWidth="1"/>
-    <col min="11598" max="11599" width="10.83203125" customWidth="1"/>
-    <col min="11616" max="11633" width="10.83203125" customWidth="1"/>
-    <col min="11636" max="11637" width="10.83203125" customWidth="1"/>
-    <col min="11640" max="11649" width="10.83203125" customWidth="1"/>
-    <col min="11651" max="11655" width="10.83203125" customWidth="1"/>
-    <col min="11657" max="11659" width="10.83203125" customWidth="1"/>
-    <col min="11662" max="11662" width="10.83203125" customWidth="1"/>
-    <col min="11664" max="11665" width="10.83203125" customWidth="1"/>
-    <col min="11669" max="11669" width="10.83203125" customWidth="1"/>
-    <col min="11671" max="11672" width="10.83203125" customWidth="1"/>
-    <col min="11674" max="11674" width="10.83203125" customWidth="1"/>
-    <col min="11676" max="11676" width="10.83203125" customWidth="1"/>
-    <col min="11679" max="11681" width="10.83203125" customWidth="1"/>
-    <col min="11684" max="11686" width="10.83203125" customWidth="1"/>
-    <col min="11692" max="11692" width="10.83203125" customWidth="1"/>
-    <col min="11694" max="11704" width="10.83203125" customWidth="1"/>
-    <col min="11706" max="11707" width="10.83203125" customWidth="1"/>
-    <col min="11709" max="11710" width="10.83203125" customWidth="1"/>
-    <col min="11714" max="11716" width="10.83203125" customWidth="1"/>
-    <col min="11718" max="11720" width="10.83203125" customWidth="1"/>
-    <col min="11722" max="11724" width="10.83203125" customWidth="1"/>
-    <col min="11726" max="11726" width="10.83203125" customWidth="1"/>
-    <col min="11728" max="11728" width="10.83203125" customWidth="1"/>
-    <col min="11744" max="11761" width="10.83203125" customWidth="1"/>
-    <col min="11770" max="11831" width="10.83203125" customWidth="1"/>
-    <col min="11836" max="11836" width="10.83203125" customWidth="1"/>
-    <col min="11838" max="11838" width="10.83203125" customWidth="1"/>
-    <col min="11842" max="11844" width="10.83203125" customWidth="1"/>
-    <col min="11846" max="11848" width="10.83203125" customWidth="1"/>
-    <col min="11850" max="11852" width="10.83203125" customWidth="1"/>
-    <col min="11854" max="11854" width="10.83203125" customWidth="1"/>
-    <col min="11856" max="11856" width="10.83203125" customWidth="1"/>
-    <col min="11872" max="11889" width="10.83203125" customWidth="1"/>
-    <col min="11892" max="11893" width="10.83203125" customWidth="1"/>
-    <col min="11896" max="11905" width="10.83203125" customWidth="1"/>
-    <col min="11907" max="11911" width="10.83203125" customWidth="1"/>
-    <col min="11913" max="11915" width="10.83203125" customWidth="1"/>
-    <col min="11918" max="11918" width="10.83203125" customWidth="1"/>
-    <col min="11920" max="11921" width="10.83203125" customWidth="1"/>
-    <col min="11925" max="11925" width="10.83203125" customWidth="1"/>
-    <col min="11927" max="11928" width="10.83203125" customWidth="1"/>
-    <col min="11930" max="11930" width="10.83203125" customWidth="1"/>
-    <col min="11932" max="11932" width="10.83203125" customWidth="1"/>
-    <col min="11935" max="11937" width="10.83203125" customWidth="1"/>
-    <col min="11940" max="11942" width="10.83203125" customWidth="1"/>
-    <col min="11948" max="11948" width="10.83203125" customWidth="1"/>
-    <col min="11950" max="11952" width="10.83203125" customWidth="1"/>
-    <col min="11962" max="12021" width="10.83203125" customWidth="1"/>
-    <col min="12028" max="12030" width="10.83203125" customWidth="1"/>
-    <col min="12034" max="12036" width="10.83203125" customWidth="1"/>
-    <col min="12038" max="12040" width="10.83203125" customWidth="1"/>
-    <col min="12042" max="12044" width="10.83203125" customWidth="1"/>
-    <col min="12046" max="12046" width="10.83203125" customWidth="1"/>
-    <col min="12048" max="12048" width="10.83203125" customWidth="1"/>
-    <col min="12064" max="12081" width="10.83203125" customWidth="1"/>
-    <col min="12083" max="12083" width="10.83203125" customWidth="1"/>
-    <col min="12085" max="12085" width="10.83203125" customWidth="1"/>
-    <col min="12087" max="12088" width="10.83203125" customWidth="1"/>
-    <col min="12090" max="12091" width="10.83203125" customWidth="1"/>
-    <col min="12094" max="12094" width="10.83203125" customWidth="1"/>
-    <col min="12096" max="12096" width="10.83203125" customWidth="1"/>
-    <col min="12099" max="12099" width="10.83203125" customWidth="1"/>
-    <col min="12106" max="12108" width="10.83203125" customWidth="1"/>
-    <col min="12111" max="12111" width="10.83203125" customWidth="1"/>
-    <col min="12128" max="12145" width="10.83203125" customWidth="1"/>
-    <col min="12148" max="12149" width="10.83203125" customWidth="1"/>
-    <col min="12152" max="12161" width="10.83203125" customWidth="1"/>
-    <col min="12163" max="12167" width="10.83203125" customWidth="1"/>
-    <col min="12169" max="12171" width="10.83203125" customWidth="1"/>
-    <col min="12174" max="12174" width="10.83203125" customWidth="1"/>
-    <col min="12176" max="12177" width="10.83203125" customWidth="1"/>
-    <col min="12181" max="12181" width="10.83203125" customWidth="1"/>
-    <col min="12183" max="12184" width="10.83203125" customWidth="1"/>
-    <col min="12186" max="12186" width="10.83203125" customWidth="1"/>
-    <col min="12188" max="12188" width="10.83203125" customWidth="1"/>
-    <col min="12191" max="12193" width="10.83203125" customWidth="1"/>
-    <col min="12196" max="12198" width="10.83203125" customWidth="1"/>
-    <col min="12204" max="12204" width="10.83203125" customWidth="1"/>
-    <col min="12206" max="12208" width="10.83203125" customWidth="1"/>
-    <col min="12211" max="12216" width="10.83203125" customWidth="1"/>
-    <col min="12218" max="12219" width="10.83203125" customWidth="1"/>
-    <col min="12221" max="12222" width="10.83203125" customWidth="1"/>
-    <col min="12226" max="12228" width="10.83203125" customWidth="1"/>
-    <col min="12230" max="12232" width="10.83203125" customWidth="1"/>
-    <col min="12234" max="12236" width="10.83203125" customWidth="1"/>
-    <col min="12238" max="12238" width="10.83203125" customWidth="1"/>
-    <col min="12240" max="12240" width="10.83203125" customWidth="1"/>
-    <col min="12256" max="12283" width="10.83203125" customWidth="1"/>
-    <col min="12285" max="12286" width="10.83203125" customWidth="1"/>
-    <col min="12290" max="12292" width="10.83203125" customWidth="1"/>
-    <col min="12294" max="12296" width="10.83203125" customWidth="1"/>
-    <col min="12298" max="12300" width="10.83203125" customWidth="1"/>
-    <col min="12302" max="12302" width="10.83203125" customWidth="1"/>
-    <col min="12304" max="12304" width="10.83203125" customWidth="1"/>
-    <col min="12307" max="12307" width="10.83203125" customWidth="1"/>
-    <col min="12314" max="12339" width="10.83203125" customWidth="1"/>
-    <col min="12341" max="12345" width="10.83203125" customWidth="1"/>
-    <col min="12347" max="12352" width="10.83203125" customWidth="1"/>
-    <col min="12384" max="12408" width="10.83203125" customWidth="1"/>
-    <col min="12410" max="12411" width="10.83203125" customWidth="1"/>
-    <col min="12413" max="12414" width="10.83203125" customWidth="1"/>
-    <col min="12418" max="12420" width="10.83203125" customWidth="1"/>
-    <col min="12422" max="12424" width="10.83203125" customWidth="1"/>
-    <col min="12426" max="12428" width="10.83203125" customWidth="1"/>
-    <col min="12430" max="12430" width="10.83203125" customWidth="1"/>
-    <col min="12432" max="12432" width="10.83203125" customWidth="1"/>
-    <col min="12448" max="12465" width="10.83203125" customWidth="1"/>
-    <col min="12474" max="12496" width="10.83203125" customWidth="1"/>
-    <col min="12512" max="12528" width="10.83203125" customWidth="1"/>
-    <col min="12532" max="12533" width="10.83203125" customWidth="1"/>
-    <col min="12535" max="12537" width="10.83203125" customWidth="1"/>
-    <col min="12540" max="12540" width="10.83203125" customWidth="1"/>
-    <col min="12544" max="12544" width="10.83203125" customWidth="1"/>
-    <col min="12546" max="12546" width="10.83203125" customWidth="1"/>
-    <col min="12548" max="12548" width="10.83203125" customWidth="1"/>
-    <col min="12550" max="12560" width="10.83203125" customWidth="1"/>
-    <col min="12563" max="12563" width="10.83203125" customWidth="1"/>
-    <col min="12570" max="12595" width="10.83203125" customWidth="1"/>
-    <col min="12597" max="12601" width="10.83203125" customWidth="1"/>
-    <col min="12603" max="12608" width="10.83203125" customWidth="1"/>
-    <col min="12640" max="12661" width="10.83203125" customWidth="1"/>
-    <col min="12663" max="12664" width="10.83203125" customWidth="1"/>
-    <col min="12666" max="12667" width="10.83203125" customWidth="1"/>
-    <col min="12669" max="12670" width="10.83203125" customWidth="1"/>
-    <col min="12674" max="12676" width="10.83203125" customWidth="1"/>
-    <col min="12678" max="12680" width="10.83203125" customWidth="1"/>
-    <col min="12682" max="12684" width="10.83203125" customWidth="1"/>
-    <col min="12686" max="12686" width="10.83203125" customWidth="1"/>
-    <col min="12688" max="12688" width="10.83203125" customWidth="1"/>
-    <col min="12704" max="12721" width="10.83203125" customWidth="1"/>
-    <col min="12730" max="12752" width="10.83203125" customWidth="1"/>
-    <col min="12768" max="12784" width="10.83203125" customWidth="1"/>
-    <col min="12786" max="12880" width="10.83203125" customWidth="1"/>
-    <col min="12896" max="12915" width="10.83203125" customWidth="1"/>
-    <col min="12917" max="12976" width="10.83203125" customWidth="1"/>
-    <col min="12980" max="13043" width="10.83203125" customWidth="1"/>
-    <col min="13045" max="13045" width="10.83203125" customWidth="1"/>
-    <col min="13049" max="13049" width="10.83203125" customWidth="1"/>
-    <col min="13052" max="13054" width="10.83203125" customWidth="1"/>
-    <col min="13058" max="13060" width="10.83203125" customWidth="1"/>
-    <col min="13062" max="13064" width="10.83203125" customWidth="1"/>
-    <col min="13066" max="13068" width="10.83203125" customWidth="1"/>
-    <col min="13070" max="13070" width="10.83203125" customWidth="1"/>
-    <col min="13072" max="13072" width="10.83203125" customWidth="1"/>
-    <col min="13088" max="13232" width="10.83203125" customWidth="1"/>
-    <col min="13234" max="13277" width="10.83203125" customWidth="1"/>
-    <col min="13280" max="13299" width="10.83203125" customWidth="1"/>
-    <col min="13301" max="13304" width="10.83203125" customWidth="1"/>
-    <col min="13308" max="13310" width="10.83203125" customWidth="1"/>
-    <col min="13314" max="13316" width="10.83203125" customWidth="1"/>
-    <col min="13318" max="13320" width="10.83203125" customWidth="1"/>
-    <col min="13322" max="13324" width="10.83203125" customWidth="1"/>
-    <col min="13326" max="13326" width="10.83203125" customWidth="1"/>
-    <col min="13328" max="13328" width="10.83203125" customWidth="1"/>
-    <col min="13344" max="13438" width="10.83203125" customWidth="1"/>
-    <col min="13443" max="13446" width="10.83203125" customWidth="1"/>
-    <col min="13448" max="13451" width="10.83203125" customWidth="1"/>
-    <col min="13454" max="13456" width="10.83203125" customWidth="1"/>
-    <col min="13458" max="13553" width="10.83203125" customWidth="1"/>
-    <col min="13555" max="13557" width="10.83203125" customWidth="1"/>
-    <col min="13559" max="13559" width="10.83203125" customWidth="1"/>
-    <col min="13563" max="13563" width="10.83203125" customWidth="1"/>
-    <col min="13565" max="13565" width="10.83203125" customWidth="1"/>
-    <col min="13567" max="13567" width="10.83203125" customWidth="1"/>
-    <col min="13569" max="13569" width="10.83203125" customWidth="1"/>
-    <col min="13571" max="13571" width="10.83203125" customWidth="1"/>
-    <col min="13573" max="13573" width="10.83203125" customWidth="1"/>
-    <col min="13575" max="13575" width="10.83203125" customWidth="1"/>
-    <col min="13577" max="13577" width="10.83203125" customWidth="1"/>
-    <col min="13579" max="13580" width="10.83203125" customWidth="1"/>
-    <col min="13583" max="14064" width="10.83203125" customWidth="1"/>
-    <col min="14067" max="15153" width="10.83203125" customWidth="1"/>
-    <col min="15156" max="15157" width="10.83203125" customWidth="1"/>
-    <col min="15160" max="15169" width="10.83203125" customWidth="1"/>
-    <col min="15171" max="15175" width="10.83203125" customWidth="1"/>
-    <col min="15177" max="15179" width="10.83203125" customWidth="1"/>
-    <col min="15182" max="15182" width="10.83203125" customWidth="1"/>
-    <col min="15184" max="15185" width="10.83203125" customWidth="1"/>
-    <col min="15189" max="15189" width="10.83203125" customWidth="1"/>
-    <col min="15191" max="15192" width="10.83203125" customWidth="1"/>
-    <col min="15194" max="15194" width="10.83203125" customWidth="1"/>
-    <col min="15196" max="15196" width="10.83203125" customWidth="1"/>
-    <col min="15199" max="15201" width="10.83203125" customWidth="1"/>
-    <col min="15204" max="15206" width="10.83203125" customWidth="1"/>
-    <col min="15212" max="15212" width="10.83203125" customWidth="1"/>
-    <col min="15214" max="15217" width="10.83203125" customWidth="1"/>
-    <col min="15220" max="15221" width="10.83203125" customWidth="1"/>
-    <col min="15224" max="15233" width="10.83203125" customWidth="1"/>
-    <col min="15235" max="15239" width="10.83203125" customWidth="1"/>
-    <col min="15241" max="15243" width="10.83203125" customWidth="1"/>
-    <col min="15246" max="15246" width="10.83203125" customWidth="1"/>
-    <col min="15248" max="15249" width="10.83203125" customWidth="1"/>
-    <col min="15253" max="15253" width="10.83203125" customWidth="1"/>
-    <col min="15255" max="15256" width="10.83203125" customWidth="1"/>
-    <col min="15258" max="15258" width="10.83203125" customWidth="1"/>
-    <col min="15260" max="15260" width="10.83203125" customWidth="1"/>
-    <col min="15263" max="15265" width="10.83203125" customWidth="1"/>
-    <col min="15268" max="15270" width="10.83203125" customWidth="1"/>
-    <col min="15276" max="15276" width="10.83203125" customWidth="1"/>
-    <col min="15278" max="15283" width="10.83203125" customWidth="1"/>
-    <col min="15285" max="15286" width="10.83203125" customWidth="1"/>
-    <col min="15288" max="15289" width="10.83203125" customWidth="1"/>
-    <col min="15291" max="15291" width="10.83203125" customWidth="1"/>
-    <col min="15293" max="15294" width="10.83203125" customWidth="1"/>
-    <col min="15296" max="15297" width="10.83203125" customWidth="1"/>
-    <col min="15300" max="15304" width="10.83203125" customWidth="1"/>
-    <col min="15307" max="15308" width="10.83203125" customWidth="1"/>
-    <col min="15310" max="15312" width="10.83203125" customWidth="1"/>
-    <col min="15314" max="15483" width="10.83203125" customWidth="1"/>
-    <col min="15485" max="15486" width="10.83203125" customWidth="1"/>
-    <col min="15490" max="15492" width="10.83203125" customWidth="1"/>
-    <col min="15494" max="15496" width="10.83203125" customWidth="1"/>
-    <col min="15498" max="15500" width="10.83203125" customWidth="1"/>
-    <col min="15502" max="15502" width="10.83203125" customWidth="1"/>
-    <col min="15504" max="15504" width="10.83203125" customWidth="1"/>
-    <col min="15520" max="15536" width="10.83203125" customWidth="1"/>
-    <col min="15538" max="15538" width="10.83203125" customWidth="1"/>
-    <col min="15544" max="15544" width="10.83203125" customWidth="1"/>
-    <col min="15546" max="15547" width="10.83203125" customWidth="1"/>
-    <col min="15550" max="15550" width="10.83203125" customWidth="1"/>
-    <col min="15552" max="15552" width="10.83203125" customWidth="1"/>
-    <col min="15555" max="15555" width="10.83203125" customWidth="1"/>
-    <col min="15562" max="15564" width="10.83203125" customWidth="1"/>
-    <col min="15567" max="15567" width="10.83203125" customWidth="1"/>
-    <col min="15584" max="15606" width="10.83203125" customWidth="1"/>
-    <col min="15609" max="15611" width="10.83203125" customWidth="1"/>
-    <col min="15613" max="15614" width="10.83203125" customWidth="1"/>
-    <col min="15618" max="15620" width="10.83203125" customWidth="1"/>
-    <col min="15622" max="15624" width="10.83203125" customWidth="1"/>
-    <col min="15626" max="15628" width="10.83203125" customWidth="1"/>
-    <col min="15630" max="15630" width="10.83203125" customWidth="1"/>
-    <col min="15632" max="15632" width="10.83203125" customWidth="1"/>
-    <col min="15648" max="15732" width="10.83203125" customWidth="1"/>
-    <col min="15737" max="15739" width="10.83203125" customWidth="1"/>
-    <col min="15741" max="15742" width="10.83203125" customWidth="1"/>
-    <col min="15746" max="15748" width="10.83203125" customWidth="1"/>
-    <col min="15750" max="15752" width="10.83203125" customWidth="1"/>
-    <col min="15754" max="15756" width="10.83203125" customWidth="1"/>
-    <col min="15758" max="15758" width="10.83203125" customWidth="1"/>
-    <col min="15760" max="15760" width="10.83203125" customWidth="1"/>
-    <col min="15776" max="15792" width="10.83203125" customWidth="1"/>
-    <col min="15794" max="15794" width="10.83203125" customWidth="1"/>
-    <col min="15798" max="15801" width="10.83203125" customWidth="1"/>
-    <col min="15806" max="15806" width="10.83203125" customWidth="1"/>
-    <col min="15808" max="15809" width="10.83203125" customWidth="1"/>
-    <col min="15811" max="15811" width="10.83203125" customWidth="1"/>
-    <col min="15818" max="15820" width="10.83203125" customWidth="1"/>
-    <col min="15823" max="15823" width="10.83203125" customWidth="1"/>
-    <col min="15840" max="15861" width="10.83203125" customWidth="1"/>
-    <col min="15865" max="15867" width="10.83203125" customWidth="1"/>
-    <col min="15869" max="15870" width="10.83203125" customWidth="1"/>
-    <col min="15874" max="15876" width="10.83203125" customWidth="1"/>
-    <col min="15878" max="15880" width="10.83203125" customWidth="1"/>
-    <col min="15882" max="15884" width="10.83203125" customWidth="1"/>
-    <col min="15886" max="15886" width="10.83203125" customWidth="1"/>
-    <col min="15888" max="15888" width="10.83203125" customWidth="1"/>
-    <col min="15904" max="15921" width="10.83203125" customWidth="1"/>
-    <col min="15926" max="15927" width="10.83203125" customWidth="1"/>
-    <col min="15931" max="15933" width="10.83203125" customWidth="1"/>
-    <col min="15937" max="15937" width="10.83203125" customWidth="1"/>
-    <col min="15939" max="15940" width="10.83203125" customWidth="1"/>
-    <col min="15944" max="15946" width="10.83203125" customWidth="1"/>
-    <col min="15950" max="15951" width="10.83203125" customWidth="1"/>
-    <col min="15968" max="15988" width="10.83203125" customWidth="1"/>
-    <col min="15990" max="15992" width="10.83203125" customWidth="1"/>
-    <col min="15994" max="15995" width="10.83203125" customWidth="1"/>
-    <col min="15997" max="15998" width="10.83203125" customWidth="1"/>
-    <col min="16002" max="16004" width="10.83203125" customWidth="1"/>
-    <col min="16006" max="16008" width="10.83203125" customWidth="1"/>
-    <col min="16010" max="16012" width="10.83203125" customWidth="1"/>
-    <col min="16014" max="16014" width="10.83203125" customWidth="1"/>
-    <col min="16016" max="16016" width="10.83203125" customWidth="1"/>
-    <col min="16032" max="16048" width="10.83203125" customWidth="1"/>
-    <col min="16050" max="16050" width="10.83203125" customWidth="1"/>
-    <col min="16054" max="16057" width="10.83203125" customWidth="1"/>
-    <col min="16062" max="16062" width="10.83203125" customWidth="1"/>
-    <col min="16064" max="16065" width="10.83203125" customWidth="1"/>
-    <col min="16067" max="16067" width="10.83203125" customWidth="1"/>
-    <col min="16074" max="16076" width="10.83203125" customWidth="1"/>
-    <col min="16079" max="16079" width="10.83203125" customWidth="1"/>
-    <col min="16096" max="16112" width="10.83203125" customWidth="1"/>
-    <col min="16114" max="16114" width="10.83203125" customWidth="1"/>
-    <col min="16118" max="16118" width="10.83203125" customWidth="1"/>
-    <col min="16120" max="16120" width="10.83203125" customWidth="1"/>
-    <col min="16122" max="16176" width="10.83203125" customWidth="1"/>
-    <col min="16178" max="16178" width="10.83203125" customWidth="1"/>
-    <col min="16182" max="16182" width="10.83203125" customWidth="1"/>
-    <col min="16184" max="16184" width="10.83203125" customWidth="1"/>
-    <col min="16186" max="16245" width="10.83203125" customWidth="1"/>
-    <col min="16247" max="16248" width="10.83203125" customWidth="1"/>
-    <col min="16250" max="16251" width="10.83203125" customWidth="1"/>
-    <col min="16253" max="16254" width="10.83203125" customWidth="1"/>
-    <col min="16258" max="16260" width="10.83203125" customWidth="1"/>
-    <col min="16262" max="16264" width="10.83203125" customWidth="1"/>
-    <col min="16266" max="16268" width="10.83203125" customWidth="1"/>
-    <col min="16270" max="16270" width="10.83203125" customWidth="1"/>
-    <col min="16272" max="16272" width="10.83203125" customWidth="1"/>
-    <col min="16288" max="16304" width="10.83203125" customWidth="1"/>
-    <col min="16306" max="16307" width="10.83203125" customWidth="1"/>
-    <col min="16310" max="16312" width="10.83203125" customWidth="1"/>
-    <col min="16314" max="16315" width="10.83203125" customWidth="1"/>
-    <col min="16318" max="16318" width="10.83203125" customWidth="1"/>
-    <col min="16320" max="16320" width="10.83203125" customWidth="1"/>
-    <col min="16323" max="16323" width="10.83203125" customWidth="1"/>
-    <col min="16325" max="16329" width="10.83203125" customWidth="1"/>
-    <col min="16331" max="16332" width="10.83203125" customWidth="1"/>
-    <col min="16335" max="16335" width="10.83203125" customWidth="1"/>
-    <col min="16352" max="16368" width="10.83203125" customWidth="1"/>
-    <col min="16372" max="16374" width="10.83203125" customWidth="1"/>
-    <col min="16376" max="16376" width="10.83203125" customWidth="1"/>
-    <col min="16379" max="16384" width="10.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>